<commit_message>
Moved Manual Data Entry into DataLoader, Added Sheet Data Entry for Drag and Drop
</commit_message>
<xml_diff>
--- a/data/StudentData.xlsx
+++ b/data/StudentData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5849" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7050" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -119,6 +119,30 @@
   </si>
   <si>
     <t>S, GL</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>John T. Baker Middle School</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>wr</t>
+  </si>
+  <si>
+    <t>Benjamin Banneker Middle School</t>
   </si>
 </sst>
 </file>
@@ -455,7 +479,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:G207"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
@@ -489,32 +513,32 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>122534</v>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>111111.0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>122789</v>
+        <v>122534</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -526,18 +550,18 @@
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>122873</v>
+        <v>122789</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -560,7 +584,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>123788</v>
+        <v>122873</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -577,13 +601,13 @@
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
+      <c r="G5" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>130892</v>
+        <v>123788</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -595,18 +619,18 @@
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>132394</v>
+        <v>130892</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -618,18 +642,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>132532</v>
+        <v>132394</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -652,7 +676,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>132853</v>
+        <v>132532</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -666,7 +690,7 @@
       <c r="E9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -675,7 +699,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>134333</v>
+        <v>132853</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -689,16 +713,16 @@
       <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>10</v>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>134390</v>
+        <v>134333</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -709,19 +733,19 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>9</v>
+      <c r="E11" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>135062</v>
+        <v>134390</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -732,11 +756,11 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>10</v>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>9</v>
@@ -744,7 +768,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>137940</v>
+        <v>135062</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -756,18 +780,18 @@
         <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>140093</v>
+        <v>137940</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -785,12 +809,12 @@
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>140892</v>
+        <v>140093</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -802,9 +826,9 @@
         <v>7</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -813,7 +837,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>142310</v>
+        <v>140892</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -824,19 +848,19 @@
       <c r="D16" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>9</v>
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>146632</v>
+        <v>142310</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -847,19 +871,19 @@
       <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>156681</v>
+        <v>146632</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -877,12 +901,12 @@
         <v>10</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>161618</v>
+        <v>156681</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -893,7 +917,7 @@
       <c r="D19" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="2" t="s">
@@ -905,7 +929,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>168329</v>
+        <v>161618</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -916,11 +940,11 @@
       <c r="D20" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>10</v>
+      <c r="E20" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>10</v>
@@ -928,7 +952,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>169650</v>
+        <v>168329</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -942,7 +966,7 @@
       <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -951,7 +975,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>173425</v>
+        <v>169650</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -965,7 +989,7 @@
       <c r="E22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -974,7 +998,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>178071</v>
+        <v>173425</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -992,12 +1016,12 @@
         <v>9</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>178156</v>
+        <v>178071</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -1015,12 +1039,12 @@
         <v>9</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>181903</v>
+        <v>178156</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -1032,18 +1056,18 @@
         <v>7</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>9</v>
+      <c r="G25" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>182120</v>
+        <v>181903</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -1055,10 +1079,10 @@
         <v>7</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>9</v>
@@ -1066,7 +1090,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>186663</v>
+        <v>182120</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -1078,10 +1102,10 @@
         <v>7</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>9</v>
@@ -1089,7 +1113,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>187393</v>
+        <v>186663</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -1106,13 +1130,13 @@
       <c r="F28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>10</v>
+      <c r="G28" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>190029</v>
+        <v>187393</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -1123,10 +1147,10 @@
       <c r="D29" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="E29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G29" s="2" t="s">
@@ -1135,7 +1159,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>194574</v>
+        <v>190029</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -1146,8 +1170,8 @@
       <c r="D30" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>10</v>
+      <c r="E30" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>9</v>
@@ -1158,7 +1182,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>198048</v>
+        <v>194574</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -1172,16 +1196,16 @@
       <c r="E31" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>9</v>
+      <c r="F31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>198741</v>
+        <v>198048</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1198,13 +1222,13 @@
       <c r="F32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>10</v>
+      <c r="G32" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>199787</v>
+        <v>198741</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -1216,18 +1240,18 @@
         <v>7</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>9</v>
+      <c r="G33" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>200672</v>
+        <v>199787</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -1239,18 +1263,18 @@
         <v>7</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>210938</v>
+        <v>200672</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
@@ -1261,19 +1285,19 @@
       <c r="D35" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="3" t="s">
+      <c r="E35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>225969</v>
+        <v>210938</v>
       </c>
       <c r="B36" t="s">
         <v>7</v>
@@ -1284,42 +1308,42 @@
       <c r="D36" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>10</v>
+      <c r="E36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>231348</v>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>213456.0</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>232461</v>
+        <v>225969</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -1334,15 +1358,15 @@
         <v>10</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>257317</v>
+        <v>231348</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
@@ -1354,7 +1378,7 @@
         <v>7</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>10</v>
@@ -1365,7 +1389,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>276682</v>
+        <v>232461</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1377,41 +1401,41 @@
         <v>7</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>278390</v>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>234539.0</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>292270</v>
+        <v>257317</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
@@ -1425,16 +1449,16 @@
       <c r="E42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>9</v>
+      <c r="F42" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>292271</v>
+        <v>276682</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
@@ -1446,18 +1470,18 @@
         <v>7</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>9</v>
+      <c r="G43" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>299774</v>
+        <v>278390</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -1480,7 +1504,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>299880</v>
+        <v>292270</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
@@ -1494,7 +1518,7 @@
       <c r="E45" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G45" s="2" t="s">
@@ -1503,7 +1527,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>406490</v>
+        <v>292271</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
@@ -1515,18 +1539,18 @@
         <v>7</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>409089</v>
+        <v>299774</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -1549,7 +1573,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>411168</v>
+        <v>299880</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
@@ -1567,12 +1591,12 @@
         <v>9</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>417688</v>
+        <v>406490</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -1583,7 +1607,7 @@
       <c r="D49" t="s">
         <v>7</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F49" s="2" t="s">
@@ -1595,7 +1619,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>419371</v>
+        <v>409089</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
@@ -1613,35 +1637,35 @@
         <v>9</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>419659</v>
+        <v>411168</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>420119</v>
+        <v>417688</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -1652,19 +1676,19 @@
       <c r="D52" t="s">
         <v>7</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E52" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>436542</v>
+        <v>419371</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
@@ -1682,12 +1706,12 @@
         <v>9</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>439155</v>
+        <v>419659</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -1705,12 +1729,12 @@
         <v>9</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>441021</v>
+        <v>420119</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -1722,18 +1746,18 @@
         <v>7</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>442262</v>
+        <v>436542</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
@@ -1748,15 +1772,15 @@
         <v>10</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>442931</v>
+        <v>439155</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -1767,19 +1791,19 @@
       <c r="D57" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>9</v>
+      <c r="E57" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>443257</v>
+        <v>441021</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
@@ -1790,8 +1814,8 @@
       <c r="D58" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>9</v>
+      <c r="E58" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>9</v>
@@ -1802,7 +1826,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>446253</v>
+        <v>442262</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -1814,18 +1838,18 @@
         <v>7</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>448013</v>
+        <v>442931</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
@@ -1836,19 +1860,19 @@
       <c r="D60" t="s">
         <v>7</v>
       </c>
-      <c r="E60" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G60" s="3" t="s">
+      <c r="E60" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>452390</v>
+        <v>443257</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -1859,19 +1883,19 @@
       <c r="D61" t="s">
         <v>7</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="E61" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G61" s="3" t="s">
-        <v>9</v>
+      <c r="G61" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>452992</v>
+        <v>446253</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
@@ -1883,18 +1907,18 @@
         <v>7</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G62" s="3" t="s">
-        <v>9</v>
+      <c r="G62" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>454280</v>
+        <v>448013</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
@@ -1908,7 +1932,7 @@
       <c r="E63" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="F63" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G63" s="3" t="s">
@@ -1917,7 +1941,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>454287</v>
+        <v>452390</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -1929,18 +1953,18 @@
         <v>7</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>454745</v>
+        <v>452992</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
@@ -1951,11 +1975,11 @@
       <c r="D65" t="s">
         <v>7</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>9</v>
+      <c r="E65" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>9</v>
@@ -1963,7 +1987,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>454770</v>
+        <v>454280</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
@@ -1975,18 +1999,18 @@
         <v>7</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>455839</v>
+        <v>454287</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
@@ -2000,16 +2024,16 @@
       <c r="E67" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>461540</v>
+        <v>454745</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
@@ -2020,11 +2044,11 @@
       <c r="D68" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="2" t="s">
-        <v>10</v>
+      <c r="E68" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G68" s="3" t="s">
         <v>9</v>
@@ -2032,7 +2056,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>462838</v>
+        <v>454770</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
@@ -2044,18 +2068,18 @@
         <v>7</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>463934</v>
+        <v>455839</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
@@ -2066,8 +2090,8 @@
       <c r="D70" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>9</v>
+      <c r="E70" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>9</v>
@@ -2078,7 +2102,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>464863</v>
+        <v>461540</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
@@ -2090,7 +2114,7 @@
         <v>7</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>9</v>
@@ -2101,7 +2125,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>465018</v>
+        <v>462838</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
@@ -2115,7 +2139,7 @@
       <c r="E72" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="F72" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G72" s="3" t="s">
@@ -2124,7 +2148,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>465085</v>
+        <v>463934</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
@@ -2135,19 +2159,19 @@
       <c r="D73" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="2" t="s">
-        <v>10</v>
+      <c r="E73" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G73" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>465090</v>
+        <v>464863</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
@@ -2159,7 +2183,7 @@
         <v>7</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>9</v>
@@ -2170,7 +2194,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>465141</v>
+        <v>465018</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
@@ -2184,16 +2208,16 @@
       <c r="E75" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G75" s="2" t="s">
+      <c r="F75" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>465275</v>
+        <v>465085</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
@@ -2205,18 +2229,18 @@
         <v>7</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G76" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>465391</v>
+        <v>465090</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -2228,18 +2252,18 @@
         <v>7</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G77" s="2" t="s">
-        <v>10</v>
+      <c r="G77" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>465431</v>
+        <v>465141</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
@@ -2250,10 +2274,10 @@
       <c r="D78" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" s="3" t="s">
+      <c r="E78" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G78" s="2" t="s">
@@ -2262,7 +2286,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>465456</v>
+        <v>465275</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
@@ -2274,18 +2298,18 @@
         <v>7</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>465484</v>
+        <v>465391</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
@@ -2297,7 +2321,7 @@
         <v>7</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>9</v>
@@ -2308,7 +2332,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>465595</v>
+        <v>465431</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -2319,19 +2343,19 @@
       <c r="D81" t="s">
         <v>7</v>
       </c>
-      <c r="E81" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>10</v>
+      <c r="E81" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>465644</v>
+        <v>465456</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
@@ -2346,15 +2370,15 @@
         <v>10</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>465653</v>
+        <v>465484</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
@@ -2377,7 +2401,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>465814</v>
+        <v>465595</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
@@ -2389,18 +2413,18 @@
         <v>7</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>465850</v>
+        <v>465644</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
@@ -2414,16 +2438,16 @@
       <c r="E85" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F85" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>10</v>
+      <c r="F85" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>466433</v>
+        <v>465653</v>
       </c>
       <c r="B86" t="s">
         <v>7</v>
@@ -2434,10 +2458,10 @@
       <c r="D86" t="s">
         <v>7</v>
       </c>
-      <c r="E86" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="3" t="s">
+      <c r="E86" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G86" s="2" t="s">
@@ -2446,7 +2470,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>466579</v>
+        <v>465814</v>
       </c>
       <c r="B87" t="s">
         <v>7</v>
@@ -2469,7 +2493,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>466801</v>
+        <v>465850</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
@@ -2483,16 +2507,16 @@
       <c r="E88" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F88" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>9</v>
+      <c r="F88" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>466831</v>
+        <v>466433</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
@@ -2503,19 +2527,19 @@
       <c r="D89" t="s">
         <v>7</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F89" s="2" t="s">
+      <c r="E89" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>466968</v>
+        <v>466579</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
@@ -2527,18 +2551,18 @@
         <v>7</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>467069</v>
+        <v>466801</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
@@ -2550,41 +2574,41 @@
         <v>7</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G91" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
-        <v>467189</v>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>466803.0</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C92" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D92" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="E92" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" t="s">
+        <v>10</v>
+      </c>
+      <c r="G92" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>467214</v>
+        <v>466831</v>
       </c>
       <c r="B93" t="s">
         <v>7</v>
@@ -2595,19 +2619,19 @@
       <c r="D93" t="s">
         <v>7</v>
       </c>
-      <c r="E93" s="3" t="s">
+      <c r="E93" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>467243</v>
+        <v>466968</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
@@ -2621,7 +2645,7 @@
       <c r="E94" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="F94" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G94" s="2" t="s">
@@ -2630,7 +2654,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>467436</v>
+        <v>467069</v>
       </c>
       <c r="B95" t="s">
         <v>7</v>
@@ -2642,18 +2666,18 @@
         <v>7</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G95" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G95" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>467451</v>
+        <v>467189</v>
       </c>
       <c r="B96" t="s">
         <v>7</v>
@@ -2664,19 +2688,19 @@
       <c r="D96" t="s">
         <v>7</v>
       </c>
-      <c r="E96" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>10</v>
+      <c r="E96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>467455</v>
+        <v>467214</v>
       </c>
       <c r="B97" t="s">
         <v>7</v>
@@ -2687,19 +2711,19 @@
       <c r="D97" t="s">
         <v>7</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>10</v>
+      <c r="E97" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>467461</v>
+        <v>467243</v>
       </c>
       <c r="B98" t="s">
         <v>7</v>
@@ -2711,18 +2735,18 @@
         <v>7</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F98" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F98" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>467465</v>
+        <v>467436</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
@@ -2737,15 +2761,15 @@
         <v>10</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>467493</v>
+        <v>467451</v>
       </c>
       <c r="B100" t="s">
         <v>7</v>
@@ -2756,19 +2780,19 @@
       <c r="D100" t="s">
         <v>7</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>9</v>
+      <c r="E100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>467497</v>
+        <v>467455</v>
       </c>
       <c r="B101" t="s">
         <v>7</v>
@@ -2783,15 +2807,15 @@
         <v>10</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G101" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G101" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>467501</v>
+        <v>467461</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
@@ -2806,15 +2830,15 @@
         <v>9</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>467636</v>
+        <v>467465</v>
       </c>
       <c r="B103" t="s">
         <v>7</v>
@@ -2826,18 +2850,18 @@
         <v>7</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G103" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>467744</v>
+        <v>467493</v>
       </c>
       <c r="B104" t="s">
         <v>7</v>
@@ -2848,10 +2872,10 @@
       <c r="D104" t="s">
         <v>7</v>
       </c>
-      <c r="E104" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F104" s="2" t="s">
+      <c r="E104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G104" s="3" t="s">
@@ -2860,7 +2884,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>467750</v>
+        <v>467497</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>
@@ -2871,19 +2895,19 @@
       <c r="D105" t="s">
         <v>7</v>
       </c>
-      <c r="E105" s="3" t="s">
-        <v>9</v>
+      <c r="E105" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>467765</v>
+        <v>467501</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
@@ -2895,10 +2919,10 @@
         <v>7</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>10</v>
@@ -2906,7 +2930,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>467775</v>
+        <v>467636</v>
       </c>
       <c r="B107" t="s">
         <v>7</v>
@@ -2918,18 +2942,18 @@
         <v>7</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G107" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>467836</v>
+        <v>467744</v>
       </c>
       <c r="B108" t="s">
         <v>7</v>
@@ -2940,19 +2964,19 @@
       <c r="D108" t="s">
         <v>7</v>
       </c>
-      <c r="E108" s="2" t="s">
-        <v>10</v>
+      <c r="E108" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G108" s="2" t="s">
-        <v>10</v>
+      <c r="G108" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>467870</v>
+        <v>467750</v>
       </c>
       <c r="B109" t="s">
         <v>7</v>
@@ -2963,19 +2987,19 @@
       <c r="D109" t="s">
         <v>7</v>
       </c>
-      <c r="E109" s="2" t="s">
-        <v>10</v>
+      <c r="E109" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>467873</v>
+        <v>467765</v>
       </c>
       <c r="B110" t="s">
         <v>7</v>
@@ -2987,9 +3011,9 @@
         <v>7</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F110" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G110" s="2" t="s">
@@ -2998,7 +3022,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>467940</v>
+        <v>467775</v>
       </c>
       <c r="B111" t="s">
         <v>7</v>
@@ -3009,8 +3033,8 @@
       <c r="D111" t="s">
         <v>7</v>
       </c>
-      <c r="E111" s="3" t="s">
-        <v>9</v>
+      <c r="E111" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>9</v>
@@ -3021,7 +3045,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>467947</v>
+        <v>467836</v>
       </c>
       <c r="B112" t="s">
         <v>7</v>
@@ -3039,12 +3063,12 @@
         <v>9</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>467963</v>
+        <v>467870</v>
       </c>
       <c r="B113" t="s">
         <v>7</v>
@@ -3056,7 +3080,7 @@
         <v>7</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>9</v>
@@ -3067,7 +3091,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>467975</v>
+        <v>467873</v>
       </c>
       <c r="B114" t="s">
         <v>7</v>
@@ -3084,19 +3108,19 @@
       <c r="F114" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G114" s="3" t="s">
-        <v>9</v>
+      <c r="G114" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>467986</v>
+        <v>467940</v>
       </c>
       <c r="B115" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D115" t="s">
         <v>7</v>
@@ -3107,13 +3131,13 @@
       <c r="F115" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G115" s="3" t="s">
-        <v>9</v>
+      <c r="G115" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>468167</v>
+        <v>467947</v>
       </c>
       <c r="B116" t="s">
         <v>7</v>
@@ -3125,18 +3149,18 @@
         <v>7</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>468178</v>
+        <v>467963</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
@@ -3148,10 +3172,10 @@
         <v>7</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>9</v>
@@ -3159,7 +3183,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>468255</v>
+        <v>467975</v>
       </c>
       <c r="B118" t="s">
         <v>7</v>
@@ -3176,36 +3200,36 @@
       <c r="F118" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="G118" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>468284</v>
+        <v>467986</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C119" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D119" t="s">
         <v>7</v>
       </c>
-      <c r="E119" s="2" t="s">
-        <v>10</v>
+      <c r="E119" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G119" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G119" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>468311</v>
+        <v>468167</v>
       </c>
       <c r="B120" t="s">
         <v>7</v>
@@ -3220,15 +3244,15 @@
         <v>9</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>468546</v>
+        <v>468178</v>
       </c>
       <c r="B121" t="s">
         <v>7</v>
@@ -3243,15 +3267,15 @@
         <v>10</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>468554</v>
+        <v>468255</v>
       </c>
       <c r="B122" t="s">
         <v>7</v>
@@ -3266,15 +3290,15 @@
         <v>9</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>468556</v>
+        <v>468284</v>
       </c>
       <c r="B123" t="s">
         <v>7</v>
@@ -3292,12 +3316,12 @@
         <v>10</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>468607</v>
+        <v>468311</v>
       </c>
       <c r="B124" t="s">
         <v>7</v>
@@ -3309,18 +3333,18 @@
         <v>7</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>468643</v>
+        <v>468546</v>
       </c>
       <c r="B125" t="s">
         <v>7</v>
@@ -3343,7 +3367,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>468736</v>
+        <v>468554</v>
       </c>
       <c r="B126" t="s">
         <v>7</v>
@@ -3355,18 +3379,18 @@
         <v>7</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F126" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>468763</v>
+        <v>468556</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
@@ -3378,7 +3402,7 @@
         <v>7</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>10</v>
@@ -3389,7 +3413,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>468841</v>
+        <v>468607</v>
       </c>
       <c r="B128" t="s">
         <v>7</v>
@@ -3404,7 +3428,7 @@
         <v>10</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>10</v>
@@ -3412,7 +3436,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>468859</v>
+        <v>468643</v>
       </c>
       <c r="B129" t="s">
         <v>7</v>
@@ -3427,15 +3451,15 @@
         <v>10</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>468876</v>
+        <v>468736</v>
       </c>
       <c r="B130" t="s">
         <v>7</v>
@@ -3447,7 +3471,7 @@
         <v>7</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F130" s="3" t="s">
         <v>9</v>
@@ -3458,7 +3482,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>468882</v>
+        <v>468763</v>
       </c>
       <c r="B131" t="s">
         <v>7</v>
@@ -3473,15 +3497,15 @@
         <v>9</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G131" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>468898</v>
+        <v>468841</v>
       </c>
       <c r="B132" t="s">
         <v>7</v>
@@ -3493,7 +3517,7 @@
         <v>7</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>10</v>
@@ -3504,7 +3528,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>468903</v>
+        <v>468859</v>
       </c>
       <c r="B133" t="s">
         <v>7</v>
@@ -3515,19 +3539,19 @@
       <c r="D133" t="s">
         <v>7</v>
       </c>
-      <c r="E133" s="3" t="s">
-        <v>9</v>
+      <c r="E133" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G133" s="2" t="s">
-        <v>10</v>
+      <c r="G133" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A134" s="4">
-        <v>468961</v>
+      <c r="A134" s="1">
+        <v>468876</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
@@ -3539,9 +3563,9 @@
         <v>7</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F134" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F134" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G134" s="3" t="s">
@@ -3550,7 +3574,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>469129</v>
+        <v>468882</v>
       </c>
       <c r="B135" t="s">
         <v>7</v>
@@ -3562,10 +3586,10 @@
         <v>7</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>9</v>
@@ -3573,7 +3597,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>469142</v>
+        <v>468898</v>
       </c>
       <c r="B136" t="s">
         <v>7</v>
@@ -3585,18 +3609,18 @@
         <v>7</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>469186</v>
+        <v>468903</v>
       </c>
       <c r="B137" t="s">
         <v>7</v>
@@ -3607,19 +3631,19 @@
       <c r="D137" t="s">
         <v>7</v>
       </c>
-      <c r="E137" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F137" s="3" t="s">
-        <v>9</v>
+      <c r="E137" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="1">
-        <v>469193</v>
+      <c r="A138" s="4">
+        <v>468961</v>
       </c>
       <c r="B138" t="s">
         <v>7</v>
@@ -3630,19 +3654,19 @@
       <c r="D138" t="s">
         <v>7</v>
       </c>
-      <c r="E138" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F138" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G138" s="2" t="s">
+      <c r="E138" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G138" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>469213</v>
+        <v>469129</v>
       </c>
       <c r="B139" t="s">
         <v>7</v>
@@ -3657,15 +3681,15 @@
         <v>10</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>469288</v>
+        <v>469142</v>
       </c>
       <c r="B140" t="s">
         <v>7</v>
@@ -3677,18 +3701,18 @@
         <v>7</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A141" s="4">
-        <v>469327</v>
+      <c r="A141" s="1">
+        <v>469186</v>
       </c>
       <c r="B141" t="s">
         <v>7</v>
@@ -3702,16 +3726,16 @@
       <c r="E141" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F141" s="2" t="s">
+      <c r="F141" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>469351</v>
+        <v>469193</v>
       </c>
       <c r="B142" t="s">
         <v>7</v>
@@ -3722,19 +3746,19 @@
       <c r="D142" t="s">
         <v>7</v>
       </c>
-      <c r="E142" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>10</v>
+      <c r="E142" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G142" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>469358</v>
+        <v>469213</v>
       </c>
       <c r="B143" t="s">
         <v>7</v>
@@ -3745,19 +3769,19 @@
       <c r="D143" t="s">
         <v>7</v>
       </c>
-      <c r="E143" s="3" t="s">
-        <v>9</v>
+      <c r="E143" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>469474</v>
+        <v>469288</v>
       </c>
       <c r="B144" t="s">
         <v>7</v>
@@ -3774,13 +3798,13 @@
       <c r="F144" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G144" s="3" t="s">
+      <c r="G144" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" s="1">
-        <v>469486</v>
+      <c r="A145" s="4">
+        <v>469327</v>
       </c>
       <c r="B145" t="s">
         <v>7</v>
@@ -3792,7 +3816,7 @@
         <v>7</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>9</v>
@@ -3803,7 +3827,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>469625</v>
+        <v>469351</v>
       </c>
       <c r="B146" t="s">
         <v>7</v>
@@ -3818,15 +3842,15 @@
         <v>9</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>469740</v>
+        <v>469358</v>
       </c>
       <c r="B147" t="s">
         <v>7</v>
@@ -3837,11 +3861,11 @@
       <c r="D147" t="s">
         <v>7</v>
       </c>
-      <c r="E147" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F147" s="3" t="s">
-        <v>9</v>
+      <c r="E147" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>9</v>
@@ -3849,7 +3873,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>469823</v>
+        <v>469474</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
@@ -3864,15 +3888,15 @@
         <v>9</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G148" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>469857</v>
+        <v>469486</v>
       </c>
       <c r="B149" t="s">
         <v>7</v>
@@ -3890,12 +3914,12 @@
         <v>9</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>469975</v>
+        <v>469625</v>
       </c>
       <c r="B150" t="s">
         <v>7</v>
@@ -3918,7 +3942,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>470129</v>
+        <v>469740</v>
       </c>
       <c r="B151" t="s">
         <v>7</v>
@@ -3930,18 +3954,18 @@
         <v>7</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F151" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F151" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>470144</v>
+        <v>469823</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
@@ -3953,18 +3977,18 @@
         <v>7</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>470282</v>
+        <v>469857</v>
       </c>
       <c r="B153" t="s">
         <v>7</v>
@@ -3976,7 +4000,7 @@
         <v>7</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>9</v>
@@ -3987,7 +4011,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>470290</v>
+        <v>469975</v>
       </c>
       <c r="B154" t="s">
         <v>7</v>
@@ -3999,18 +4023,18 @@
         <v>7</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G154" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G154" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>470309</v>
+        <v>470129</v>
       </c>
       <c r="B155" t="s">
         <v>7</v>
@@ -4022,10 +4046,10 @@
         <v>7</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G155" s="2" t="s">
         <v>10</v>
@@ -4033,7 +4057,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>470373</v>
+        <v>470144</v>
       </c>
       <c r="B156" t="s">
         <v>7</v>
@@ -4048,7 +4072,7 @@
         <v>10</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G156" s="2" t="s">
         <v>9</v>
@@ -4056,7 +4080,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>470405</v>
+        <v>470282</v>
       </c>
       <c r="B157" t="s">
         <v>7</v>
@@ -4068,18 +4092,18 @@
         <v>7</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G157" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G157" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>470467</v>
+        <v>470290</v>
       </c>
       <c r="B158" t="s">
         <v>7</v>
@@ -4094,15 +4118,15 @@
         <v>10</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G158" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G158" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>470488</v>
+        <v>470309</v>
       </c>
       <c r="B159" t="s">
         <v>7</v>
@@ -4114,18 +4138,18 @@
         <v>7</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F159" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="F159" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>470638</v>
+        <v>470373</v>
       </c>
       <c r="B160" t="s">
         <v>7</v>
@@ -4139,16 +4163,16 @@
       <c r="E160" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F160" s="3" t="s">
+      <c r="F160" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>470668</v>
+        <v>470405</v>
       </c>
       <c r="B161" t="s">
         <v>7</v>
@@ -4160,18 +4184,18 @@
         <v>7</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G161" s="2" t="s">
-        <v>10</v>
+      <c r="G161" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>470754</v>
+        <v>470467</v>
       </c>
       <c r="B162" t="s">
         <v>7</v>
@@ -4185,16 +4209,16 @@
       <c r="E162" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F162" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G162" s="3" t="s">
+      <c r="F162" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G162" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>470773</v>
+        <v>470488</v>
       </c>
       <c r="B163" t="s">
         <v>7</v>
@@ -4206,18 +4230,18 @@
         <v>7</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F163" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G163" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G163" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>470782</v>
+        <v>470638</v>
       </c>
       <c r="B164" t="s">
         <v>7</v>
@@ -4229,18 +4253,18 @@
         <v>7</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F164" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F164" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>470830</v>
+        <v>470668</v>
       </c>
       <c r="B165" t="s">
         <v>7</v>
@@ -4252,18 +4276,18 @@
         <v>7</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>470859</v>
+        <v>470754</v>
       </c>
       <c r="B166" t="s">
         <v>7</v>
@@ -4277,16 +4301,16 @@
       <c r="E166" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F166" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G166" s="2" t="s">
+      <c r="F166" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G166" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>470921</v>
+        <v>470773</v>
       </c>
       <c r="B167" t="s">
         <v>7</v>
@@ -4298,18 +4322,18 @@
         <v>7</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G167" s="2" t="s">
-        <v>10</v>
+      <c r="G167" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>470974</v>
+        <v>470782</v>
       </c>
       <c r="B168" t="s">
         <v>7</v>
@@ -4321,18 +4345,18 @@
         <v>7</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>471016</v>
+        <v>470830</v>
       </c>
       <c r="B169" t="s">
         <v>7</v>
@@ -4347,15 +4371,15 @@
         <v>10</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>471028</v>
+        <v>470859</v>
       </c>
       <c r="B170" t="s">
         <v>7</v>
@@ -4366,19 +4390,19 @@
       <c r="D170" t="s">
         <v>7</v>
       </c>
-      <c r="E170" s="3" t="s">
-        <v>9</v>
+      <c r="E170" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G170" s="3" t="s">
+      <c r="G170" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>471129</v>
+        <v>470921</v>
       </c>
       <c r="B171" t="s">
         <v>7</v>
@@ -4393,15 +4417,15 @@
         <v>10</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G171" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="G171" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>471229</v>
+        <v>470974</v>
       </c>
       <c r="B172" t="s">
         <v>7</v>
@@ -4415,8 +4439,8 @@
       <c r="E172" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F172" s="3" t="s">
-        <v>9</v>
+      <c r="F172" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G172" s="2" t="s">
         <v>10</v>
@@ -4424,7 +4448,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>471255</v>
+        <v>471016</v>
       </c>
       <c r="B173" t="s">
         <v>7</v>
@@ -4447,7 +4471,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>471263</v>
+        <v>471028</v>
       </c>
       <c r="B174" t="s">
         <v>7</v>
@@ -4458,19 +4482,19 @@
       <c r="D174" t="s">
         <v>7</v>
       </c>
-      <c r="E174" s="2" t="s">
-        <v>10</v>
+      <c r="E174" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F174" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G174" s="2" t="s">
+      <c r="G174" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>471492</v>
+        <v>471129</v>
       </c>
       <c r="B175" t="s">
         <v>7</v>
@@ -4485,15 +4509,15 @@
         <v>10</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G175" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>471545</v>
+        <v>471229</v>
       </c>
       <c r="B176" t="s">
         <v>7</v>
@@ -4507,16 +4531,16 @@
       <c r="E176" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F176" s="2" t="s">
+      <c r="F176" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>471760</v>
+        <v>471255</v>
       </c>
       <c r="B177" t="s">
         <v>7</v>
@@ -4539,7 +4563,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>472004</v>
+        <v>471263</v>
       </c>
       <c r="B178" t="s">
         <v>7</v>
@@ -4551,18 +4575,18 @@
         <v>7</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>472145</v>
+        <v>471492</v>
       </c>
       <c r="B179" t="s">
         <v>7</v>
@@ -4574,7 +4598,7 @@
         <v>7</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>9</v>
@@ -4585,7 +4609,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>472434</v>
+        <v>471545</v>
       </c>
       <c r="B180" t="s">
         <v>7</v>
@@ -4597,18 +4621,18 @@
         <v>7</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>472501</v>
+        <v>471760</v>
       </c>
       <c r="B181" t="s">
         <v>7</v>
@@ -4620,18 +4644,18 @@
         <v>7</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G181" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>472537</v>
+        <v>472004</v>
       </c>
       <c r="B182" t="s">
         <v>7</v>
@@ -4643,18 +4667,18 @@
         <v>7</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G182" s="3" t="s">
-        <v>9</v>
+      <c r="G182" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>472593</v>
+        <v>472145</v>
       </c>
       <c r="B183" t="s">
         <v>7</v>
@@ -4666,10 +4690,10 @@
         <v>7</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G183" s="2" t="s">
         <v>10</v>
@@ -4677,7 +4701,7 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>472782</v>
+        <v>472434</v>
       </c>
       <c r="B184" t="s">
         <v>7</v>
@@ -4689,18 +4713,18 @@
         <v>7</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>472962</v>
+        <v>472501</v>
       </c>
       <c r="B185" t="s">
         <v>7</v>
@@ -4712,18 +4736,18 @@
         <v>7</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F185" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>473195</v>
+        <v>472537</v>
       </c>
       <c r="B186" t="s">
         <v>7</v>
@@ -4735,18 +4759,18 @@
         <v>7</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F186" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G186" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>473215</v>
+        <v>472593</v>
       </c>
       <c r="B187" t="s">
         <v>7</v>
@@ -4761,15 +4785,15 @@
         <v>10</v>
       </c>
       <c r="F187" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>473482</v>
+        <v>472782</v>
       </c>
       <c r="B188" t="s">
         <v>7</v>
@@ -4787,12 +4811,12 @@
         <v>9</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>473708</v>
+        <v>472962</v>
       </c>
       <c r="B189" t="s">
         <v>7</v>
@@ -4806,16 +4830,16 @@
       <c r="E189" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F189" s="2" t="s">
+      <c r="F189" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>473899</v>
+        <v>473195</v>
       </c>
       <c r="B190" t="s">
         <v>7</v>
@@ -4827,7 +4851,7 @@
         <v>7</v>
       </c>
       <c r="E190" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F190" s="2" t="s">
         <v>9</v>
@@ -4838,7 +4862,7 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>475115</v>
+        <v>473215</v>
       </c>
       <c r="B191" t="s">
         <v>7</v>
@@ -4853,7 +4877,7 @@
         <v>10</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G191" s="2" t="s">
         <v>9</v>
@@ -4861,7 +4885,7 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>476008</v>
+        <v>473482</v>
       </c>
       <c r="B192" t="s">
         <v>7</v>
@@ -4884,7 +4908,7 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>476289</v>
+        <v>473708</v>
       </c>
       <c r="B193" t="s">
         <v>7</v>
@@ -4898,16 +4922,16 @@
       <c r="E193" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F193" s="3" t="s">
+      <c r="F193" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>476531</v>
+        <v>473899</v>
       </c>
       <c r="B194" t="s">
         <v>7</v>
@@ -4919,10 +4943,10 @@
         <v>7</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F194" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G194" s="2" t="s">
         <v>10</v>
@@ -4930,7 +4954,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>476883</v>
+        <v>475115</v>
       </c>
       <c r="B195" t="s">
         <v>7</v>
@@ -4942,18 +4966,18 @@
         <v>7</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F195" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>476968</v>
+        <v>476008</v>
       </c>
       <c r="B196" t="s">
         <v>7</v>
@@ -4968,7 +4992,7 @@
         <v>10</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G196" s="2" t="s">
         <v>10</v>
@@ -4976,7 +5000,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>477153</v>
+        <v>476289</v>
       </c>
       <c r="B197" t="s">
         <v>7</v>
@@ -4990,7 +5014,7 @@
       <c r="E197" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F197" s="2" t="s">
+      <c r="F197" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G197" s="2" t="s">
@@ -4999,7 +5023,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>477738</v>
+        <v>476531</v>
       </c>
       <c r="B198" t="s">
         <v>7</v>
@@ -5011,10 +5035,10 @@
         <v>7</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F198" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G198" s="2" t="s">
         <v>10</v>
@@ -5022,7 +5046,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>478406</v>
+        <v>476883</v>
       </c>
       <c r="B199" t="s">
         <v>7</v>
@@ -5040,12 +5064,12 @@
         <v>9</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>478589</v>
+        <v>476968</v>
       </c>
       <c r="B200" t="s">
         <v>7</v>
@@ -5063,12 +5087,12 @@
         <v>10</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>479276</v>
+        <v>477153</v>
       </c>
       <c r="B201" t="s">
         <v>7</v>
@@ -5080,35 +5104,150 @@
         <v>7</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F201" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
+        <v>477738</v>
+      </c>
+      <c r="B202" t="s">
+        <v>7</v>
+      </c>
+      <c r="C202" t="s">
+        <v>8</v>
+      </c>
+      <c r="D202" t="s">
+        <v>7</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F202" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G202" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>478406</v>
+      </c>
+      <c r="B203" t="s">
+        <v>7</v>
+      </c>
+      <c r="C203" t="s">
+        <v>8</v>
+      </c>
+      <c r="D203" t="s">
+        <v>7</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F203" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>478589</v>
+      </c>
+      <c r="B204" t="s">
+        <v>7</v>
+      </c>
+      <c r="C204" t="s">
+        <v>8</v>
+      </c>
+      <c r="D204" t="s">
+        <v>7</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G204" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>479276</v>
+      </c>
+      <c r="B205" t="s">
+        <v>7</v>
+      </c>
+      <c r="C205" t="s">
+        <v>8</v>
+      </c>
+      <c r="D205" t="s">
+        <v>7</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F205" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G205" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
         <v>479658</v>
       </c>
-      <c r="B202" t="s">
-        <v>7</v>
-      </c>
-      <c r="C202" t="s">
-        <v>8</v>
-      </c>
-      <c r="D202" t="s">
-        <v>7</v>
-      </c>
-      <c r="E202" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F202" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G202" s="2" t="s">
+      <c r="B206" t="s">
+        <v>7</v>
+      </c>
+      <c r="C206" t="s">
+        <v>8</v>
+      </c>
+      <c r="D206" t="s">
+        <v>7</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F206" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G206" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="n">
+        <v>987654.0</v>
+      </c>
+      <c r="B207" t="s">
+        <v>7</v>
+      </c>
+      <c r="C207" t="s">
+        <v>8</v>
+      </c>
+      <c r="D207" t="s">
+        <v>31</v>
+      </c>
+      <c r="E207" t="s">
+        <v>10</v>
+      </c>
+      <c r="F207" t="s">
+        <v>9</v>
+      </c>
+      <c r="G207" t="s">
         <v>9</v>
       </c>
     </row>
@@ -5119,7 +5258,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H202"/>
+  <dimension ref="A1:H203"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9865,6 +10004,30 @@
       <c r="G202"/>
       <c r="H202"/>
     </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>23</v>
+      </c>
+      <c r="B203" t="n">
+        <v>987654.0</v>
+      </c>
+      <c r="C203" t="s">
+        <v>7</v>
+      </c>
+      <c r="D203" t="s">
+        <v>8</v>
+      </c>
+      <c r="E203" t="s">
+        <v>21</v>
+      </c>
+      <c r="F203" t="s">
+        <v>22</v>
+      </c>
+      <c r="G203" t="s">
+        <v>19</v>
+      </c>
+      <c r="H203"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Added GUIs for InformationSheet Settings
</commit_message>
<xml_diff>
--- a/data/StudentData.xlsx
+++ b/data/StudentData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25697" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25859" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -182,6 +182,18 @@
   </si>
   <si>
     <t>Humanities, SMCS</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -518,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
       <selection activeCell="F170" sqref="F170"/>
@@ -644,32 +656,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>123788</v>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>123456.0</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>130892</v>
+        <v>123788</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -681,18 +693,18 @@
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>132394</v>
+        <v>130892</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -704,18 +716,18 @@
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>132532</v>
+        <v>132394</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -738,7 +750,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>132853</v>
+        <v>132532</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -752,7 +764,7 @@
       <c r="E10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -761,7 +773,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>134333</v>
+        <v>132853</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -775,16 +787,16 @@
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>10</v>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>134390</v>
+        <v>134333</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -795,19 +807,19 @@
       <c r="D12" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>9</v>
+      <c r="E12" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>135062</v>
+        <v>134390</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -818,11 +830,11 @@
       <c r="D13" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>10</v>
+      <c r="E13" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>9</v>
@@ -830,7 +842,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>137940</v>
+        <v>135062</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -842,18 +854,18 @@
         <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>140093</v>
+        <v>137940</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -871,12 +883,12 @@
         <v>9</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>140892</v>
+        <v>140093</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -888,9 +900,9 @@
         <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -899,7 +911,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>142310</v>
+        <v>140892</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -910,19 +922,19 @@
       <c r="D17" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>9</v>
+      <c r="E17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>146632</v>
+        <v>142310</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -933,19 +945,19 @@
       <c r="D18" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>156681</v>
+        <v>146632</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
@@ -963,12 +975,12 @@
         <v>10</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>161618</v>
+        <v>156681</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -979,7 +991,7 @@
       <c r="D20" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -991,7 +1003,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>168329</v>
+        <v>161618</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
@@ -1002,11 +1014,11 @@
       <c r="D21" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>10</v>
+      <c r="E21" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>10</v>
@@ -1014,7 +1026,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>169650</v>
+        <v>168329</v>
       </c>
       <c r="B22" t="s">
         <v>7</v>
@@ -1028,7 +1040,7 @@
       <c r="E22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -1037,7 +1049,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>173425</v>
+        <v>169650</v>
       </c>
       <c r="B23" t="s">
         <v>7</v>
@@ -1051,7 +1063,7 @@
       <c r="E23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -1060,7 +1072,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>178071</v>
+        <v>173425</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
@@ -1078,12 +1090,12 @@
         <v>9</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>178156</v>
+        <v>178071</v>
       </c>
       <c r="B25" t="s">
         <v>7</v>
@@ -1101,12 +1113,12 @@
         <v>9</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>181903</v>
+        <v>178156</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
@@ -1118,18 +1130,18 @@
         <v>7</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="3" t="s">
-        <v>9</v>
+      <c r="G26" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>182120</v>
+        <v>181903</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
@@ -1141,10 +1153,10 @@
         <v>7</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>9</v>
@@ -1152,7 +1164,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>186663</v>
+        <v>182120</v>
       </c>
       <c r="B28" t="s">
         <v>7</v>
@@ -1164,10 +1176,10 @@
         <v>7</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>9</v>
@@ -1175,7 +1187,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>187393</v>
+        <v>186663</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
@@ -1192,13 +1204,13 @@
       <c r="F29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>10</v>
+      <c r="G29" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>190029</v>
+        <v>187393</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
@@ -1209,10 +1221,10 @@
       <c r="D30" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G30" s="2" t="s">
@@ -1221,7 +1233,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>194574</v>
+        <v>190029</v>
       </c>
       <c r="B31" t="s">
         <v>7</v>
@@ -1232,8 +1244,8 @@
       <c r="D31" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>10</v>
+      <c r="E31" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>9</v>
@@ -1244,7 +1256,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>198048</v>
+        <v>194574</v>
       </c>
       <c r="B32" t="s">
         <v>7</v>
@@ -1258,16 +1270,16 @@
       <c r="E32" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>9</v>
+      <c r="F32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>198741</v>
+        <v>198048</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
@@ -1284,13 +1296,13 @@
       <c r="F33" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="2" t="s">
-        <v>10</v>
+      <c r="G33" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>199787</v>
+        <v>198741</v>
       </c>
       <c r="B34" t="s">
         <v>7</v>
@@ -1302,18 +1314,18 @@
         <v>7</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>9</v>
+      <c r="G34" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>200672</v>
+        <v>199787</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
@@ -1325,110 +1337,110 @@
         <v>7</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
+        <v>200672</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>210938</v>
       </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>213456</v>
-      </c>
       <c r="B37" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
+        <v>213456</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>215351</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>41</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>42</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>43</v>
       </c>
-      <c r="E38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>225969</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="E39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>9</v>
+      </c>
+      <c r="G39" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>231348</v>
+        <v>225969</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1440,7 +1452,7 @@
         <v>7</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>10</v>
@@ -1451,76 +1463,76 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
+        <v>231348</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>232461</v>
       </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>234539</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>31</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>31</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>31</v>
       </c>
-      <c r="E42" t="s">
-        <v>10</v>
-      </c>
-      <c r="F42" t="s">
-        <v>9</v>
-      </c>
-      <c r="G42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>257317</v>
-      </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>9</v>
+      <c r="E43" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>276682</v>
+        <v>257317</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
@@ -1532,18 +1544,18 @@
         <v>7</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>278390</v>
+        <v>276682</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
@@ -1555,10 +1567,10 @@
         <v>7</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>10</v>
@@ -1566,7 +1578,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>292270</v>
+        <v>278390</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
@@ -1580,7 +1592,7 @@
       <c r="E46" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F46" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G46" s="2" t="s">
@@ -1589,7 +1601,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>292271</v>
+        <v>292270</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -1603,16 +1615,16 @@
       <c r="E47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>9</v>
+      <c r="F47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>299774</v>
+        <v>292271</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
@@ -1627,84 +1639,84 @@
         <v>10</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
+        <v>299774</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>299880</v>
       </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" t="s">
-        <v>8</v>
-      </c>
-      <c r="D49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
         <v>353515</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>38</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>39</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>40</v>
       </c>
-      <c r="E50" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
-        <v>406490</v>
-      </c>
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
-        <v>8</v>
-      </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>10</v>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>409089</v>
+        <v>406490</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -1716,7 +1728,7 @@
         <v>7</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>9</v>
@@ -1727,22 +1739,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>411168</v>
+        <v>409089</v>
       </c>
       <c r="B53" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>10</v>
@@ -1750,22 +1762,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>417688</v>
+        <v>411168</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>10</v>
@@ -1773,7 +1785,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>419371</v>
+        <v>417688</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -1784,19 +1796,19 @@
       <c r="D55" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>10</v>
+      <c r="E55" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>419659</v>
+        <v>419371</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
@@ -1819,7 +1831,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>420119</v>
+        <v>419659</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -1831,7 +1843,7 @@
         <v>7</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>9</v>
@@ -1842,7 +1854,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>436542</v>
+        <v>420119</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
@@ -1854,18 +1866,18 @@
         <v>7</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>439155</v>
+        <v>436542</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -1888,7 +1900,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>441021</v>
+        <v>439155</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
@@ -1911,7 +1923,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>442262</v>
+        <v>441021</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -1926,15 +1938,15 @@
         <v>10</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>442931</v>
+        <v>442262</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
@@ -1945,11 +1957,11 @@
       <c r="D62" t="s">
         <v>7</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>9</v>
+      <c r="E62" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>9</v>
@@ -1957,7 +1969,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>443257</v>
+        <v>442931</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
@@ -1975,12 +1987,12 @@
         <v>9</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>446253</v>
+        <v>443257</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -1991,7 +2003,7 @@
       <c r="D64" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="E64" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
@@ -2003,7 +2015,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>448013</v>
+        <v>446253</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
@@ -2015,18 +2027,18 @@
         <v>7</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>452390</v>
+        <v>448013</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
@@ -2038,9 +2050,9 @@
         <v>7</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G66" s="3" t="s">
@@ -2049,7 +2061,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>452992</v>
+        <v>452390</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
@@ -2061,7 +2073,7 @@
         <v>7</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>9</v>
@@ -2072,7 +2084,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>454280</v>
+        <v>452992</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
@@ -2095,7 +2107,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>454287</v>
+        <v>454280</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
@@ -2109,16 +2121,16 @@
       <c r="E69" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>10</v>
+      <c r="F69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>454745</v>
+        <v>454287</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
@@ -2129,19 +2141,19 @@
       <c r="D70" t="s">
         <v>7</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>9</v>
+      <c r="E70" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>454770</v>
+        <v>454745</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
@@ -2152,19 +2164,19 @@
       <c r="D71" t="s">
         <v>7</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="E71" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>10</v>
+      <c r="G71" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>455839</v>
+        <v>454770</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
@@ -2176,18 +2188,18 @@
         <v>7</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>461540</v>
+        <v>455839</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
@@ -2204,82 +2216,82 @@
       <c r="F73" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G73" s="3" t="s">
+      <c r="G73" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
+        <v>461540</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>462838</v>
       </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s">
-        <v>8</v>
-      </c>
-      <c r="D74" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>463462</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>44</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>45</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D76" t="s">
         <v>46</v>
       </c>
-      <c r="E75" t="s">
-        <v>10</v>
-      </c>
-      <c r="F75" t="s">
-        <v>9</v>
-      </c>
-      <c r="G75" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>463934</v>
-      </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" t="s">
-        <v>7</v>
-      </c>
-      <c r="E76" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G76" s="2" t="s">
+      <c r="E76" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>464863</v>
+        <v>463934</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -2290,19 +2302,19 @@
       <c r="D77" t="s">
         <v>7</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E77" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="G77" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>465018</v>
+        <v>464863</v>
       </c>
       <c r="B78" t="s">
         <v>7</v>
@@ -2314,9 +2326,9 @@
         <v>7</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F78" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F78" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G78" s="3" t="s">
@@ -2325,7 +2337,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>465085</v>
+        <v>465018</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
@@ -2339,8 +2351,8 @@
       <c r="E79" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F79" s="2" t="s">
-        <v>10</v>
+      <c r="F79" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>9</v>
@@ -2348,7 +2360,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>465090</v>
+        <v>465085</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
@@ -2363,7 +2375,7 @@
         <v>10</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>9</v>
@@ -2371,7 +2383,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>465141</v>
+        <v>465090</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -2388,13 +2400,13 @@
       <c r="F81" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G81" s="2" t="s">
+      <c r="G81" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>465275</v>
+        <v>465141</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
@@ -2406,7 +2418,7 @@
         <v>7</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>9</v>
@@ -2417,7 +2429,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>465391</v>
+        <v>465275</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
@@ -2435,12 +2447,12 @@
         <v>9</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>465431</v>
+        <v>465391</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
@@ -2451,19 +2463,19 @@
       <c r="D84" t="s">
         <v>7</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F84" s="3" t="s">
+      <c r="E84" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>465484</v>
+        <v>465431</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
@@ -2474,19 +2486,19 @@
       <c r="D85" t="s">
         <v>7</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F85" s="2" t="s">
+      <c r="E85" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>465644</v>
+        <v>465484</v>
       </c>
       <c r="B86" t="s">
         <v>7</v>
@@ -2503,13 +2515,13 @@
       <c r="F86" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G86" s="3" t="s">
-        <v>9</v>
+      <c r="G86" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>465653</v>
+        <v>465644</v>
       </c>
       <c r="B87" t="s">
         <v>7</v>
@@ -2526,13 +2538,13 @@
       <c r="F87" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G87" s="2" t="s">
-        <v>10</v>
+      <c r="G87" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>465814</v>
+        <v>465653</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
@@ -2544,18 +2556,18 @@
         <v>7</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>465850</v>
+        <v>465814</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
@@ -2567,18 +2579,18 @@
         <v>7</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>466433</v>
+        <v>465850</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
@@ -2589,8 +2601,8 @@
       <c r="D90" t="s">
         <v>7</v>
       </c>
-      <c r="E90" s="3" t="s">
-        <v>9</v>
+      <c r="E90" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>9</v>
@@ -2601,7 +2613,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>466579</v>
+        <v>466433</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
@@ -2612,88 +2624,88 @@
       <c r="D91" t="s">
         <v>7</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F91" s="2" t="s">
+      <c r="E91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
+        <v>466579</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>466801</v>
       </c>
-      <c r="B92" t="s">
-        <v>7</v>
-      </c>
-      <c r="C92" t="s">
-        <v>8</v>
-      </c>
-      <c r="D92" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93">
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
         <v>466803</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B94" t="s">
         <v>33</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C94" t="s">
         <v>33</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D94" t="s">
         <v>33</v>
       </c>
-      <c r="E93" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" t="s">
-        <v>10</v>
-      </c>
-      <c r="G93" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
-        <v>466831</v>
-      </c>
-      <c r="B94" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" t="s">
-        <v>7</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>9</v>
+      <c r="E94" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" t="s">
+        <v>10</v>
+      </c>
+      <c r="G94" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>466968</v>
+        <v>466831</v>
       </c>
       <c r="B95" t="s">
         <v>7</v>
@@ -2705,18 +2717,18 @@
         <v>7</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>467069</v>
+        <v>466968</v>
       </c>
       <c r="B96" t="s">
         <v>7</v>
@@ -2728,18 +2740,18 @@
         <v>7</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>467189</v>
+        <v>467069</v>
       </c>
       <c r="B97" t="s">
         <v>7</v>
@@ -2753,8 +2765,8 @@
       <c r="E97" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>9</v>
+      <c r="F97" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G97" s="3" t="s">
         <v>9</v>
@@ -2762,7 +2774,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>467214</v>
+        <v>467189</v>
       </c>
       <c r="B98" t="s">
         <v>7</v>
@@ -2773,19 +2785,19 @@
       <c r="D98" t="s">
         <v>7</v>
       </c>
-      <c r="E98" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>10</v>
+      <c r="E98" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>467243</v>
+        <v>467214</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
@@ -2796,11 +2808,11 @@
       <c r="D99" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>9</v>
+      <c r="E99" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>10</v>
@@ -2808,7 +2820,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>467436</v>
+        <v>467243</v>
       </c>
       <c r="B100" t="s">
         <v>7</v>
@@ -2822,16 +2834,16 @@
       <c r="E100" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F100" s="2" t="s">
+      <c r="F100" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>467451</v>
+        <v>467436</v>
       </c>
       <c r="B101" t="s">
         <v>7</v>
@@ -2842,19 +2854,19 @@
       <c r="D101" t="s">
         <v>7</v>
       </c>
-      <c r="E101" s="3" t="s">
-        <v>9</v>
+      <c r="E101" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>467455</v>
+        <v>467451</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
@@ -2865,19 +2877,19 @@
       <c r="D102" t="s">
         <v>7</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>10</v>
+      <c r="E102" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>467461</v>
+        <v>467455</v>
       </c>
       <c r="B103" t="s">
         <v>7</v>
@@ -2889,7 +2901,7 @@
         <v>7</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>9</v>
@@ -2900,7 +2912,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>467493</v>
+        <v>467461</v>
       </c>
       <c r="B104" t="s">
         <v>7</v>
@@ -2914,16 +2926,16 @@
       <c r="E104" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F104" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G104" s="3" t="s">
+      <c r="F104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>467497</v>
+        <v>467493</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>
@@ -2935,10 +2947,10 @@
         <v>7</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>9</v>
@@ -2946,7 +2958,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>467501</v>
+        <v>467497</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
@@ -2958,18 +2970,18 @@
         <v>7</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G106" s="2" t="s">
-        <v>10</v>
+      <c r="G106" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>467636</v>
+        <v>467501</v>
       </c>
       <c r="B107" t="s">
         <v>7</v>
@@ -2983,16 +2995,16 @@
       <c r="E107" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>9</v>
+      <c r="F107" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>467744</v>
+        <v>467636</v>
       </c>
       <c r="B108" t="s">
         <v>7</v>
@@ -3003,10 +3015,10 @@
       <c r="D108" t="s">
         <v>7</v>
       </c>
-      <c r="E108" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F108" s="2" t="s">
+      <c r="E108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G108" s="3" t="s">
@@ -3015,7 +3027,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>467750</v>
+        <v>467744</v>
       </c>
       <c r="B109" t="s">
         <v>7</v>
@@ -3032,13 +3044,13 @@
       <c r="F109" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G109" s="2" t="s">
-        <v>10</v>
+      <c r="G109" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>467765</v>
+        <v>467750</v>
       </c>
       <c r="B110" t="s">
         <v>7</v>
@@ -3049,10 +3061,10 @@
       <c r="D110" t="s">
         <v>7</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F110" s="3" t="s">
+      <c r="E110" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G110" s="2" t="s">
@@ -3061,7 +3073,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>467775</v>
+        <v>467765</v>
       </c>
       <c r="B111" t="s">
         <v>7</v>
@@ -3075,7 +3087,7 @@
       <c r="E111" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="F111" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G111" s="2" t="s">
@@ -3084,7 +3096,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>467836</v>
+        <v>467775</v>
       </c>
       <c r="B112" t="s">
         <v>7</v>
@@ -3107,7 +3119,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>467870</v>
+        <v>467836</v>
       </c>
       <c r="B113" t="s">
         <v>7</v>
@@ -3125,12 +3137,12 @@
         <v>9</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>467873</v>
+        <v>467870</v>
       </c>
       <c r="B114" t="s">
         <v>7</v>
@@ -3142,18 +3154,18 @@
         <v>7</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>467940</v>
+        <v>467873</v>
       </c>
       <c r="B115" t="s">
         <v>7</v>
@@ -3164,7 +3176,7 @@
       <c r="D115" t="s">
         <v>7</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="E115" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F115" s="2" t="s">
@@ -3176,7 +3188,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>467947</v>
+        <v>467940</v>
       </c>
       <c r="B116" t="s">
         <v>7</v>
@@ -3187,19 +3199,19 @@
       <c r="D116" t="s">
         <v>7</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>10</v>
+      <c r="E116" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>467963</v>
+        <v>467947</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
@@ -3211,7 +3223,7 @@
         <v>7</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>9</v>
@@ -3222,7 +3234,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>467975</v>
+        <v>467963</v>
       </c>
       <c r="B118" t="s">
         <v>7</v>
@@ -3239,24 +3251,24 @@
       <c r="F118" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G118" s="3" t="s">
+      <c r="G118" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>467986</v>
+        <v>467975</v>
       </c>
       <c r="B119" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C119" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D119" t="s">
         <v>7</v>
       </c>
-      <c r="E119" s="3" t="s">
+      <c r="E119" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F119" s="2" t="s">
@@ -3268,30 +3280,30 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>468167</v>
+        <v>467986</v>
       </c>
       <c r="B120" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C120" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D120" t="s">
         <v>7</v>
       </c>
-      <c r="E120" s="2" t="s">
+      <c r="E120" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G120" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>468178</v>
+        <v>468167</v>
       </c>
       <c r="B121" t="s">
         <v>7</v>
@@ -3303,18 +3315,18 @@
         <v>7</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>468255</v>
+        <v>468178</v>
       </c>
       <c r="B122" t="s">
         <v>7</v>
@@ -3326,10 +3338,10 @@
         <v>7</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>9</v>
@@ -3337,7 +3349,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>468284</v>
+        <v>468255</v>
       </c>
       <c r="B123" t="s">
         <v>7</v>
@@ -3349,10 +3361,10 @@
         <v>7</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>9</v>
@@ -3360,7 +3372,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>468311</v>
+        <v>468284</v>
       </c>
       <c r="B124" t="s">
         <v>7</v>
@@ -3372,10 +3384,10 @@
         <v>7</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>9</v>
@@ -3383,7 +3395,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>468546</v>
+        <v>468311</v>
       </c>
       <c r="B125" t="s">
         <v>7</v>
@@ -3395,18 +3407,18 @@
         <v>7</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F125" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>468554</v>
+        <v>468546</v>
       </c>
       <c r="B126" t="s">
         <v>7</v>
@@ -3418,10 +3430,10 @@
         <v>7</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>10</v>
@@ -3429,7 +3441,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>468607</v>
+        <v>468554</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
@@ -3441,10 +3453,10 @@
         <v>7</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>10</v>
@@ -3452,7 +3464,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>468643</v>
+        <v>468607</v>
       </c>
       <c r="B128" t="s">
         <v>7</v>
@@ -3475,7 +3487,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>468736</v>
+        <v>468643</v>
       </c>
       <c r="B129" t="s">
         <v>7</v>
@@ -3489,16 +3501,16 @@
       <c r="E129" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F129" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G129" s="3" t="s">
-        <v>9</v>
+      <c r="F129" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>468763</v>
+        <v>468736</v>
       </c>
       <c r="B130" t="s">
         <v>7</v>
@@ -3510,18 +3522,18 @@
         <v>7</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F130" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G130" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>468859</v>
+        <v>468763</v>
       </c>
       <c r="B131" t="s">
         <v>7</v>
@@ -3533,18 +3545,18 @@
         <v>7</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G131" s="3" t="s">
-        <v>9</v>
+      <c r="G131" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>468876</v>
+        <v>468859</v>
       </c>
       <c r="B132" t="s">
         <v>7</v>
@@ -3556,10 +3568,10 @@
         <v>7</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F132" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>9</v>
@@ -3567,7 +3579,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>468882</v>
+        <v>468876</v>
       </c>
       <c r="B133" t="s">
         <v>7</v>
@@ -3581,7 +3593,7 @@
       <c r="E133" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F133" s="2" t="s">
+      <c r="F133" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G133" s="3" t="s">
@@ -3590,7 +3602,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>468898</v>
+        <v>468882</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
@@ -3605,62 +3617,62 @@
         <v>9</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G134" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
+        <v>468898</v>
+      </c>
+      <c r="B135" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135" t="s">
+        <v>8</v>
+      </c>
+      <c r="D135" t="s">
+        <v>7</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
         <v>468903</v>
       </c>
-      <c r="B135" t="s">
-        <v>7</v>
-      </c>
-      <c r="C135" t="s">
-        <v>8</v>
-      </c>
-      <c r="D135" t="s">
-        <v>7</v>
-      </c>
-      <c r="E135" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="4">
+      <c r="B136" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136" t="s">
+        <v>8</v>
+      </c>
+      <c r="D136" t="s">
+        <v>7</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="4">
         <v>468961</v>
       </c>
-      <c r="B136" t="s">
-        <v>7</v>
-      </c>
-      <c r="C136" t="s">
-        <v>8</v>
-      </c>
-      <c r="D136" t="s">
-        <v>7</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="1">
-        <v>469129</v>
-      </c>
       <c r="B137" t="s">
         <v>7</v>
       </c>
@@ -3674,7 +3686,7 @@
         <v>10</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G137" s="3" t="s">
         <v>9</v>
@@ -3682,7 +3694,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>469142</v>
+        <v>469129</v>
       </c>
       <c r="B138" t="s">
         <v>7</v>
@@ -3699,13 +3711,13 @@
       <c r="F138" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G138" s="2" t="s">
+      <c r="G138" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>469186</v>
+        <v>469142</v>
       </c>
       <c r="B139" t="s">
         <v>7</v>
@@ -3717,10 +3729,10 @@
         <v>7</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F139" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>9</v>
@@ -3728,7 +3740,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>469193</v>
+        <v>469186</v>
       </c>
       <c r="B140" t="s">
         <v>7</v>
@@ -3739,7 +3751,7 @@
       <c r="D140" t="s">
         <v>7</v>
       </c>
-      <c r="E140" s="3" t="s">
+      <c r="E140" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F140" s="3" t="s">
@@ -3751,7 +3763,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>469213</v>
+        <v>469193</v>
       </c>
       <c r="B141" t="s">
         <v>7</v>
@@ -3762,66 +3774,66 @@
       <c r="D141" t="s">
         <v>7</v>
       </c>
-      <c r="E141" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F141" s="2" t="s">
+      <c r="E141" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F141" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G141" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
+        <v>469213</v>
+      </c>
+      <c r="B142" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" t="s">
+        <v>7</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
         <v>469288</v>
       </c>
-      <c r="B142" t="s">
-        <v>7</v>
-      </c>
-      <c r="C142" t="s">
-        <v>8</v>
-      </c>
-      <c r="D142" t="s">
-        <v>7</v>
-      </c>
-      <c r="E142" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F142" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G142" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="4">
+      <c r="B143" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143" t="s">
+        <v>8</v>
+      </c>
+      <c r="D143" t="s">
+        <v>7</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="4">
         <v>469327</v>
       </c>
-      <c r="B143" t="s">
-        <v>7</v>
-      </c>
-      <c r="C143" t="s">
-        <v>8</v>
-      </c>
-      <c r="D143" t="s">
-        <v>7</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F143" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G143" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A144" s="1">
-        <v>469351</v>
-      </c>
       <c r="B144" t="s">
         <v>7</v>
       </c>
@@ -3835,7 +3847,7 @@
         <v>9</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>10</v>
@@ -3843,7 +3855,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>469358</v>
+        <v>469351</v>
       </c>
       <c r="B145" t="s">
         <v>7</v>
@@ -3854,19 +3866,19 @@
       <c r="D145" t="s">
         <v>7</v>
       </c>
-      <c r="E145" s="3" t="s">
+      <c r="E145" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F145" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>469474</v>
+        <v>469358</v>
       </c>
       <c r="B146" t="s">
         <v>7</v>
@@ -3877,19 +3889,19 @@
       <c r="D146" t="s">
         <v>7</v>
       </c>
-      <c r="E146" s="2" t="s">
+      <c r="E146" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G146" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G146" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>469486</v>
+        <v>469474</v>
       </c>
       <c r="B147" t="s">
         <v>7</v>
@@ -3901,18 +3913,18 @@
         <v>7</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G147" s="2" t="s">
-        <v>10</v>
+      <c r="G147" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>469625</v>
+        <v>469486</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
@@ -3924,18 +3936,18 @@
         <v>7</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F148" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>469740</v>
+        <v>469625</v>
       </c>
       <c r="B149" t="s">
         <v>7</v>
@@ -3949,7 +3961,7 @@
       <c r="E149" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F149" s="3" t="s">
+      <c r="F149" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G149" s="2" t="s">
@@ -3958,7 +3970,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>469823</v>
+        <v>469740</v>
       </c>
       <c r="B150" t="s">
         <v>7</v>
@@ -3972,16 +3984,16 @@
       <c r="E150" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F150" s="2" t="s">
-        <v>10</v>
+      <c r="F150" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>469857</v>
+        <v>469823</v>
       </c>
       <c r="B151" t="s">
         <v>7</v>
@@ -3993,18 +4005,18 @@
         <v>7</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>469975</v>
+        <v>469857</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
@@ -4016,7 +4028,7 @@
         <v>7</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>9</v>
@@ -4027,7 +4039,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>470129</v>
+        <v>469975</v>
       </c>
       <c r="B153" t="s">
         <v>7</v>
@@ -4039,18 +4051,18 @@
         <v>7</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>470144</v>
+        <v>470129</v>
       </c>
       <c r="B154" t="s">
         <v>7</v>
@@ -4065,15 +4077,15 @@
         <v>10</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>470282</v>
+        <v>470144</v>
       </c>
       <c r="B155" t="s">
         <v>7</v>
@@ -4085,10 +4097,10 @@
         <v>7</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G155" s="2" t="s">
         <v>9</v>
@@ -4096,7 +4108,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>470290</v>
+        <v>470282</v>
       </c>
       <c r="B156" t="s">
         <v>7</v>
@@ -4108,18 +4120,18 @@
         <v>7</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G156" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G156" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>470309</v>
+        <v>470290</v>
       </c>
       <c r="B157" t="s">
         <v>7</v>
@@ -4131,18 +4143,18 @@
         <v>7</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F157" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G157" s="2" t="s">
-        <v>10</v>
+      <c r="G157" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>470373</v>
+        <v>470309</v>
       </c>
       <c r="B158" t="s">
         <v>7</v>
@@ -4154,18 +4166,18 @@
         <v>7</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>470405</v>
+        <v>470373</v>
       </c>
       <c r="B159" t="s">
         <v>7</v>
@@ -4180,15 +4192,15 @@
         <v>10</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G159" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G159" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>470467</v>
+        <v>470405</v>
       </c>
       <c r="B160" t="s">
         <v>7</v>
@@ -4203,15 +4215,15 @@
         <v>10</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G160" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G160" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>470488</v>
+        <v>470467</v>
       </c>
       <c r="B161" t="s">
         <v>7</v>
@@ -4225,7 +4237,7 @@
       <c r="E161" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F161" s="3" t="s">
+      <c r="F161" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G161" s="2" t="s">
@@ -4234,7 +4246,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>470638</v>
+        <v>470488</v>
       </c>
       <c r="B162" t="s">
         <v>7</v>
@@ -4252,12 +4264,12 @@
         <v>9</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>470668</v>
+        <v>470638</v>
       </c>
       <c r="B163" t="s">
         <v>7</v>
@@ -4269,10 +4281,10 @@
         <v>7</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F163" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G163" s="2" t="s">
         <v>10</v>
@@ -4280,7 +4292,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>470754</v>
+        <v>470668</v>
       </c>
       <c r="B164" t="s">
         <v>7</v>
@@ -4292,18 +4304,18 @@
         <v>7</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F164" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G164" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="F164" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G164" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>470773</v>
+        <v>470754</v>
       </c>
       <c r="B165" t="s">
         <v>7</v>
@@ -4315,9 +4327,9 @@
         <v>7</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F165" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F165" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G165" s="3" t="s">
@@ -4326,7 +4338,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>470782</v>
+        <v>470773</v>
       </c>
       <c r="B166" t="s">
         <v>7</v>
@@ -4343,13 +4355,13 @@
       <c r="F166" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G166" s="2" t="s">
+      <c r="G166" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>470830</v>
+        <v>470782</v>
       </c>
       <c r="B167" t="s">
         <v>7</v>
@@ -4361,10 +4373,10 @@
         <v>7</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G167" s="2" t="s">
         <v>9</v>
@@ -4372,7 +4384,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>470859</v>
+        <v>470830</v>
       </c>
       <c r="B168" t="s">
         <v>7</v>
@@ -4387,7 +4399,7 @@
         <v>10</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G168" s="2" t="s">
         <v>9</v>
@@ -4395,7 +4407,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>470921</v>
+        <v>470859</v>
       </c>
       <c r="B169" t="s">
         <v>7</v>
@@ -4413,12 +4425,12 @@
         <v>9</v>
       </c>
       <c r="G169" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>471016</v>
+        <v>470921</v>
       </c>
       <c r="B170" t="s">
         <v>7</v>
@@ -4441,7 +4453,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>471028</v>
+        <v>471016</v>
       </c>
       <c r="B171" t="s">
         <v>7</v>
@@ -4452,19 +4464,19 @@
       <c r="D171" t="s">
         <v>7</v>
       </c>
-      <c r="E171" s="3" t="s">
-        <v>9</v>
+      <c r="E171" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G171" s="3" t="s">
-        <v>9</v>
+      <c r="G171" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>471129</v>
+        <v>471028</v>
       </c>
       <c r="B172" t="s">
         <v>7</v>
@@ -4475,11 +4487,11 @@
       <c r="D172" t="s">
         <v>7</v>
       </c>
-      <c r="E172" s="2" t="s">
-        <v>10</v>
+      <c r="E172" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G172" s="3" t="s">
         <v>9</v>
@@ -4487,7 +4499,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>471229</v>
+        <v>471129</v>
       </c>
       <c r="B173" t="s">
         <v>7</v>
@@ -4501,16 +4513,16 @@
       <c r="E173" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F173" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G173" s="2" t="s">
-        <v>10</v>
+      <c r="F173" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>471255</v>
+        <v>471229</v>
       </c>
       <c r="B174" t="s">
         <v>7</v>
@@ -4524,7 +4536,7 @@
       <c r="E174" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F174" s="2" t="s">
+      <c r="F174" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G174" s="2" t="s">
@@ -4533,7 +4545,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>471263</v>
+        <v>471255</v>
       </c>
       <c r="B175" t="s">
         <v>7</v>
@@ -4551,12 +4563,12 @@
         <v>9</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>471492</v>
+        <v>471263</v>
       </c>
       <c r="B176" t="s">
         <v>7</v>
@@ -4574,12 +4586,12 @@
         <v>9</v>
       </c>
       <c r="G176" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>471545</v>
+        <v>471492</v>
       </c>
       <c r="B177" t="s">
         <v>7</v>
@@ -4597,12 +4609,12 @@
         <v>9</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>471760</v>
+        <v>471545</v>
       </c>
       <c r="B178" t="s">
         <v>7</v>
@@ -4620,12 +4632,12 @@
         <v>9</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>472004</v>
+        <v>471760</v>
       </c>
       <c r="B179" t="s">
         <v>7</v>
@@ -4637,10 +4649,10 @@
         <v>7</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G179" s="2" t="s">
         <v>10</v>
@@ -4648,7 +4660,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>472145</v>
+        <v>472004</v>
       </c>
       <c r="B180" t="s">
         <v>7</v>
@@ -4663,7 +4675,7 @@
         <v>9</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G180" s="2" t="s">
         <v>10</v>
@@ -4671,7 +4683,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>472434</v>
+        <v>472145</v>
       </c>
       <c r="B181" t="s">
         <v>7</v>
@@ -4686,7 +4698,7 @@
         <v>9</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G181" s="2" t="s">
         <v>10</v>
@@ -4694,7 +4706,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>472501</v>
+        <v>472434</v>
       </c>
       <c r="B182" t="s">
         <v>7</v>
@@ -4709,15 +4721,15 @@
         <v>9</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G182" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>472537</v>
+        <v>472501</v>
       </c>
       <c r="B183" t="s">
         <v>7</v>
@@ -4729,18 +4741,18 @@
         <v>7</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G183" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G183" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>472782</v>
+        <v>472537</v>
       </c>
       <c r="B184" t="s">
         <v>7</v>
@@ -4755,15 +4767,15 @@
         <v>10</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G184" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G184" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>472962</v>
+        <v>472782</v>
       </c>
       <c r="B185" t="s">
         <v>7</v>
@@ -4777,16 +4789,16 @@
       <c r="E185" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F185" s="3" t="s">
+      <c r="F185" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G185" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>473195</v>
+        <v>472962</v>
       </c>
       <c r="B186" t="s">
         <v>7</v>
@@ -4798,9 +4810,9 @@
         <v>7</v>
       </c>
       <c r="E186" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F186" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F186" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G186" s="2" t="s">
@@ -4809,7 +4821,7 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>473215</v>
+        <v>473195</v>
       </c>
       <c r="B187" t="s">
         <v>7</v>
@@ -4821,18 +4833,18 @@
         <v>7</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F187" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>473482</v>
+        <v>473215</v>
       </c>
       <c r="B188" t="s">
         <v>7</v>
@@ -4850,12 +4862,12 @@
         <v>9</v>
       </c>
       <c r="G188" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>473708</v>
+        <v>473482</v>
       </c>
       <c r="B189" t="s">
         <v>7</v>
@@ -4873,12 +4885,12 @@
         <v>9</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>473899</v>
+        <v>473708</v>
       </c>
       <c r="B190" t="s">
         <v>7</v>
@@ -4896,12 +4908,12 @@
         <v>9</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>475115</v>
+        <v>473899</v>
       </c>
       <c r="B191" t="s">
         <v>7</v>
@@ -4916,15 +4928,15 @@
         <v>10</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>476008</v>
+        <v>475115</v>
       </c>
       <c r="B192" t="s">
         <v>7</v>
@@ -4939,15 +4951,15 @@
         <v>10</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>476289</v>
+        <v>476008</v>
       </c>
       <c r="B193" t="s">
         <v>7</v>
@@ -4961,7 +4973,7 @@
       <c r="E193" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F193" s="3" t="s">
+      <c r="F193" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G193" s="2" t="s">
@@ -4970,7 +4982,7 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>476531</v>
+        <v>476289</v>
       </c>
       <c r="B194" t="s">
         <v>7</v>
@@ -4982,10 +4994,10 @@
         <v>7</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F194" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="F194" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G194" s="2" t="s">
         <v>10</v>
@@ -4993,7 +5005,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>476883</v>
+        <v>476531</v>
       </c>
       <c r="B195" t="s">
         <v>7</v>
@@ -5008,7 +5020,7 @@
         <v>9</v>
       </c>
       <c r="F195" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G195" s="2" t="s">
         <v>10</v>
@@ -5016,7 +5028,7 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>477153</v>
+        <v>476883</v>
       </c>
       <c r="B196" t="s">
         <v>7</v>
@@ -5028,7 +5040,7 @@
         <v>7</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F196" s="2" t="s">
         <v>9</v>
@@ -5039,7 +5051,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>477738</v>
+        <v>477153</v>
       </c>
       <c r="B197" t="s">
         <v>7</v>
@@ -5062,7 +5074,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>478406</v>
+        <v>477738</v>
       </c>
       <c r="B198" t="s">
         <v>7</v>
@@ -5074,18 +5086,18 @@
         <v>7</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F198" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G198" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>478589</v>
+        <v>478406</v>
       </c>
       <c r="B199" t="s">
         <v>7</v>
@@ -5097,10 +5109,10 @@
         <v>7</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F199" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G199" s="2" t="s">
         <v>9</v>
@@ -5108,7 +5120,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>479276</v>
+        <v>478589</v>
       </c>
       <c r="B200" t="s">
         <v>7</v>
@@ -5120,10 +5132,10 @@
         <v>7</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F200" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G200" s="2" t="s">
         <v>9</v>
@@ -5131,47 +5143,70 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
+        <v>479276</v>
+      </c>
+      <c r="B201" t="s">
+        <v>7</v>
+      </c>
+      <c r="C201" t="s">
+        <v>8</v>
+      </c>
+      <c r="D201" t="s">
+        <v>7</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F201" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G201" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
         <v>479658</v>
       </c>
-      <c r="B201" t="s">
-        <v>7</v>
-      </c>
-      <c r="C201" t="s">
-        <v>8</v>
-      </c>
-      <c r="D201" t="s">
-        <v>7</v>
-      </c>
-      <c r="E201" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F201" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G201" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A202">
+      <c r="B202" t="s">
+        <v>7</v>
+      </c>
+      <c r="C202" t="s">
+        <v>8</v>
+      </c>
+      <c r="D202" t="s">
+        <v>7</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F202" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G202" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203">
         <v>987654</v>
       </c>
-      <c r="B202" t="s">
-        <v>7</v>
-      </c>
-      <c r="C202" t="s">
-        <v>8</v>
-      </c>
-      <c r="D202" t="s">
+      <c r="B203" t="s">
+        <v>7</v>
+      </c>
+      <c r="C203" t="s">
+        <v>8</v>
+      </c>
+      <c r="D203" t="s">
         <v>30</v>
       </c>
-      <c r="E202" t="s">
-        <v>10</v>
-      </c>
-      <c r="F202" t="s">
-        <v>9</v>
-      </c>
-      <c r="G202" t="s">
+      <c r="E203" t="s">
+        <v>10</v>
+      </c>
+      <c r="F203" t="s">
+        <v>9</v>
+      </c>
+      <c r="G203" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a Data wasn't added to the application screen
</commit_message>
<xml_diff>
--- a/data/StudentData.xlsx
+++ b/data/StudentData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mecha\Documents\GitHub\Invited-Meeting-Scheduler\data\"/>
     </mc:Choice>
@@ -14,10 +14,11 @@
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
+    <sheet name="ScheduleData" r:id="rId5" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11863" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -140,11 +141,60 @@
   <si>
     <t>tjftnntd</t>
   </si>
+  <si>
+    <t>Rotations Needed</t>
+  </si>
+  <si>
+    <t>ROT1</t>
+  </si>
+  <si>
+    <t>ROT2</t>
+  </si>
+  <si>
+    <t>ROT3</t>
+  </si>
+  <si>
+    <t>ROT4</t>
+  </si>
+  <si>
+    <t>1 Rotations: SMCS</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>3 Rotations: Global, Humanities, SMCS</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>2 Rotations: Global, Humanities</t>
+  </si>
+  <si>
+    <t>1 Rotations: Global</t>
+  </si>
+  <si>
+    <t>1 Rotations: Humanities</t>
+  </si>
+  <si>
+    <t>2 Rotations: Global, SMCS</t>
+  </si>
+  <si>
+    <t>2 Rotations: Humanities, SMCS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -482,7 +532,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5203,4 +5253,4839 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H205"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="n">
+        <v>111111.0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="n">
+        <v>122534.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="n">
+        <v>122789.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="n">
+        <v>122873.0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="n">
+        <v>123456.0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="n">
+        <v>123788.0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="n">
+        <v>130892.0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="n">
+        <v>132394.0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="n">
+        <v>132532.0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" t="n">
+        <v>132853.0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="n">
+        <v>134333.0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="n">
+        <v>134390.0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="n">
+        <v>135062.0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="n">
+        <v>137940.0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="n">
+        <v>140093.0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="n">
+        <v>140892.0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="n">
+        <v>142310.0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="n">
+        <v>146632.0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="n">
+        <v>156681.0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="n">
+        <v>161618.0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21"/>
+      <c r="H21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="n">
+        <v>168329.0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="n">
+        <v>169650.0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23"/>
+      <c r="H23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="n">
+        <v>173425.0</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="n">
+        <v>178071.0</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="n">
+        <v>178156.0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26"/>
+      <c r="H26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="n">
+        <v>181903.0</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="n">
+        <v>182120.0</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="n">
+        <v>186663.0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>47</v>
+      </c>
+      <c r="G29" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="n">
+        <v>187393.0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" t="n">
+        <v>190029.0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="n">
+        <v>194574.0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>48</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="n">
+        <v>198048.0</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="n">
+        <v>198741.0</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="n">
+        <v>199787.0</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="n">
+        <v>200672.0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36"/>
+      <c r="H36"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="n">
+        <v>210938.0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="n">
+        <v>213456.0</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" t="s">
+        <v>45</v>
+      </c>
+      <c r="G38" t="s">
+        <v>48</v>
+      </c>
+      <c r="H38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="n">
+        <v>215351.0</v>
+      </c>
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" t="n">
+        <v>225969.0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40"/>
+      <c r="H40"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="n">
+        <v>231348.0</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>45</v>
+      </c>
+      <c r="G41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" t="n">
+        <v>232461.0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G42"/>
+      <c r="H42"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="n">
+        <v>234539.0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" t="s">
+        <v>48</v>
+      </c>
+      <c r="G43"/>
+      <c r="H43"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="n">
+        <v>257317.0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" t="s">
+        <v>47</v>
+      </c>
+      <c r="G44"/>
+      <c r="H44"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>276682.0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" t="s">
+        <v>44</v>
+      </c>
+      <c r="G45"/>
+      <c r="H45"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" t="n">
+        <v>278390.0</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G46"/>
+      <c r="H46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="n">
+        <v>292270.0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" t="s">
+        <v>48</v>
+      </c>
+      <c r="G47"/>
+      <c r="H47"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" t="n">
+        <v>292271.0</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" t="s">
+        <v>44</v>
+      </c>
+      <c r="G48"/>
+      <c r="H48"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" t="n">
+        <v>299774.0</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49"/>
+      <c r="H49"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" t="n">
+        <v>299880.0</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" t="s">
+        <v>48</v>
+      </c>
+      <c r="G50"/>
+      <c r="H50"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="n">
+        <v>353515.0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" t="s">
+        <v>22</v>
+      </c>
+      <c r="E51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" t="s">
+        <v>47</v>
+      </c>
+      <c r="G51" t="s">
+        <v>44</v>
+      </c>
+      <c r="H51"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="n">
+        <v>353621.0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" t="s">
+        <v>48</v>
+      </c>
+      <c r="F52" t="s">
+        <v>45</v>
+      </c>
+      <c r="G52" t="s">
+        <v>44</v>
+      </c>
+      <c r="H52"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="n">
+        <v>406490.0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" t="s">
+        <v>48</v>
+      </c>
+      <c r="F53" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" t="s">
+        <v>44</v>
+      </c>
+      <c r="H53"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" t="n">
+        <v>409089.0</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" t="s">
+        <v>44</v>
+      </c>
+      <c r="G54"/>
+      <c r="H54"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>43</v>
+      </c>
+      <c r="B55" t="n">
+        <v>411168.0</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" t="s">
+        <v>45</v>
+      </c>
+      <c r="G55"/>
+      <c r="H55"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" t="n">
+        <v>417688.0</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" t="s">
+        <v>48</v>
+      </c>
+      <c r="G56" t="s">
+        <v>44</v>
+      </c>
+      <c r="H56"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" t="n">
+        <v>419371.0</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" t="s">
+        <v>48</v>
+      </c>
+      <c r="G57" t="s">
+        <v>47</v>
+      </c>
+      <c r="H57"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" t="n">
+        <v>419659.0</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>44</v>
+      </c>
+      <c r="F58" t="s">
+        <v>48</v>
+      </c>
+      <c r="G58" t="s">
+        <v>47</v>
+      </c>
+      <c r="H58"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" t="n">
+        <v>420119.0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" t="s">
+        <v>47</v>
+      </c>
+      <c r="G59" t="s">
+        <v>44</v>
+      </c>
+      <c r="H59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" t="n">
+        <v>436542.0</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>44</v>
+      </c>
+      <c r="F60" t="s">
+        <v>48</v>
+      </c>
+      <c r="G60"/>
+      <c r="H60"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" t="n">
+        <v>439155.0</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>48</v>
+      </c>
+      <c r="F61" t="s">
+        <v>44</v>
+      </c>
+      <c r="G61"/>
+      <c r="H61"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62" t="n">
+        <v>441021.0</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>44</v>
+      </c>
+      <c r="F62" t="s">
+        <v>48</v>
+      </c>
+      <c r="G62"/>
+      <c r="H62"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>51</v>
+      </c>
+      <c r="B63" t="n">
+        <v>442262.0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>44</v>
+      </c>
+      <c r="F63" t="s">
+        <v>47</v>
+      </c>
+      <c r="G63"/>
+      <c r="H63"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>46</v>
+      </c>
+      <c r="B64" t="n">
+        <v>442931.0</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>47</v>
+      </c>
+      <c r="F64" t="s">
+        <v>45</v>
+      </c>
+      <c r="G64" t="s">
+        <v>48</v>
+      </c>
+      <c r="H64" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B65" t="n">
+        <v>443257.0</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" t="s">
+        <v>44</v>
+      </c>
+      <c r="G65" t="s">
+        <v>48</v>
+      </c>
+      <c r="H65"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>52</v>
+      </c>
+      <c r="B66" t="n">
+        <v>446253.0</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" t="s">
+        <v>48</v>
+      </c>
+      <c r="G66" t="s">
+        <v>44</v>
+      </c>
+      <c r="H66"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>49</v>
+      </c>
+      <c r="B67" t="n">
+        <v>448013.0</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>48</v>
+      </c>
+      <c r="F67" t="s">
+        <v>44</v>
+      </c>
+      <c r="G67" t="s">
+        <v>47</v>
+      </c>
+      <c r="H67"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68" t="n">
+        <v>452390.0</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" t="s">
+        <v>47</v>
+      </c>
+      <c r="G68" t="s">
+        <v>44</v>
+      </c>
+      <c r="H68" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>49</v>
+      </c>
+      <c r="B69" t="n">
+        <v>452992.0</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>8</v>
+      </c>
+      <c r="E69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F69" t="s">
+        <v>48</v>
+      </c>
+      <c r="G69" t="s">
+        <v>44</v>
+      </c>
+      <c r="H69"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>49</v>
+      </c>
+      <c r="B70" t="n">
+        <v>454280.0</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
+        <v>8</v>
+      </c>
+      <c r="E70" t="s">
+        <v>48</v>
+      </c>
+      <c r="F70" t="s">
+        <v>44</v>
+      </c>
+      <c r="G70" t="s">
+        <v>47</v>
+      </c>
+      <c r="H70"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>50</v>
+      </c>
+      <c r="B71" t="n">
+        <v>454287.0</v>
+      </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" t="s">
+        <v>8</v>
+      </c>
+      <c r="E71" t="s">
+        <v>48</v>
+      </c>
+      <c r="F71" t="s">
+        <v>44</v>
+      </c>
+      <c r="G71"/>
+      <c r="H71"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>53</v>
+      </c>
+      <c r="B72" t="n">
+        <v>454745.0</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" t="s">
+        <v>8</v>
+      </c>
+      <c r="E72" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" t="s">
+        <v>45</v>
+      </c>
+      <c r="G72" t="s">
+        <v>47</v>
+      </c>
+      <c r="H72"/>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>43</v>
+      </c>
+      <c r="B73" t="n">
+        <v>454770.0</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>8</v>
+      </c>
+      <c r="E73" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" t="s">
+        <v>44</v>
+      </c>
+      <c r="G73"/>
+      <c r="H73"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>49</v>
+      </c>
+      <c r="B74" t="n">
+        <v>455839.0</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" t="s">
+        <v>8</v>
+      </c>
+      <c r="E74" t="s">
+        <v>48</v>
+      </c>
+      <c r="F74" t="s">
+        <v>44</v>
+      </c>
+      <c r="G74" t="s">
+        <v>47</v>
+      </c>
+      <c r="H74"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>49</v>
+      </c>
+      <c r="B75" t="n">
+        <v>461540.0</v>
+      </c>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>8</v>
+      </c>
+      <c r="E75" t="s">
+        <v>47</v>
+      </c>
+      <c r="F75" t="s">
+        <v>48</v>
+      </c>
+      <c r="G75" t="s">
+        <v>44</v>
+      </c>
+      <c r="H75"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>49</v>
+      </c>
+      <c r="B76" t="n">
+        <v>462838.0</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" t="s">
+        <v>8</v>
+      </c>
+      <c r="E76" t="s">
+        <v>48</v>
+      </c>
+      <c r="F76" t="s">
+        <v>47</v>
+      </c>
+      <c r="G76" t="s">
+        <v>44</v>
+      </c>
+      <c r="H76"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B77" t="n">
+        <v>463462.0</v>
+      </c>
+      <c r="C77" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F77" t="s">
+        <v>48</v>
+      </c>
+      <c r="G77" t="s">
+        <v>44</v>
+      </c>
+      <c r="H77"/>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B78" t="n">
+        <v>463934.0</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" t="s">
+        <v>47</v>
+      </c>
+      <c r="F78" t="s">
+        <v>45</v>
+      </c>
+      <c r="G78" t="s">
+        <v>48</v>
+      </c>
+      <c r="H78" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>46</v>
+      </c>
+      <c r="B79" t="n">
+        <v>464863.0</v>
+      </c>
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" t="s">
+        <v>45</v>
+      </c>
+      <c r="F79" t="s">
+        <v>47</v>
+      </c>
+      <c r="G79" t="s">
+        <v>44</v>
+      </c>
+      <c r="H79" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>49</v>
+      </c>
+      <c r="B80" t="n">
+        <v>465018.0</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>8</v>
+      </c>
+      <c r="E80" t="s">
+        <v>48</v>
+      </c>
+      <c r="F80" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" t="s">
+        <v>44</v>
+      </c>
+      <c r="H80"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>51</v>
+      </c>
+      <c r="B81" t="n">
+        <v>465085.0</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" t="s">
+        <v>47</v>
+      </c>
+      <c r="F81" t="s">
+        <v>44</v>
+      </c>
+      <c r="G81"/>
+      <c r="H81"/>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>49</v>
+      </c>
+      <c r="B82" t="n">
+        <v>465090.0</v>
+      </c>
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" t="s">
+        <v>47</v>
+      </c>
+      <c r="F82" t="s">
+        <v>48</v>
+      </c>
+      <c r="G82" t="s">
+        <v>44</v>
+      </c>
+      <c r="H82"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>49</v>
+      </c>
+      <c r="B83" t="n">
+        <v>465141.0</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" t="s">
+        <v>44</v>
+      </c>
+      <c r="F83" t="s">
+        <v>47</v>
+      </c>
+      <c r="G83" t="s">
+        <v>48</v>
+      </c>
+      <c r="H83"/>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B84" t="n">
+        <v>465275.0</v>
+      </c>
+      <c r="C84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" t="s">
+        <v>47</v>
+      </c>
+      <c r="F84" t="s">
+        <v>45</v>
+      </c>
+      <c r="G84" t="s">
+        <v>48</v>
+      </c>
+      <c r="H84" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" t="n">
+        <v>465391.0</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" t="s">
+        <v>48</v>
+      </c>
+      <c r="F85" t="s">
+        <v>45</v>
+      </c>
+      <c r="G85" t="s">
+        <v>44</v>
+      </c>
+      <c r="H85"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>46</v>
+      </c>
+      <c r="B86" t="n">
+        <v>465431.0</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>8</v>
+      </c>
+      <c r="E86" t="s">
+        <v>45</v>
+      </c>
+      <c r="F86" t="s">
+        <v>47</v>
+      </c>
+      <c r="G86" t="s">
+        <v>44</v>
+      </c>
+      <c r="H86" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>50</v>
+      </c>
+      <c r="B87" t="n">
+        <v>465484.0</v>
+      </c>
+      <c r="C87" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>8</v>
+      </c>
+      <c r="E87" t="s">
+        <v>44</v>
+      </c>
+      <c r="F87" t="s">
+        <v>48</v>
+      </c>
+      <c r="G87"/>
+      <c r="H87"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>49</v>
+      </c>
+      <c r="B88" t="n">
+        <v>465644.0</v>
+      </c>
+      <c r="C88" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" t="s">
+        <v>8</v>
+      </c>
+      <c r="E88" t="s">
+        <v>48</v>
+      </c>
+      <c r="F88" t="s">
+        <v>47</v>
+      </c>
+      <c r="G88" t="s">
+        <v>44</v>
+      </c>
+      <c r="H88"/>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>50</v>
+      </c>
+      <c r="B89" t="n">
+        <v>465653.0</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>8</v>
+      </c>
+      <c r="E89" t="s">
+        <v>48</v>
+      </c>
+      <c r="F89" t="s">
+        <v>44</v>
+      </c>
+      <c r="G89"/>
+      <c r="H89"/>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>46</v>
+      </c>
+      <c r="B90" t="n">
+        <v>465814.0</v>
+      </c>
+      <c r="C90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" t="s">
+        <v>8</v>
+      </c>
+      <c r="E90" t="s">
+        <v>47</v>
+      </c>
+      <c r="F90" t="s">
+        <v>45</v>
+      </c>
+      <c r="G90" t="s">
+        <v>48</v>
+      </c>
+      <c r="H90" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>50</v>
+      </c>
+      <c r="B91" t="n">
+        <v>465850.0</v>
+      </c>
+      <c r="C91" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" t="s">
+        <v>8</v>
+      </c>
+      <c r="E91" t="s">
+        <v>44</v>
+      </c>
+      <c r="F91" t="s">
+        <v>48</v>
+      </c>
+      <c r="G91"/>
+      <c r="H91"/>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92" t="n">
+        <v>466433.0</v>
+      </c>
+      <c r="C92" t="s">
+        <v>7</v>
+      </c>
+      <c r="D92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" t="s">
+        <v>48</v>
+      </c>
+      <c r="F92" t="s">
+        <v>45</v>
+      </c>
+      <c r="G92" t="s">
+        <v>44</v>
+      </c>
+      <c r="H92"/>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>46</v>
+      </c>
+      <c r="B93" t="n">
+        <v>466579.0</v>
+      </c>
+      <c r="C93" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93" t="s">
+        <v>45</v>
+      </c>
+      <c r="F93" t="s">
+        <v>47</v>
+      </c>
+      <c r="G93" t="s">
+        <v>44</v>
+      </c>
+      <c r="H93" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>49</v>
+      </c>
+      <c r="B94" t="n">
+        <v>466801.0</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94" t="s">
+        <v>8</v>
+      </c>
+      <c r="E94" t="s">
+        <v>47</v>
+      </c>
+      <c r="F94" t="s">
+        <v>48</v>
+      </c>
+      <c r="G94" t="s">
+        <v>44</v>
+      </c>
+      <c r="H94"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>43</v>
+      </c>
+      <c r="B95" t="n">
+        <v>466803.0</v>
+      </c>
+      <c r="C95" t="s">
+        <v>16</v>
+      </c>
+      <c r="D95" t="s">
+        <v>16</v>
+      </c>
+      <c r="E95" t="s">
+        <v>44</v>
+      </c>
+      <c r="F95" t="s">
+        <v>45</v>
+      </c>
+      <c r="G95"/>
+      <c r="H95"/>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>46</v>
+      </c>
+      <c r="B96" t="n">
+        <v>466831.0</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" t="s">
+        <v>8</v>
+      </c>
+      <c r="E96" t="s">
+        <v>47</v>
+      </c>
+      <c r="F96" t="s">
+        <v>45</v>
+      </c>
+      <c r="G96" t="s">
+        <v>48</v>
+      </c>
+      <c r="H96" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>50</v>
+      </c>
+      <c r="B97" t="n">
+        <v>466968.0</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" t="s">
+        <v>8</v>
+      </c>
+      <c r="E97" t="s">
+        <v>48</v>
+      </c>
+      <c r="F97" t="s">
+        <v>44</v>
+      </c>
+      <c r="G97"/>
+      <c r="H97"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>53</v>
+      </c>
+      <c r="B98" t="n">
+        <v>467069.0</v>
+      </c>
+      <c r="C98" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" t="s">
+        <v>8</v>
+      </c>
+      <c r="E98" t="s">
+        <v>45</v>
+      </c>
+      <c r="F98" t="s">
+        <v>47</v>
+      </c>
+      <c r="G98" t="s">
+        <v>44</v>
+      </c>
+      <c r="H98"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>46</v>
+      </c>
+      <c r="B99" t="n">
+        <v>467189.0</v>
+      </c>
+      <c r="C99" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" t="s">
+        <v>8</v>
+      </c>
+      <c r="E99" t="s">
+        <v>45</v>
+      </c>
+      <c r="F99" t="s">
+        <v>47</v>
+      </c>
+      <c r="G99" t="s">
+        <v>44</v>
+      </c>
+      <c r="H99" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>43</v>
+      </c>
+      <c r="B100" t="n">
+        <v>467214.0</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>8</v>
+      </c>
+      <c r="E100" t="s">
+        <v>45</v>
+      </c>
+      <c r="F100" t="s">
+        <v>44</v>
+      </c>
+      <c r="G100"/>
+      <c r="H100"/>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>50</v>
+      </c>
+      <c r="B101" t="n">
+        <v>467243.0</v>
+      </c>
+      <c r="C101" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" t="s">
+        <v>8</v>
+      </c>
+      <c r="E101" t="s">
+        <v>44</v>
+      </c>
+      <c r="F101" t="s">
+        <v>48</v>
+      </c>
+      <c r="G101"/>
+      <c r="H101"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>49</v>
+      </c>
+      <c r="B102" t="n">
+        <v>467436.0</v>
+      </c>
+      <c r="C102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" t="s">
+        <v>44</v>
+      </c>
+      <c r="F102" t="s">
+        <v>47</v>
+      </c>
+      <c r="G102" t="s">
+        <v>48</v>
+      </c>
+      <c r="H102"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>43</v>
+      </c>
+      <c r="B103" t="n">
+        <v>467451.0</v>
+      </c>
+      <c r="C103" t="s">
+        <v>7</v>
+      </c>
+      <c r="D103" t="s">
+        <v>8</v>
+      </c>
+      <c r="E103" t="s">
+        <v>44</v>
+      </c>
+      <c r="F103" t="s">
+        <v>45</v>
+      </c>
+      <c r="G103"/>
+      <c r="H103"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>49</v>
+      </c>
+      <c r="B104" t="n">
+        <v>467455.0</v>
+      </c>
+      <c r="C104" t="s">
+        <v>7</v>
+      </c>
+      <c r="D104" t="s">
+        <v>8</v>
+      </c>
+      <c r="E104" t="s">
+        <v>47</v>
+      </c>
+      <c r="F104" t="s">
+        <v>48</v>
+      </c>
+      <c r="G104" t="s">
+        <v>44</v>
+      </c>
+      <c r="H104"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>46</v>
+      </c>
+      <c r="B105" t="n">
+        <v>467461.0</v>
+      </c>
+      <c r="C105" t="s">
+        <v>7</v>
+      </c>
+      <c r="D105" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" t="s">
+        <v>47</v>
+      </c>
+      <c r="F105" t="s">
+        <v>45</v>
+      </c>
+      <c r="G105" t="s">
+        <v>48</v>
+      </c>
+      <c r="H105" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>46</v>
+      </c>
+      <c r="B106" t="n">
+        <v>467493.0</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" t="s">
+        <v>8</v>
+      </c>
+      <c r="E106" t="s">
+        <v>45</v>
+      </c>
+      <c r="F106" t="s">
+        <v>47</v>
+      </c>
+      <c r="G106" t="s">
+        <v>44</v>
+      </c>
+      <c r="H106" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>51</v>
+      </c>
+      <c r="B107" t="n">
+        <v>467497.0</v>
+      </c>
+      <c r="C107" t="s">
+        <v>7</v>
+      </c>
+      <c r="D107" t="s">
+        <v>8</v>
+      </c>
+      <c r="E107" t="s">
+        <v>44</v>
+      </c>
+      <c r="F107" t="s">
+        <v>47</v>
+      </c>
+      <c r="G107"/>
+      <c r="H107"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>43</v>
+      </c>
+      <c r="B108" t="n">
+        <v>467501.0</v>
+      </c>
+      <c r="C108" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" t="s">
+        <v>8</v>
+      </c>
+      <c r="E108" t="s">
+        <v>45</v>
+      </c>
+      <c r="F108" t="s">
+        <v>44</v>
+      </c>
+      <c r="G108"/>
+      <c r="H108"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>46</v>
+      </c>
+      <c r="B109" t="n">
+        <v>467636.0</v>
+      </c>
+      <c r="C109" t="s">
+        <v>7</v>
+      </c>
+      <c r="D109" t="s">
+        <v>8</v>
+      </c>
+      <c r="E109" t="s">
+        <v>47</v>
+      </c>
+      <c r="F109" t="s">
+        <v>45</v>
+      </c>
+      <c r="G109" t="s">
+        <v>48</v>
+      </c>
+      <c r="H109" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>46</v>
+      </c>
+      <c r="B110" t="n">
+        <v>467744.0</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+      <c r="D110" t="s">
+        <v>8</v>
+      </c>
+      <c r="E110" t="s">
+        <v>45</v>
+      </c>
+      <c r="F110" t="s">
+        <v>47</v>
+      </c>
+      <c r="G110" t="s">
+        <v>44</v>
+      </c>
+      <c r="H110" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>52</v>
+      </c>
+      <c r="B111" t="n">
+        <v>467750.0</v>
+      </c>
+      <c r="C111" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" t="s">
+        <v>48</v>
+      </c>
+      <c r="F111" t="s">
+        <v>45</v>
+      </c>
+      <c r="G111" t="s">
+        <v>44</v>
+      </c>
+      <c r="H111"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>50</v>
+      </c>
+      <c r="B112" t="n">
+        <v>467765.0</v>
+      </c>
+      <c r="C112" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" t="s">
+        <v>48</v>
+      </c>
+      <c r="F112" t="s">
+        <v>44</v>
+      </c>
+      <c r="G112"/>
+      <c r="H112"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>50</v>
+      </c>
+      <c r="B113" t="n">
+        <v>467775.0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" t="s">
+        <v>8</v>
+      </c>
+      <c r="E113" t="s">
+        <v>44</v>
+      </c>
+      <c r="F113" t="s">
+        <v>48</v>
+      </c>
+      <c r="G113"/>
+      <c r="H113"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>50</v>
+      </c>
+      <c r="B114" t="n">
+        <v>467836.0</v>
+      </c>
+      <c r="C114" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114" t="s">
+        <v>8</v>
+      </c>
+      <c r="E114" t="s">
+        <v>48</v>
+      </c>
+      <c r="F114" t="s">
+        <v>44</v>
+      </c>
+      <c r="G114"/>
+      <c r="H114"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>49</v>
+      </c>
+      <c r="B115" t="n">
+        <v>467870.0</v>
+      </c>
+      <c r="C115" t="s">
+        <v>7</v>
+      </c>
+      <c r="D115" t="s">
+        <v>8</v>
+      </c>
+      <c r="E115" t="s">
+        <v>48</v>
+      </c>
+      <c r="F115" t="s">
+        <v>47</v>
+      </c>
+      <c r="G115" t="s">
+        <v>44</v>
+      </c>
+      <c r="H115"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>52</v>
+      </c>
+      <c r="B116" t="n">
+        <v>467873.0</v>
+      </c>
+      <c r="C116" t="s">
+        <v>7</v>
+      </c>
+      <c r="D116" t="s">
+        <v>8</v>
+      </c>
+      <c r="E116" t="s">
+        <v>45</v>
+      </c>
+      <c r="F116" t="s">
+        <v>48</v>
+      </c>
+      <c r="G116" t="s">
+        <v>44</v>
+      </c>
+      <c r="H116"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>52</v>
+      </c>
+      <c r="B117" t="n">
+        <v>467940.0</v>
+      </c>
+      <c r="C117" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" t="s">
+        <v>48</v>
+      </c>
+      <c r="F117" t="s">
+        <v>45</v>
+      </c>
+      <c r="G117" t="s">
+        <v>44</v>
+      </c>
+      <c r="H117"/>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>49</v>
+      </c>
+      <c r="B118" t="n">
+        <v>467947.0</v>
+      </c>
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" t="s">
+        <v>44</v>
+      </c>
+      <c r="F118" t="s">
+        <v>47</v>
+      </c>
+      <c r="G118" t="s">
+        <v>48</v>
+      </c>
+      <c r="H118"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>46</v>
+      </c>
+      <c r="B119" t="n">
+        <v>467963.0</v>
+      </c>
+      <c r="C119" t="s">
+        <v>7</v>
+      </c>
+      <c r="D119" t="s">
+        <v>8</v>
+      </c>
+      <c r="E119" t="s">
+        <v>47</v>
+      </c>
+      <c r="F119" t="s">
+        <v>45</v>
+      </c>
+      <c r="G119" t="s">
+        <v>48</v>
+      </c>
+      <c r="H119" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>46</v>
+      </c>
+      <c r="B120" t="n">
+        <v>467975.0</v>
+      </c>
+      <c r="C120" t="s">
+        <v>7</v>
+      </c>
+      <c r="D120" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" t="s">
+        <v>45</v>
+      </c>
+      <c r="F120" t="s">
+        <v>47</v>
+      </c>
+      <c r="G120" t="s">
+        <v>44</v>
+      </c>
+      <c r="H120" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>46</v>
+      </c>
+      <c r="B121" t="n">
+        <v>467986.0</v>
+      </c>
+      <c r="C121" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="s">
+        <v>47</v>
+      </c>
+      <c r="F121" t="s">
+        <v>45</v>
+      </c>
+      <c r="G121" t="s">
+        <v>48</v>
+      </c>
+      <c r="H121" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>43</v>
+      </c>
+      <c r="B122" t="n">
+        <v>468167.0</v>
+      </c>
+      <c r="C122" t="s">
+        <v>7</v>
+      </c>
+      <c r="D122" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" t="s">
+        <v>44</v>
+      </c>
+      <c r="F122" t="s">
+        <v>45</v>
+      </c>
+      <c r="G122"/>
+      <c r="H122"/>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>51</v>
+      </c>
+      <c r="B123" t="n">
+        <v>468178.0</v>
+      </c>
+      <c r="C123" t="s">
+        <v>7</v>
+      </c>
+      <c r="D123" t="s">
+        <v>8</v>
+      </c>
+      <c r="E123" t="s">
+        <v>47</v>
+      </c>
+      <c r="F123" t="s">
+        <v>44</v>
+      </c>
+      <c r="G123"/>
+      <c r="H123"/>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>46</v>
+      </c>
+      <c r="B124" t="n">
+        <v>468255.0</v>
+      </c>
+      <c r="C124" t="s">
+        <v>7</v>
+      </c>
+      <c r="D124" t="s">
+        <v>8</v>
+      </c>
+      <c r="E124" t="s">
+        <v>45</v>
+      </c>
+      <c r="F124" t="s">
+        <v>47</v>
+      </c>
+      <c r="G124" t="s">
+        <v>44</v>
+      </c>
+      <c r="H124" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>51</v>
+      </c>
+      <c r="B125" t="n">
+        <v>468284.0</v>
+      </c>
+      <c r="C125" t="s">
+        <v>7</v>
+      </c>
+      <c r="D125" t="s">
+        <v>8</v>
+      </c>
+      <c r="E125" t="s">
+        <v>44</v>
+      </c>
+      <c r="F125" t="s">
+        <v>47</v>
+      </c>
+      <c r="G125"/>
+      <c r="H125"/>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>46</v>
+      </c>
+      <c r="B126" t="n">
+        <v>468311.0</v>
+      </c>
+      <c r="C126" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" t="s">
+        <v>8</v>
+      </c>
+      <c r="E126" t="s">
+        <v>47</v>
+      </c>
+      <c r="F126" t="s">
+        <v>45</v>
+      </c>
+      <c r="G126" t="s">
+        <v>48</v>
+      </c>
+      <c r="H126" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>50</v>
+      </c>
+      <c r="B127" t="n">
+        <v>468546.0</v>
+      </c>
+      <c r="C127" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" t="s">
+        <v>8</v>
+      </c>
+      <c r="E127" t="s">
+        <v>44</v>
+      </c>
+      <c r="F127" t="s">
+        <v>48</v>
+      </c>
+      <c r="G127"/>
+      <c r="H127"/>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>43</v>
+      </c>
+      <c r="B128" t="n">
+        <v>468554.0</v>
+      </c>
+      <c r="C128" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" t="s">
+        <v>45</v>
+      </c>
+      <c r="F128" t="s">
+        <v>44</v>
+      </c>
+      <c r="G128"/>
+      <c r="H128"/>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>50</v>
+      </c>
+      <c r="B129" t="n">
+        <v>468607.0</v>
+      </c>
+      <c r="C129" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" t="s">
+        <v>8</v>
+      </c>
+      <c r="E129" t="s">
+        <v>48</v>
+      </c>
+      <c r="F129" t="s">
+        <v>44</v>
+      </c>
+      <c r="G129"/>
+      <c r="H129"/>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>50</v>
+      </c>
+      <c r="B130" t="n">
+        <v>468643.0</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130" t="s">
+        <v>8</v>
+      </c>
+      <c r="E130" t="s">
+        <v>44</v>
+      </c>
+      <c r="F130" t="s">
+        <v>48</v>
+      </c>
+      <c r="G130"/>
+      <c r="H130"/>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>49</v>
+      </c>
+      <c r="B131" t="n">
+        <v>468736.0</v>
+      </c>
+      <c r="C131" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" t="s">
+        <v>8</v>
+      </c>
+      <c r="E131" t="s">
+        <v>47</v>
+      </c>
+      <c r="F131" t="s">
+        <v>48</v>
+      </c>
+      <c r="G131" t="s">
+        <v>44</v>
+      </c>
+      <c r="H131"/>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>43</v>
+      </c>
+      <c r="B132" t="n">
+        <v>468763.0</v>
+      </c>
+      <c r="C132" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132" t="s">
+        <v>8</v>
+      </c>
+      <c r="E132" t="s">
+        <v>44</v>
+      </c>
+      <c r="F132" t="s">
+        <v>45</v>
+      </c>
+      <c r="G132"/>
+      <c r="H132"/>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>51</v>
+      </c>
+      <c r="B133" t="n">
+        <v>468859.0</v>
+      </c>
+      <c r="C133" t="s">
+        <v>7</v>
+      </c>
+      <c r="D133" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" t="s">
+        <v>47</v>
+      </c>
+      <c r="F133" t="s">
+        <v>44</v>
+      </c>
+      <c r="G133"/>
+      <c r="H133"/>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>46</v>
+      </c>
+      <c r="B134" t="n">
+        <v>468876.0</v>
+      </c>
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" t="s">
+        <v>45</v>
+      </c>
+      <c r="F134" t="s">
+        <v>47</v>
+      </c>
+      <c r="G134" t="s">
+        <v>44</v>
+      </c>
+      <c r="H134" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>46</v>
+      </c>
+      <c r="B135" t="n">
+        <v>468882.0</v>
+      </c>
+      <c r="C135" t="s">
+        <v>7</v>
+      </c>
+      <c r="D135" t="s">
+        <v>8</v>
+      </c>
+      <c r="E135" t="s">
+        <v>47</v>
+      </c>
+      <c r="F135" t="s">
+        <v>45</v>
+      </c>
+      <c r="G135" t="s">
+        <v>48</v>
+      </c>
+      <c r="H135" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>43</v>
+      </c>
+      <c r="B136" t="n">
+        <v>468898.0</v>
+      </c>
+      <c r="C136" t="s">
+        <v>7</v>
+      </c>
+      <c r="D136" t="s">
+        <v>8</v>
+      </c>
+      <c r="E136" t="s">
+        <v>45</v>
+      </c>
+      <c r="F136" t="s">
+        <v>44</v>
+      </c>
+      <c r="G136"/>
+      <c r="H136"/>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>43</v>
+      </c>
+      <c r="B137" t="n">
+        <v>468903.0</v>
+      </c>
+      <c r="C137" t="s">
+        <v>7</v>
+      </c>
+      <c r="D137" t="s">
+        <v>8</v>
+      </c>
+      <c r="E137" t="s">
+        <v>44</v>
+      </c>
+      <c r="F137" t="s">
+        <v>45</v>
+      </c>
+      <c r="G137"/>
+      <c r="H137"/>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>49</v>
+      </c>
+      <c r="B138" t="n">
+        <v>468961.0</v>
+      </c>
+      <c r="C138" t="s">
+        <v>7</v>
+      </c>
+      <c r="D138" t="s">
+        <v>8</v>
+      </c>
+      <c r="E138" t="s">
+        <v>48</v>
+      </c>
+      <c r="F138" t="s">
+        <v>47</v>
+      </c>
+      <c r="G138" t="s">
+        <v>44</v>
+      </c>
+      <c r="H138"/>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>51</v>
+      </c>
+      <c r="B139" t="n">
+        <v>469129.0</v>
+      </c>
+      <c r="C139" t="s">
+        <v>7</v>
+      </c>
+      <c r="D139" t="s">
+        <v>8</v>
+      </c>
+      <c r="E139" t="s">
+        <v>44</v>
+      </c>
+      <c r="F139" t="s">
+        <v>47</v>
+      </c>
+      <c r="G139"/>
+      <c r="H139"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>51</v>
+      </c>
+      <c r="B140" t="n">
+        <v>469142.0</v>
+      </c>
+      <c r="C140" t="s">
+        <v>7</v>
+      </c>
+      <c r="D140" t="s">
+        <v>8</v>
+      </c>
+      <c r="E140" t="s">
+        <v>47</v>
+      </c>
+      <c r="F140" t="s">
+        <v>44</v>
+      </c>
+      <c r="G140"/>
+      <c r="H140"/>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>46</v>
+      </c>
+      <c r="B141" t="n">
+        <v>469186.0</v>
+      </c>
+      <c r="C141" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" t="s">
+        <v>8</v>
+      </c>
+      <c r="E141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F141" t="s">
+        <v>47</v>
+      </c>
+      <c r="G141" t="s">
+        <v>44</v>
+      </c>
+      <c r="H141" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>46</v>
+      </c>
+      <c r="B142" t="n">
+        <v>469193.0</v>
+      </c>
+      <c r="C142" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142" t="s">
+        <v>8</v>
+      </c>
+      <c r="E142" t="s">
+        <v>47</v>
+      </c>
+      <c r="F142" t="s">
+        <v>45</v>
+      </c>
+      <c r="G142" t="s">
+        <v>48</v>
+      </c>
+      <c r="H142" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>50</v>
+      </c>
+      <c r="B143" t="n">
+        <v>469213.0</v>
+      </c>
+      <c r="C143" t="s">
+        <v>7</v>
+      </c>
+      <c r="D143" t="s">
+        <v>8</v>
+      </c>
+      <c r="E143" t="s">
+        <v>48</v>
+      </c>
+      <c r="F143" t="s">
+        <v>44</v>
+      </c>
+      <c r="G143"/>
+      <c r="H143"/>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>46</v>
+      </c>
+      <c r="B144" t="n">
+        <v>469288.0</v>
+      </c>
+      <c r="C144" t="s">
+        <v>7</v>
+      </c>
+      <c r="D144" t="s">
+        <v>8</v>
+      </c>
+      <c r="E144" t="s">
+        <v>45</v>
+      </c>
+      <c r="F144" t="s">
+        <v>47</v>
+      </c>
+      <c r="G144" t="s">
+        <v>44</v>
+      </c>
+      <c r="H144" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>52</v>
+      </c>
+      <c r="B145" t="n">
+        <v>469327.0</v>
+      </c>
+      <c r="C145" t="s">
+        <v>7</v>
+      </c>
+      <c r="D145" t="s">
+        <v>8</v>
+      </c>
+      <c r="E145" t="s">
+        <v>45</v>
+      </c>
+      <c r="F145" t="s">
+        <v>48</v>
+      </c>
+      <c r="G145" t="s">
+        <v>44</v>
+      </c>
+      <c r="H145"/>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>43</v>
+      </c>
+      <c r="B146" t="n">
+        <v>469351.0</v>
+      </c>
+      <c r="C146" t="s">
+        <v>7</v>
+      </c>
+      <c r="D146" t="s">
+        <v>8</v>
+      </c>
+      <c r="E146" t="s">
+        <v>45</v>
+      </c>
+      <c r="F146" t="s">
+        <v>44</v>
+      </c>
+      <c r="G146"/>
+      <c r="H146"/>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>53</v>
+      </c>
+      <c r="B147" t="n">
+        <v>469358.0</v>
+      </c>
+      <c r="C147" t="s">
+        <v>7</v>
+      </c>
+      <c r="D147" t="s">
+        <v>8</v>
+      </c>
+      <c r="E147" t="s">
+        <v>44</v>
+      </c>
+      <c r="F147" t="s">
+        <v>45</v>
+      </c>
+      <c r="G147" t="s">
+        <v>47</v>
+      </c>
+      <c r="H147"/>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>46</v>
+      </c>
+      <c r="B148" t="n">
+        <v>469474.0</v>
+      </c>
+      <c r="C148" t="s">
+        <v>7</v>
+      </c>
+      <c r="D148" t="s">
+        <v>8</v>
+      </c>
+      <c r="E148" t="s">
+        <v>47</v>
+      </c>
+      <c r="F148" t="s">
+        <v>45</v>
+      </c>
+      <c r="G148" t="s">
+        <v>48</v>
+      </c>
+      <c r="H148" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>50</v>
+      </c>
+      <c r="B149" t="n">
+        <v>469486.0</v>
+      </c>
+      <c r="C149" t="s">
+        <v>7</v>
+      </c>
+      <c r="D149" t="s">
+        <v>8</v>
+      </c>
+      <c r="E149" t="s">
+        <v>44</v>
+      </c>
+      <c r="F149" t="s">
+        <v>48</v>
+      </c>
+      <c r="G149"/>
+      <c r="H149"/>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>46</v>
+      </c>
+      <c r="B150" t="n">
+        <v>469625.0</v>
+      </c>
+      <c r="C150" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" t="s">
+        <v>8</v>
+      </c>
+      <c r="E150" t="s">
+        <v>45</v>
+      </c>
+      <c r="F150" t="s">
+        <v>47</v>
+      </c>
+      <c r="G150" t="s">
+        <v>44</v>
+      </c>
+      <c r="H150" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>46</v>
+      </c>
+      <c r="B151" t="n">
+        <v>469740.0</v>
+      </c>
+      <c r="C151" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151" t="s">
+        <v>8</v>
+      </c>
+      <c r="E151" t="s">
+        <v>47</v>
+      </c>
+      <c r="F151" t="s">
+        <v>45</v>
+      </c>
+      <c r="G151" t="s">
+        <v>48</v>
+      </c>
+      <c r="H151" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>43</v>
+      </c>
+      <c r="B152" t="n">
+        <v>469823.0</v>
+      </c>
+      <c r="C152" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" t="s">
+        <v>8</v>
+      </c>
+      <c r="E152" t="s">
+        <v>44</v>
+      </c>
+      <c r="F152" t="s">
+        <v>45</v>
+      </c>
+      <c r="G152"/>
+      <c r="H152"/>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>49</v>
+      </c>
+      <c r="B153" t="n">
+        <v>469857.0</v>
+      </c>
+      <c r="C153" t="s">
+        <v>7</v>
+      </c>
+      <c r="D153" t="s">
+        <v>8</v>
+      </c>
+      <c r="E153" t="s">
+        <v>44</v>
+      </c>
+      <c r="F153" t="s">
+        <v>48</v>
+      </c>
+      <c r="G153" t="s">
+        <v>47</v>
+      </c>
+      <c r="H153"/>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>46</v>
+      </c>
+      <c r="B154" t="n">
+        <v>469975.0</v>
+      </c>
+      <c r="C154" t="s">
+        <v>7</v>
+      </c>
+      <c r="D154" t="s">
+        <v>8</v>
+      </c>
+      <c r="E154" t="s">
+        <v>45</v>
+      </c>
+      <c r="F154" t="s">
+        <v>47</v>
+      </c>
+      <c r="G154" t="s">
+        <v>44</v>
+      </c>
+      <c r="H154" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>50</v>
+      </c>
+      <c r="B155" t="n">
+        <v>470129.0</v>
+      </c>
+      <c r="C155" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155" t="s">
+        <v>8</v>
+      </c>
+      <c r="E155" t="s">
+        <v>48</v>
+      </c>
+      <c r="F155" t="s">
+        <v>44</v>
+      </c>
+      <c r="G155"/>
+      <c r="H155"/>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>51</v>
+      </c>
+      <c r="B156" t="n">
+        <v>470144.0</v>
+      </c>
+      <c r="C156" t="s">
+        <v>7</v>
+      </c>
+      <c r="D156" t="s">
+        <v>8</v>
+      </c>
+      <c r="E156" t="s">
+        <v>44</v>
+      </c>
+      <c r="F156" t="s">
+        <v>47</v>
+      </c>
+      <c r="G156"/>
+      <c r="H156"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>46</v>
+      </c>
+      <c r="B157" t="n">
+        <v>470282.0</v>
+      </c>
+      <c r="C157" t="s">
+        <v>7</v>
+      </c>
+      <c r="D157" t="s">
+        <v>8</v>
+      </c>
+      <c r="E157" t="s">
+        <v>47</v>
+      </c>
+      <c r="F157" t="s">
+        <v>45</v>
+      </c>
+      <c r="G157" t="s">
+        <v>48</v>
+      </c>
+      <c r="H157" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>51</v>
+      </c>
+      <c r="B158" t="n">
+        <v>470290.0</v>
+      </c>
+      <c r="C158" t="s">
+        <v>7</v>
+      </c>
+      <c r="D158" t="s">
+        <v>8</v>
+      </c>
+      <c r="E158" t="s">
+        <v>47</v>
+      </c>
+      <c r="F158" t="s">
+        <v>44</v>
+      </c>
+      <c r="G158"/>
+      <c r="H158"/>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>43</v>
+      </c>
+      <c r="B159" t="n">
+        <v>470309.0</v>
+      </c>
+      <c r="C159" t="s">
+        <v>7</v>
+      </c>
+      <c r="D159" t="s">
+        <v>8</v>
+      </c>
+      <c r="E159" t="s">
+        <v>45</v>
+      </c>
+      <c r="F159" t="s">
+        <v>44</v>
+      </c>
+      <c r="G159"/>
+      <c r="H159"/>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>49</v>
+      </c>
+      <c r="B160" t="n">
+        <v>470373.0</v>
+      </c>
+      <c r="C160" t="s">
+        <v>7</v>
+      </c>
+      <c r="D160" t="s">
+        <v>8</v>
+      </c>
+      <c r="E160" t="s">
+        <v>48</v>
+      </c>
+      <c r="F160" t="s">
+        <v>47</v>
+      </c>
+      <c r="G160" t="s">
+        <v>44</v>
+      </c>
+      <c r="H160"/>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>51</v>
+      </c>
+      <c r="B161" t="n">
+        <v>470405.0</v>
+      </c>
+      <c r="C161" t="s">
+        <v>7</v>
+      </c>
+      <c r="D161" t="s">
+        <v>8</v>
+      </c>
+      <c r="E161" t="s">
+        <v>44</v>
+      </c>
+      <c r="F161" t="s">
+        <v>47</v>
+      </c>
+      <c r="G161"/>
+      <c r="H161"/>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>49</v>
+      </c>
+      <c r="B162" t="n">
+        <v>470467.0</v>
+      </c>
+      <c r="C162" t="s">
+        <v>7</v>
+      </c>
+      <c r="D162" t="s">
+        <v>8</v>
+      </c>
+      <c r="E162" t="s">
+        <v>47</v>
+      </c>
+      <c r="F162" t="s">
+        <v>48</v>
+      </c>
+      <c r="G162" t="s">
+        <v>44</v>
+      </c>
+      <c r="H162"/>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>49</v>
+      </c>
+      <c r="B163" t="n">
+        <v>470488.0</v>
+      </c>
+      <c r="C163" t="s">
+        <v>7</v>
+      </c>
+      <c r="D163" t="s">
+        <v>8</v>
+      </c>
+      <c r="E163" t="s">
+        <v>44</v>
+      </c>
+      <c r="F163" t="s">
+        <v>47</v>
+      </c>
+      <c r="G163" t="s">
+        <v>48</v>
+      </c>
+      <c r="H163"/>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>50</v>
+      </c>
+      <c r="B164" t="n">
+        <v>470638.0</v>
+      </c>
+      <c r="C164" t="s">
+        <v>7</v>
+      </c>
+      <c r="D164" t="s">
+        <v>8</v>
+      </c>
+      <c r="E164" t="s">
+        <v>44</v>
+      </c>
+      <c r="F164" t="s">
+        <v>48</v>
+      </c>
+      <c r="G164"/>
+      <c r="H164"/>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>43</v>
+      </c>
+      <c r="B165" t="n">
+        <v>470668.0</v>
+      </c>
+      <c r="C165" t="s">
+        <v>7</v>
+      </c>
+      <c r="D165" t="s">
+        <v>8</v>
+      </c>
+      <c r="E165" t="s">
+        <v>44</v>
+      </c>
+      <c r="F165" t="s">
+        <v>45</v>
+      </c>
+      <c r="G165"/>
+      <c r="H165"/>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>49</v>
+      </c>
+      <c r="B166" t="n">
+        <v>470754.0</v>
+      </c>
+      <c r="C166" t="s">
+        <v>7</v>
+      </c>
+      <c r="D166" t="s">
+        <v>8</v>
+      </c>
+      <c r="E166" t="s">
+        <v>48</v>
+      </c>
+      <c r="F166" t="s">
+        <v>44</v>
+      </c>
+      <c r="G166" t="s">
+        <v>47</v>
+      </c>
+      <c r="H166"/>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>46</v>
+      </c>
+      <c r="B167" t="n">
+        <v>470773.0</v>
+      </c>
+      <c r="C167" t="s">
+        <v>7</v>
+      </c>
+      <c r="D167" t="s">
+        <v>8</v>
+      </c>
+      <c r="E167" t="s">
+        <v>45</v>
+      </c>
+      <c r="F167" t="s">
+        <v>47</v>
+      </c>
+      <c r="G167" t="s">
+        <v>44</v>
+      </c>
+      <c r="H167" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>46</v>
+      </c>
+      <c r="B168" t="n">
+        <v>470782.0</v>
+      </c>
+      <c r="C168" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" t="s">
+        <v>8</v>
+      </c>
+      <c r="E168" t="s">
+        <v>47</v>
+      </c>
+      <c r="F168" t="s">
+        <v>45</v>
+      </c>
+      <c r="G168" t="s">
+        <v>48</v>
+      </c>
+      <c r="H168" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>51</v>
+      </c>
+      <c r="B169" t="n">
+        <v>470830.0</v>
+      </c>
+      <c r="C169" t="s">
+        <v>7</v>
+      </c>
+      <c r="D169" t="s">
+        <v>8</v>
+      </c>
+      <c r="E169" t="s">
+        <v>47</v>
+      </c>
+      <c r="F169" t="s">
+        <v>44</v>
+      </c>
+      <c r="G169"/>
+      <c r="H169"/>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>49</v>
+      </c>
+      <c r="B170" t="n">
+        <v>470859.0</v>
+      </c>
+      <c r="C170" t="s">
+        <v>7</v>
+      </c>
+      <c r="D170" t="s">
+        <v>8</v>
+      </c>
+      <c r="E170" t="s">
+        <v>47</v>
+      </c>
+      <c r="F170" t="s">
+        <v>48</v>
+      </c>
+      <c r="G170" t="s">
+        <v>44</v>
+      </c>
+      <c r="H170"/>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>50</v>
+      </c>
+      <c r="B171" t="n">
+        <v>470921.0</v>
+      </c>
+      <c r="C171" t="s">
+        <v>7</v>
+      </c>
+      <c r="D171" t="s">
+        <v>8</v>
+      </c>
+      <c r="E171" t="s">
+        <v>48</v>
+      </c>
+      <c r="F171" t="s">
+        <v>44</v>
+      </c>
+      <c r="G171"/>
+      <c r="H171"/>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>50</v>
+      </c>
+      <c r="B172" t="n">
+        <v>471016.0</v>
+      </c>
+      <c r="C172" t="s">
+        <v>7</v>
+      </c>
+      <c r="D172" t="s">
+        <v>8</v>
+      </c>
+      <c r="E172" t="s">
+        <v>44</v>
+      </c>
+      <c r="F172" t="s">
+        <v>48</v>
+      </c>
+      <c r="G172"/>
+      <c r="H172"/>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>46</v>
+      </c>
+      <c r="B173" t="n">
+        <v>471028.0</v>
+      </c>
+      <c r="C173" t="s">
+        <v>7</v>
+      </c>
+      <c r="D173" t="s">
+        <v>8</v>
+      </c>
+      <c r="E173" t="s">
+        <v>45</v>
+      </c>
+      <c r="F173" t="s">
+        <v>47</v>
+      </c>
+      <c r="G173" t="s">
+        <v>44</v>
+      </c>
+      <c r="H173" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>51</v>
+      </c>
+      <c r="B174" t="n">
+        <v>471129.0</v>
+      </c>
+      <c r="C174" t="s">
+        <v>7</v>
+      </c>
+      <c r="D174" t="s">
+        <v>8</v>
+      </c>
+      <c r="E174" t="s">
+        <v>44</v>
+      </c>
+      <c r="F174" t="s">
+        <v>47</v>
+      </c>
+      <c r="G174"/>
+      <c r="H174"/>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>50</v>
+      </c>
+      <c r="B175" t="n">
+        <v>471229.0</v>
+      </c>
+      <c r="C175" t="s">
+        <v>7</v>
+      </c>
+      <c r="D175" t="s">
+        <v>8</v>
+      </c>
+      <c r="E175" t="s">
+        <v>48</v>
+      </c>
+      <c r="F175" t="s">
+        <v>44</v>
+      </c>
+      <c r="G175"/>
+      <c r="H175"/>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>50</v>
+      </c>
+      <c r="B176" t="n">
+        <v>471255.0</v>
+      </c>
+      <c r="C176" t="s">
+        <v>7</v>
+      </c>
+      <c r="D176" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" t="s">
+        <v>44</v>
+      </c>
+      <c r="F176" t="s">
+        <v>48</v>
+      </c>
+      <c r="G176"/>
+      <c r="H176"/>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>49</v>
+      </c>
+      <c r="B177" t="n">
+        <v>471263.0</v>
+      </c>
+      <c r="C177" t="s">
+        <v>7</v>
+      </c>
+      <c r="D177" t="s">
+        <v>8</v>
+      </c>
+      <c r="E177" t="s">
+        <v>44</v>
+      </c>
+      <c r="F177" t="s">
+        <v>47</v>
+      </c>
+      <c r="G177" t="s">
+        <v>48</v>
+      </c>
+      <c r="H177"/>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>50</v>
+      </c>
+      <c r="B178" t="n">
+        <v>471492.0</v>
+      </c>
+      <c r="C178" t="s">
+        <v>7</v>
+      </c>
+      <c r="D178" t="s">
+        <v>8</v>
+      </c>
+      <c r="E178" t="s">
+        <v>48</v>
+      </c>
+      <c r="F178" t="s">
+        <v>44</v>
+      </c>
+      <c r="G178"/>
+      <c r="H178"/>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>49</v>
+      </c>
+      <c r="B179" t="n">
+        <v>471545.0</v>
+      </c>
+      <c r="C179" t="s">
+        <v>7</v>
+      </c>
+      <c r="D179" t="s">
+        <v>8</v>
+      </c>
+      <c r="E179" t="s">
+        <v>48</v>
+      </c>
+      <c r="F179" t="s">
+        <v>44</v>
+      </c>
+      <c r="G179" t="s">
+        <v>47</v>
+      </c>
+      <c r="H179"/>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>50</v>
+      </c>
+      <c r="B180" t="n">
+        <v>471760.0</v>
+      </c>
+      <c r="C180" t="s">
+        <v>7</v>
+      </c>
+      <c r="D180" t="s">
+        <v>8</v>
+      </c>
+      <c r="E180" t="s">
+        <v>44</v>
+      </c>
+      <c r="F180" t="s">
+        <v>48</v>
+      </c>
+      <c r="G180"/>
+      <c r="H180"/>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>43</v>
+      </c>
+      <c r="B181" t="n">
+        <v>472004.0</v>
+      </c>
+      <c r="C181" t="s">
+        <v>7</v>
+      </c>
+      <c r="D181" t="s">
+        <v>8</v>
+      </c>
+      <c r="E181" t="s">
+        <v>45</v>
+      </c>
+      <c r="F181" t="s">
+        <v>44</v>
+      </c>
+      <c r="G181"/>
+      <c r="H181"/>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>52</v>
+      </c>
+      <c r="B182" t="n">
+        <v>472145.0</v>
+      </c>
+      <c r="C182" t="s">
+        <v>7</v>
+      </c>
+      <c r="D182" t="s">
+        <v>8</v>
+      </c>
+      <c r="E182" t="s">
+        <v>48</v>
+      </c>
+      <c r="F182" t="s">
+        <v>45</v>
+      </c>
+      <c r="G182" t="s">
+        <v>44</v>
+      </c>
+      <c r="H182"/>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>43</v>
+      </c>
+      <c r="B183" t="n">
+        <v>472434.0</v>
+      </c>
+      <c r="C183" t="s">
+        <v>7</v>
+      </c>
+      <c r="D183" t="s">
+        <v>8</v>
+      </c>
+      <c r="E183" t="s">
+        <v>44</v>
+      </c>
+      <c r="F183" t="s">
+        <v>45</v>
+      </c>
+      <c r="G183"/>
+      <c r="H183"/>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>46</v>
+      </c>
+      <c r="B184" t="n">
+        <v>472501.0</v>
+      </c>
+      <c r="C184" t="s">
+        <v>7</v>
+      </c>
+      <c r="D184" t="s">
+        <v>8</v>
+      </c>
+      <c r="E184" t="s">
+        <v>47</v>
+      </c>
+      <c r="F184" t="s">
+        <v>45</v>
+      </c>
+      <c r="G184" t="s">
+        <v>48</v>
+      </c>
+      <c r="H184" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>51</v>
+      </c>
+      <c r="B185" t="n">
+        <v>472537.0</v>
+      </c>
+      <c r="C185" t="s">
+        <v>7</v>
+      </c>
+      <c r="D185" t="s">
+        <v>8</v>
+      </c>
+      <c r="E185" t="s">
+        <v>47</v>
+      </c>
+      <c r="F185" t="s">
+        <v>44</v>
+      </c>
+      <c r="G185"/>
+      <c r="H185"/>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>49</v>
+      </c>
+      <c r="B186" t="n">
+        <v>472782.0</v>
+      </c>
+      <c r="C186" t="s">
+        <v>7</v>
+      </c>
+      <c r="D186" t="s">
+        <v>8</v>
+      </c>
+      <c r="E186" t="s">
+        <v>47</v>
+      </c>
+      <c r="F186" t="s">
+        <v>48</v>
+      </c>
+      <c r="G186" t="s">
+        <v>44</v>
+      </c>
+      <c r="H186"/>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>50</v>
+      </c>
+      <c r="B187" t="n">
+        <v>472962.0</v>
+      </c>
+      <c r="C187" t="s">
+        <v>7</v>
+      </c>
+      <c r="D187" t="s">
+        <v>8</v>
+      </c>
+      <c r="E187" t="s">
+        <v>48</v>
+      </c>
+      <c r="F187" t="s">
+        <v>44</v>
+      </c>
+      <c r="G187"/>
+      <c r="H187"/>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>52</v>
+      </c>
+      <c r="B188" t="n">
+        <v>473195.0</v>
+      </c>
+      <c r="C188" t="s">
+        <v>7</v>
+      </c>
+      <c r="D188" t="s">
+        <v>8</v>
+      </c>
+      <c r="E188" t="s">
+        <v>45</v>
+      </c>
+      <c r="F188" t="s">
+        <v>48</v>
+      </c>
+      <c r="G188" t="s">
+        <v>44</v>
+      </c>
+      <c r="H188"/>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>49</v>
+      </c>
+      <c r="B189" t="n">
+        <v>473215.0</v>
+      </c>
+      <c r="C189" t="s">
+        <v>7</v>
+      </c>
+      <c r="D189" t="s">
+        <v>8</v>
+      </c>
+      <c r="E189" t="s">
+        <v>44</v>
+      </c>
+      <c r="F189" t="s">
+        <v>47</v>
+      </c>
+      <c r="G189" t="s">
+        <v>48</v>
+      </c>
+      <c r="H189"/>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>50</v>
+      </c>
+      <c r="B190" t="n">
+        <v>473482.0</v>
+      </c>
+      <c r="C190" t="s">
+        <v>7</v>
+      </c>
+      <c r="D190" t="s">
+        <v>8</v>
+      </c>
+      <c r="E190" t="s">
+        <v>44</v>
+      </c>
+      <c r="F190" t="s">
+        <v>48</v>
+      </c>
+      <c r="G190"/>
+      <c r="H190"/>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>49</v>
+      </c>
+      <c r="B191" t="n">
+        <v>473708.0</v>
+      </c>
+      <c r="C191" t="s">
+        <v>7</v>
+      </c>
+      <c r="D191" t="s">
+        <v>8</v>
+      </c>
+      <c r="E191" t="s">
+        <v>48</v>
+      </c>
+      <c r="F191" t="s">
+        <v>44</v>
+      </c>
+      <c r="G191" t="s">
+        <v>47</v>
+      </c>
+      <c r="H191"/>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>50</v>
+      </c>
+      <c r="B192" t="n">
+        <v>473899.0</v>
+      </c>
+      <c r="C192" t="s">
+        <v>7</v>
+      </c>
+      <c r="D192" t="s">
+        <v>8</v>
+      </c>
+      <c r="E192" t="s">
+        <v>48</v>
+      </c>
+      <c r="F192" t="s">
+        <v>44</v>
+      </c>
+      <c r="G192"/>
+      <c r="H192"/>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>51</v>
+      </c>
+      <c r="B193" t="n">
+        <v>475115.0</v>
+      </c>
+      <c r="C193" t="s">
+        <v>7</v>
+      </c>
+      <c r="D193" t="s">
+        <v>8</v>
+      </c>
+      <c r="E193" t="s">
+        <v>44</v>
+      </c>
+      <c r="F193" t="s">
+        <v>47</v>
+      </c>
+      <c r="G193"/>
+      <c r="H193"/>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>50</v>
+      </c>
+      <c r="B194" t="n">
+        <v>476008.0</v>
+      </c>
+      <c r="C194" t="s">
+        <v>7</v>
+      </c>
+      <c r="D194" t="s">
+        <v>8</v>
+      </c>
+      <c r="E194" t="s">
+        <v>44</v>
+      </c>
+      <c r="F194" t="s">
+        <v>48</v>
+      </c>
+      <c r="G194"/>
+      <c r="H194"/>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>50</v>
+      </c>
+      <c r="B195" t="n">
+        <v>476289.0</v>
+      </c>
+      <c r="C195" t="s">
+        <v>7</v>
+      </c>
+      <c r="D195" t="s">
+        <v>8</v>
+      </c>
+      <c r="E195" t="s">
+        <v>48</v>
+      </c>
+      <c r="F195" t="s">
+        <v>44</v>
+      </c>
+      <c r="G195"/>
+      <c r="H195"/>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>43</v>
+      </c>
+      <c r="B196" t="n">
+        <v>476531.0</v>
+      </c>
+      <c r="C196" t="s">
+        <v>7</v>
+      </c>
+      <c r="D196" t="s">
+        <v>8</v>
+      </c>
+      <c r="E196" t="s">
+        <v>45</v>
+      </c>
+      <c r="F196" t="s">
+        <v>44</v>
+      </c>
+      <c r="G196"/>
+      <c r="H196"/>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>52</v>
+      </c>
+      <c r="B197" t="n">
+        <v>476883.0</v>
+      </c>
+      <c r="C197" t="s">
+        <v>7</v>
+      </c>
+      <c r="D197" t="s">
+        <v>8</v>
+      </c>
+      <c r="E197" t="s">
+        <v>45</v>
+      </c>
+      <c r="F197" t="s">
+        <v>48</v>
+      </c>
+      <c r="G197" t="s">
+        <v>44</v>
+      </c>
+      <c r="H197"/>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>50</v>
+      </c>
+      <c r="B198" t="n">
+        <v>477153.0</v>
+      </c>
+      <c r="C198" t="s">
+        <v>7</v>
+      </c>
+      <c r="D198" t="s">
+        <v>8</v>
+      </c>
+      <c r="E198" t="s">
+        <v>44</v>
+      </c>
+      <c r="F198" t="s">
+        <v>48</v>
+      </c>
+      <c r="G198"/>
+      <c r="H198"/>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>50</v>
+      </c>
+      <c r="B199" t="n">
+        <v>477738.0</v>
+      </c>
+      <c r="C199" t="s">
+        <v>7</v>
+      </c>
+      <c r="D199" t="s">
+        <v>8</v>
+      </c>
+      <c r="E199" t="s">
+        <v>48</v>
+      </c>
+      <c r="F199" t="s">
+        <v>44</v>
+      </c>
+      <c r="G199"/>
+      <c r="H199"/>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>46</v>
+      </c>
+      <c r="B200" t="n">
+        <v>478406.0</v>
+      </c>
+      <c r="C200" t="s">
+        <v>7</v>
+      </c>
+      <c r="D200" t="s">
+        <v>8</v>
+      </c>
+      <c r="E200" t="s">
+        <v>45</v>
+      </c>
+      <c r="F200" t="s">
+        <v>47</v>
+      </c>
+      <c r="G200" t="s">
+        <v>44</v>
+      </c>
+      <c r="H200" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="s">
+        <v>51</v>
+      </c>
+      <c r="B201" t="n">
+        <v>478589.0</v>
+      </c>
+      <c r="C201" t="s">
+        <v>7</v>
+      </c>
+      <c r="D201" t="s">
+        <v>8</v>
+      </c>
+      <c r="E201" t="s">
+        <v>47</v>
+      </c>
+      <c r="F201" t="s">
+        <v>44</v>
+      </c>
+      <c r="G201"/>
+      <c r="H201"/>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>46</v>
+      </c>
+      <c r="B202" t="n">
+        <v>479276.0</v>
+      </c>
+      <c r="C202" t="s">
+        <v>7</v>
+      </c>
+      <c r="D202" t="s">
+        <v>8</v>
+      </c>
+      <c r="E202" t="s">
+        <v>47</v>
+      </c>
+      <c r="F202" t="s">
+        <v>45</v>
+      </c>
+      <c r="G202" t="s">
+        <v>48</v>
+      </c>
+      <c r="H202" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>51</v>
+      </c>
+      <c r="B203" t="n">
+        <v>479658.0</v>
+      </c>
+      <c r="C203" t="s">
+        <v>7</v>
+      </c>
+      <c r="D203" t="s">
+        <v>8</v>
+      </c>
+      <c r="E203" t="s">
+        <v>44</v>
+      </c>
+      <c r="F203" t="s">
+        <v>47</v>
+      </c>
+      <c r="G203"/>
+      <c r="H203"/>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>46</v>
+      </c>
+      <c r="B204" t="n">
+        <v>532682.0</v>
+      </c>
+      <c r="C204" t="s">
+        <v>11</v>
+      </c>
+      <c r="D204" t="s">
+        <v>33</v>
+      </c>
+      <c r="E204" t="s">
+        <v>45</v>
+      </c>
+      <c r="F204" t="s">
+        <v>47</v>
+      </c>
+      <c r="G204" t="s">
+        <v>44</v>
+      </c>
+      <c r="H204" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>49</v>
+      </c>
+      <c r="B205" t="n">
+        <v>987654.0</v>
+      </c>
+      <c r="C205" t="s">
+        <v>7</v>
+      </c>
+      <c r="D205" t="s">
+        <v>8</v>
+      </c>
+      <c r="E205" t="s">
+        <v>47</v>
+      </c>
+      <c r="F205" t="s">
+        <v>48</v>
+      </c>
+      <c r="G205" t="s">
+        <v>44</v>
+      </c>
+      <c r="H205"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Backup Process to StudentData
</commit_message>
<xml_diff>
--- a/data/StudentData.xlsx
+++ b/data/StudentData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27229" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27235" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -188,6 +188,12 @@
   </si>
   <si>
     <t>2 Rotations: Humanities, SMCS</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>efa</t>
   </si>
 </sst>
 </file>
@@ -524,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G205"/>
+  <dimension ref="A1:G206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
@@ -1685,18 +1691,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>353515</v>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>351353.0</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D51" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E51" t="s">
         <v>9</v>
@@ -1705,58 +1711,58 @@
         <v>10</v>
       </c>
       <c r="G51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
+        <v>353515</v>
+      </c>
+      <c r="B52" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
         <v>353621</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>35</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>36</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D53" t="s">
         <v>37</v>
       </c>
-      <c r="E52" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
-        <v>406490</v>
-      </c>
-      <c r="B53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G53" s="2" t="s">
+      <c r="E53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>409089</v>
+        <v>406490</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -1768,7 +1774,7 @@
         <v>7</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>9</v>
@@ -1779,22 +1785,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>411168</v>
+        <v>409089</v>
       </c>
       <c r="B55" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>10</v>
@@ -1802,22 +1808,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>417688</v>
+        <v>411168</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>10</v>
@@ -1825,7 +1831,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>419371</v>
+        <v>417688</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -1836,19 +1842,19 @@
       <c r="D57" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>10</v>
+      <c r="E57" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>419659</v>
+        <v>419371</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
@@ -1871,7 +1877,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>420119</v>
+        <v>419659</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
@@ -1883,7 +1889,7 @@
         <v>7</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>9</v>
@@ -1894,7 +1900,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>436542</v>
+        <v>420119</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
@@ -1906,18 +1912,18 @@
         <v>7</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>439155</v>
+        <v>436542</v>
       </c>
       <c r="B61" t="s">
         <v>7</v>
@@ -1940,7 +1946,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>441021</v>
+        <v>439155</v>
       </c>
       <c r="B62" t="s">
         <v>7</v>
@@ -1963,7 +1969,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>442262</v>
+        <v>441021</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
@@ -1978,15 +1984,15 @@
         <v>10</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>442931</v>
+        <v>442262</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -1997,11 +2003,11 @@
       <c r="D64" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>9</v>
+      <c r="E64" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>9</v>
@@ -2009,7 +2015,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>443257</v>
+        <v>442931</v>
       </c>
       <c r="B65" t="s">
         <v>7</v>
@@ -2027,12 +2033,12 @@
         <v>9</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>446253</v>
+        <v>443257</v>
       </c>
       <c r="B66" t="s">
         <v>7</v>
@@ -2043,7 +2049,7 @@
       <c r="D66" t="s">
         <v>7</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F66" s="2" t="s">
@@ -2055,7 +2061,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>448013</v>
+        <v>446253</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
@@ -2067,18 +2073,18 @@
         <v>7</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>452390</v>
+        <v>448013</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
@@ -2090,9 +2096,9 @@
         <v>7</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G68" s="3" t="s">
@@ -2101,7 +2107,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>452992</v>
+        <v>452390</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
@@ -2113,7 +2119,7 @@
         <v>7</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>9</v>
@@ -2124,7 +2130,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>454280</v>
+        <v>452992</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
@@ -2147,7 +2153,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>454287</v>
+        <v>454280</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
@@ -2161,16 +2167,16 @@
       <c r="E71" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>10</v>
+      <c r="F71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>454745</v>
+        <v>454287</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
@@ -2181,19 +2187,19 @@
       <c r="D72" t="s">
         <v>7</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>9</v>
+      <c r="E72" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>454770</v>
+        <v>454745</v>
       </c>
       <c r="B73" t="s">
         <v>7</v>
@@ -2204,19 +2210,19 @@
       <c r="D73" t="s">
         <v>7</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G73" s="2" t="s">
-        <v>10</v>
+      <c r="G73" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>455839</v>
+        <v>454770</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
@@ -2228,18 +2234,18 @@
         <v>7</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>461540</v>
+        <v>455839</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
@@ -2256,82 +2262,82 @@
       <c r="F75" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G75" s="3" t="s">
+      <c r="G75" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
+        <v>461540</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>462838</v>
       </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s">
-        <v>8</v>
-      </c>
-      <c r="D76" t="s">
-        <v>7</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>7</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>463462</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B78" t="s">
         <v>27</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>28</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>29</v>
       </c>
-      <c r="E77" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" t="s">
-        <v>9</v>
-      </c>
-      <c r="G77" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
-        <v>463934</v>
-      </c>
-      <c r="B78" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" t="s">
-        <v>7</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G78" s="2" t="s">
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>464863</v>
+        <v>463934</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
@@ -2342,19 +2348,19 @@
       <c r="D79" t="s">
         <v>7</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="E79" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G79" s="3" t="s">
+      <c r="G79" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>465018</v>
+        <v>464863</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
@@ -2366,9 +2372,9 @@
         <v>7</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G80" s="3" t="s">
@@ -2377,7 +2383,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>465085</v>
+        <v>465018</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -2391,8 +2397,8 @@
       <c r="E81" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>10</v>
+      <c r="F81" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G81" s="3" t="s">
         <v>9</v>
@@ -2400,7 +2406,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>465090</v>
+        <v>465085</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
@@ -2415,7 +2421,7 @@
         <v>10</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>9</v>
@@ -2423,7 +2429,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>465141</v>
+        <v>465090</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
@@ -2440,13 +2446,13 @@
       <c r="F83" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="G83" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>465275</v>
+        <v>465141</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
@@ -2458,7 +2464,7 @@
         <v>7</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>9</v>
@@ -2469,7 +2475,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>465391</v>
+        <v>465275</v>
       </c>
       <c r="B85" t="s">
         <v>7</v>
@@ -2487,12 +2493,12 @@
         <v>9</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>465431</v>
+        <v>465391</v>
       </c>
       <c r="B86" t="s">
         <v>7</v>
@@ -2503,19 +2509,19 @@
       <c r="D86" t="s">
         <v>7</v>
       </c>
-      <c r="E86" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F86" s="3" t="s">
+      <c r="E86" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>465484</v>
+        <v>465431</v>
       </c>
       <c r="B87" t="s">
         <v>7</v>
@@ -2526,19 +2532,19 @@
       <c r="D87" t="s">
         <v>7</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F87" s="2" t="s">
+      <c r="E87" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>465644</v>
+        <v>465484</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
@@ -2555,13 +2561,13 @@
       <c r="F88" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G88" s="3" t="s">
-        <v>9</v>
+      <c r="G88" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>465653</v>
+        <v>465644</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
@@ -2578,13 +2584,13 @@
       <c r="F89" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G89" s="2" t="s">
-        <v>10</v>
+      <c r="G89" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>465814</v>
+        <v>465653</v>
       </c>
       <c r="B90" t="s">
         <v>7</v>
@@ -2596,18 +2602,18 @@
         <v>7</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>465850</v>
+        <v>465814</v>
       </c>
       <c r="B91" t="s">
         <v>7</v>
@@ -2619,18 +2625,18 @@
         <v>7</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F91" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>466433</v>
+        <v>465850</v>
       </c>
       <c r="B92" t="s">
         <v>7</v>
@@ -2641,8 +2647,8 @@
       <c r="D92" t="s">
         <v>7</v>
       </c>
-      <c r="E92" s="3" t="s">
-        <v>9</v>
+      <c r="E92" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>9</v>
@@ -2653,7 +2659,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>466579</v>
+        <v>466433</v>
       </c>
       <c r="B93" t="s">
         <v>7</v>
@@ -2664,88 +2670,88 @@
       <c r="D93" t="s">
         <v>7</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F93" s="2" t="s">
+      <c r="E93" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
+        <v>466579</v>
+      </c>
+      <c r="B94" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" t="s">
+        <v>7</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
         <v>466801</v>
       </c>
-      <c r="B94" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s">
-        <v>8</v>
-      </c>
-      <c r="D94" t="s">
-        <v>7</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95">
+      <c r="B95" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" t="s">
+        <v>7</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96">
         <v>466803</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B96" t="s">
         <v>16</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C96" t="s">
         <v>16</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D96" t="s">
         <v>16</v>
       </c>
-      <c r="E95" t="s">
-        <v>9</v>
-      </c>
-      <c r="F95" t="s">
-        <v>10</v>
-      </c>
-      <c r="G95" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>466831</v>
-      </c>
-      <c r="B96" t="s">
-        <v>7</v>
-      </c>
-      <c r="C96" t="s">
-        <v>8</v>
-      </c>
-      <c r="D96" t="s">
-        <v>7</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>9</v>
+      <c r="E96" t="s">
+        <v>9</v>
+      </c>
+      <c r="F96" t="s">
+        <v>10</v>
+      </c>
+      <c r="G96" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>466968</v>
+        <v>466831</v>
       </c>
       <c r="B97" t="s">
         <v>7</v>
@@ -2757,18 +2763,18 @@
         <v>7</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>467069</v>
+        <v>466968</v>
       </c>
       <c r="B98" t="s">
         <v>7</v>
@@ -2780,18 +2786,18 @@
         <v>7</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>467189</v>
+        <v>467069</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
@@ -2805,8 +2811,8 @@
       <c r="E99" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>9</v>
+      <c r="F99" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G99" s="3" t="s">
         <v>9</v>
@@ -2814,7 +2820,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>467214</v>
+        <v>467189</v>
       </c>
       <c r="B100" t="s">
         <v>7</v>
@@ -2825,19 +2831,19 @@
       <c r="D100" t="s">
         <v>7</v>
       </c>
-      <c r="E100" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>10</v>
+      <c r="E100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>467243</v>
+        <v>467214</v>
       </c>
       <c r="B101" t="s">
         <v>7</v>
@@ -2848,11 +2854,11 @@
       <c r="D101" t="s">
         <v>7</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>9</v>
+      <c r="E101" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>10</v>
@@ -2860,7 +2866,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>467436</v>
+        <v>467243</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
@@ -2874,16 +2880,16 @@
       <c r="E102" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="F102" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>467451</v>
+        <v>467436</v>
       </c>
       <c r="B103" t="s">
         <v>7</v>
@@ -2894,19 +2900,19 @@
       <c r="D103" t="s">
         <v>7</v>
       </c>
-      <c r="E103" s="3" t="s">
-        <v>9</v>
+      <c r="E103" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G103" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>467455</v>
+        <v>467451</v>
       </c>
       <c r="B104" t="s">
         <v>7</v>
@@ -2917,19 +2923,19 @@
       <c r="D104" t="s">
         <v>7</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>10</v>
+      <c r="E104" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G104" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>467461</v>
+        <v>467455</v>
       </c>
       <c r="B105" t="s">
         <v>7</v>
@@ -2941,7 +2947,7 @@
         <v>7</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>9</v>
@@ -2952,7 +2958,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>467493</v>
+        <v>467461</v>
       </c>
       <c r="B106" t="s">
         <v>7</v>
@@ -2966,16 +2972,16 @@
       <c r="E106" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F106" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G106" s="3" t="s">
+      <c r="F106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G106" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>467497</v>
+        <v>467493</v>
       </c>
       <c r="B107" t="s">
         <v>7</v>
@@ -2987,10 +2993,10 @@
         <v>7</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F107" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G107" s="3" t="s">
         <v>9</v>
@@ -2998,7 +3004,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>467501</v>
+        <v>467497</v>
       </c>
       <c r="B108" t="s">
         <v>7</v>
@@ -3010,18 +3016,18 @@
         <v>7</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G108" s="2" t="s">
-        <v>10</v>
+      <c r="G108" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>467636</v>
+        <v>467501</v>
       </c>
       <c r="B109" t="s">
         <v>7</v>
@@ -3035,16 +3041,16 @@
       <c r="E109" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F109" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G109" s="3" t="s">
-        <v>9</v>
+      <c r="F109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>467744</v>
+        <v>467636</v>
       </c>
       <c r="B110" t="s">
         <v>7</v>
@@ -3055,10 +3061,10 @@
       <c r="D110" t="s">
         <v>7</v>
       </c>
-      <c r="E110" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F110" s="2" t="s">
+      <c r="E110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G110" s="3" t="s">
@@ -3067,7 +3073,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>467750</v>
+        <v>467744</v>
       </c>
       <c r="B111" t="s">
         <v>7</v>
@@ -3084,13 +3090,13 @@
       <c r="F111" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G111" s="2" t="s">
-        <v>10</v>
+      <c r="G111" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>467765</v>
+        <v>467750</v>
       </c>
       <c r="B112" t="s">
         <v>7</v>
@@ -3101,10 +3107,10 @@
       <c r="D112" t="s">
         <v>7</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F112" s="3" t="s">
+      <c r="E112" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G112" s="2" t="s">
@@ -3113,7 +3119,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>467775</v>
+        <v>467765</v>
       </c>
       <c r="B113" t="s">
         <v>7</v>
@@ -3127,7 +3133,7 @@
       <c r="E113" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="F113" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G113" s="2" t="s">
@@ -3136,7 +3142,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>467836</v>
+        <v>467775</v>
       </c>
       <c r="B114" t="s">
         <v>7</v>
@@ -3159,7 +3165,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>467870</v>
+        <v>467836</v>
       </c>
       <c r="B115" t="s">
         <v>7</v>
@@ -3177,12 +3183,12 @@
         <v>9</v>
       </c>
       <c r="G115" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>467873</v>
+        <v>467870</v>
       </c>
       <c r="B116" t="s">
         <v>7</v>
@@ -3194,18 +3200,18 @@
         <v>7</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G116" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>467940</v>
+        <v>467873</v>
       </c>
       <c r="B117" t="s">
         <v>7</v>
@@ -3216,7 +3222,7 @@
       <c r="D117" t="s">
         <v>7</v>
       </c>
-      <c r="E117" s="3" t="s">
+      <c r="E117" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F117" s="2" t="s">
@@ -3228,7 +3234,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>467947</v>
+        <v>467940</v>
       </c>
       <c r="B118" t="s">
         <v>7</v>
@@ -3239,19 +3245,19 @@
       <c r="D118" t="s">
         <v>7</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>10</v>
+      <c r="E118" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>467963</v>
+        <v>467947</v>
       </c>
       <c r="B119" t="s">
         <v>7</v>
@@ -3263,7 +3269,7 @@
         <v>7</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>9</v>
@@ -3274,7 +3280,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>467975</v>
+        <v>467963</v>
       </c>
       <c r="B120" t="s">
         <v>7</v>
@@ -3291,24 +3297,24 @@
       <c r="F120" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G120" s="3" t="s">
+      <c r="G120" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>467986</v>
+        <v>467975</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C121" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D121" t="s">
         <v>7</v>
       </c>
-      <c r="E121" s="3" t="s">
+      <c r="E121" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F121" s="2" t="s">
@@ -3320,30 +3326,30 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>468167</v>
+        <v>467986</v>
       </c>
       <c r="B122" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C122" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D122" t="s">
         <v>7</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="E122" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G122" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>468178</v>
+        <v>468167</v>
       </c>
       <c r="B123" t="s">
         <v>7</v>
@@ -3355,18 +3361,18 @@
         <v>7</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>468255</v>
+        <v>468178</v>
       </c>
       <c r="B124" t="s">
         <v>7</v>
@@ -3378,10 +3384,10 @@
         <v>7</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>9</v>
@@ -3389,7 +3395,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>468284</v>
+        <v>468255</v>
       </c>
       <c r="B125" t="s">
         <v>7</v>
@@ -3401,10 +3407,10 @@
         <v>7</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>9</v>
@@ -3412,7 +3418,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>468311</v>
+        <v>468284</v>
       </c>
       <c r="B126" t="s">
         <v>7</v>
@@ -3424,10 +3430,10 @@
         <v>7</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>9</v>
@@ -3435,7 +3441,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>468546</v>
+        <v>468311</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
@@ -3447,18 +3453,18 @@
         <v>7</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>468554</v>
+        <v>468546</v>
       </c>
       <c r="B128" t="s">
         <v>7</v>
@@ -3470,10 +3476,10 @@
         <v>7</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>10</v>
@@ -3481,7 +3487,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>468607</v>
+        <v>468554</v>
       </c>
       <c r="B129" t="s">
         <v>7</v>
@@ -3493,10 +3499,10 @@
         <v>7</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G129" s="2" t="s">
         <v>10</v>
@@ -3504,7 +3510,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>468643</v>
+        <v>468607</v>
       </c>
       <c r="B130" t="s">
         <v>7</v>
@@ -3527,7 +3533,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>468736</v>
+        <v>468643</v>
       </c>
       <c r="B131" t="s">
         <v>7</v>
@@ -3541,16 +3547,16 @@
       <c r="E131" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F131" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G131" s="3" t="s">
-        <v>9</v>
+      <c r="F131" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>468763</v>
+        <v>468736</v>
       </c>
       <c r="B132" t="s">
         <v>7</v>
@@ -3562,18 +3568,18 @@
         <v>7</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G132" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>468859</v>
+        <v>468763</v>
       </c>
       <c r="B133" t="s">
         <v>7</v>
@@ -3585,18 +3591,18 @@
         <v>7</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G133" s="3" t="s">
-        <v>9</v>
+      <c r="G133" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>468876</v>
+        <v>468859</v>
       </c>
       <c r="B134" t="s">
         <v>7</v>
@@ -3608,10 +3614,10 @@
         <v>7</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F134" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F134" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>9</v>
@@ -3619,7 +3625,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>468882</v>
+        <v>468876</v>
       </c>
       <c r="B135" t="s">
         <v>7</v>
@@ -3633,7 +3639,7 @@
       <c r="E135" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F135" s="2" t="s">
+      <c r="F135" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G135" s="3" t="s">
@@ -3642,7 +3648,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>468898</v>
+        <v>468882</v>
       </c>
       <c r="B136" t="s">
         <v>7</v>
@@ -3657,62 +3663,62 @@
         <v>9</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G136" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
+        <v>468898</v>
+      </c>
+      <c r="B137" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137" t="s">
+        <v>8</v>
+      </c>
+      <c r="D137" t="s">
+        <v>7</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
         <v>468903</v>
       </c>
-      <c r="B137" t="s">
-        <v>7</v>
-      </c>
-      <c r="C137" t="s">
-        <v>8</v>
-      </c>
-      <c r="D137" t="s">
-        <v>7</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F137" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G137" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="4">
+      <c r="B138" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" t="s">
+        <v>7</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F138" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="4">
         <v>468961</v>
       </c>
-      <c r="B138" t="s">
-        <v>7</v>
-      </c>
-      <c r="C138" t="s">
-        <v>8</v>
-      </c>
-      <c r="D138" t="s">
-        <v>7</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F138" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A139" s="1">
-        <v>469129</v>
-      </c>
       <c r="B139" t="s">
         <v>7</v>
       </c>
@@ -3726,7 +3732,7 @@
         <v>10</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G139" s="3" t="s">
         <v>9</v>
@@ -3734,7 +3740,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>469142</v>
+        <v>469129</v>
       </c>
       <c r="B140" t="s">
         <v>7</v>
@@ -3751,13 +3757,13 @@
       <c r="F140" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G140" s="2" t="s">
+      <c r="G140" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>469186</v>
+        <v>469142</v>
       </c>
       <c r="B141" t="s">
         <v>7</v>
@@ -3769,10 +3775,10 @@
         <v>7</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F141" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F141" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>9</v>
@@ -3780,7 +3786,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>469193</v>
+        <v>469186</v>
       </c>
       <c r="B142" t="s">
         <v>7</v>
@@ -3791,7 +3797,7 @@
       <c r="D142" t="s">
         <v>7</v>
       </c>
-      <c r="E142" s="3" t="s">
+      <c r="E142" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F142" s="3" t="s">
@@ -3803,7 +3809,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>469213</v>
+        <v>469193</v>
       </c>
       <c r="B143" t="s">
         <v>7</v>
@@ -3814,66 +3820,66 @@
       <c r="D143" t="s">
         <v>7</v>
       </c>
-      <c r="E143" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F143" s="2" t="s">
+      <c r="E143" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F143" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
+        <v>469213</v>
+      </c>
+      <c r="B144" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144" t="s">
+        <v>8</v>
+      </c>
+      <c r="D144" t="s">
+        <v>7</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
         <v>469288</v>
       </c>
-      <c r="B144" t="s">
-        <v>7</v>
-      </c>
-      <c r="C144" t="s">
-        <v>8</v>
-      </c>
-      <c r="D144" t="s">
-        <v>7</v>
-      </c>
-      <c r="E144" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F144" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G144" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" s="4">
+      <c r="B145" t="s">
+        <v>7</v>
+      </c>
+      <c r="C145" t="s">
+        <v>8</v>
+      </c>
+      <c r="D145" t="s">
+        <v>7</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="4">
         <v>469327</v>
       </c>
-      <c r="B145" t="s">
-        <v>7</v>
-      </c>
-      <c r="C145" t="s">
-        <v>8</v>
-      </c>
-      <c r="D145" t="s">
-        <v>7</v>
-      </c>
-      <c r="E145" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F145" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G145" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="1">
-        <v>469351</v>
-      </c>
       <c r="B146" t="s">
         <v>7</v>
       </c>
@@ -3887,7 +3893,7 @@
         <v>9</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>10</v>
@@ -3895,7 +3901,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>469358</v>
+        <v>469351</v>
       </c>
       <c r="B147" t="s">
         <v>7</v>
@@ -3906,19 +3912,19 @@
       <c r="D147" t="s">
         <v>7</v>
       </c>
-      <c r="E147" s="3" t="s">
+      <c r="E147" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>469474</v>
+        <v>469358</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
@@ -3929,19 +3935,19 @@
       <c r="D148" t="s">
         <v>7</v>
       </c>
-      <c r="E148" s="2" t="s">
+      <c r="E148" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G148" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G148" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>469486</v>
+        <v>469474</v>
       </c>
       <c r="B149" t="s">
         <v>7</v>
@@ -3953,18 +3959,18 @@
         <v>7</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G149" s="2" t="s">
-        <v>10</v>
+      <c r="G149" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>469625</v>
+        <v>469486</v>
       </c>
       <c r="B150" t="s">
         <v>7</v>
@@ -3976,18 +3982,18 @@
         <v>7</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>469740</v>
+        <v>469625</v>
       </c>
       <c r="B151" t="s">
         <v>7</v>
@@ -4001,7 +4007,7 @@
       <c r="E151" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F151" s="3" t="s">
+      <c r="F151" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G151" s="2" t="s">
@@ -4010,7 +4016,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>469823</v>
+        <v>469740</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
@@ -4024,16 +4030,16 @@
       <c r="E152" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F152" s="2" t="s">
-        <v>10</v>
+      <c r="F152" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>469857</v>
+        <v>469823</v>
       </c>
       <c r="B153" t="s">
         <v>7</v>
@@ -4045,18 +4051,18 @@
         <v>7</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>469975</v>
+        <v>469857</v>
       </c>
       <c r="B154" t="s">
         <v>7</v>
@@ -4068,7 +4074,7 @@
         <v>7</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>9</v>
@@ -4079,7 +4085,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>470129</v>
+        <v>469975</v>
       </c>
       <c r="B155" t="s">
         <v>7</v>
@@ -4091,18 +4097,18 @@
         <v>7</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F155" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>470144</v>
+        <v>470129</v>
       </c>
       <c r="B156" t="s">
         <v>7</v>
@@ -4117,15 +4123,15 @@
         <v>10</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>470282</v>
+        <v>470144</v>
       </c>
       <c r="B157" t="s">
         <v>7</v>
@@ -4137,10 +4143,10 @@
         <v>7</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G157" s="2" t="s">
         <v>9</v>
@@ -4148,7 +4154,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>470290</v>
+        <v>470282</v>
       </c>
       <c r="B158" t="s">
         <v>7</v>
@@ -4160,18 +4166,18 @@
         <v>7</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G158" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G158" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>470309</v>
+        <v>470290</v>
       </c>
       <c r="B159" t="s">
         <v>7</v>
@@ -4183,18 +4189,18 @@
         <v>7</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G159" s="2" t="s">
-        <v>10</v>
+      <c r="G159" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>470373</v>
+        <v>470309</v>
       </c>
       <c r="B160" t="s">
         <v>7</v>
@@ -4206,18 +4212,18 @@
         <v>7</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>470405</v>
+        <v>470373</v>
       </c>
       <c r="B161" t="s">
         <v>7</v>
@@ -4232,15 +4238,15 @@
         <v>10</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G161" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G161" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>470467</v>
+        <v>470405</v>
       </c>
       <c r="B162" t="s">
         <v>7</v>
@@ -4255,15 +4261,15 @@
         <v>10</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G162" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G162" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>470488</v>
+        <v>470467</v>
       </c>
       <c r="B163" t="s">
         <v>7</v>
@@ -4277,7 +4283,7 @@
       <c r="E163" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F163" s="3" t="s">
+      <c r="F163" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G163" s="2" t="s">
@@ -4286,7 +4292,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>470638</v>
+        <v>470488</v>
       </c>
       <c r="B164" t="s">
         <v>7</v>
@@ -4304,12 +4310,12 @@
         <v>9</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>470668</v>
+        <v>470638</v>
       </c>
       <c r="B165" t="s">
         <v>7</v>
@@ -4321,10 +4327,10 @@
         <v>7</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F165" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G165" s="2" t="s">
         <v>10</v>
@@ -4332,7 +4338,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>470754</v>
+        <v>470668</v>
       </c>
       <c r="B166" t="s">
         <v>7</v>
@@ -4344,18 +4350,18 @@
         <v>7</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G166" s="3" t="s">
-        <v>9</v>
+        <v>9</v>
+      </c>
+      <c r="F166" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G166" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>470773</v>
+        <v>470754</v>
       </c>
       <c r="B167" t="s">
         <v>7</v>
@@ -4367,9 +4373,9 @@
         <v>7</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F167" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F167" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G167" s="3" t="s">
@@ -4378,7 +4384,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>470782</v>
+        <v>470773</v>
       </c>
       <c r="B168" t="s">
         <v>7</v>
@@ -4395,13 +4401,13 @@
       <c r="F168" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G168" s="2" t="s">
+      <c r="G168" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>470830</v>
+        <v>470782</v>
       </c>
       <c r="B169" t="s">
         <v>7</v>
@@ -4413,10 +4419,10 @@
         <v>7</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G169" s="2" t="s">
         <v>9</v>
@@ -4424,7 +4430,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>470859</v>
+        <v>470830</v>
       </c>
       <c r="B170" t="s">
         <v>7</v>
@@ -4439,7 +4445,7 @@
         <v>10</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G170" s="2" t="s">
         <v>9</v>
@@ -4447,7 +4453,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>470921</v>
+        <v>470859</v>
       </c>
       <c r="B171" t="s">
         <v>7</v>
@@ -4465,12 +4471,12 @@
         <v>9</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>471016</v>
+        <v>470921</v>
       </c>
       <c r="B172" t="s">
         <v>7</v>
@@ -4493,7 +4499,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>471028</v>
+        <v>471016</v>
       </c>
       <c r="B173" t="s">
         <v>7</v>
@@ -4504,19 +4510,19 @@
       <c r="D173" t="s">
         <v>7</v>
       </c>
-      <c r="E173" s="3" t="s">
-        <v>9</v>
+      <c r="E173" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G173" s="3" t="s">
-        <v>9</v>
+      <c r="G173" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>471129</v>
+        <v>471028</v>
       </c>
       <c r="B174" t="s">
         <v>7</v>
@@ -4527,11 +4533,11 @@
       <c r="D174" t="s">
         <v>7</v>
       </c>
-      <c r="E174" s="2" t="s">
-        <v>10</v>
+      <c r="E174" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F174" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G174" s="3" t="s">
         <v>9</v>
@@ -4539,7 +4545,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>471229</v>
+        <v>471129</v>
       </c>
       <c r="B175" t="s">
         <v>7</v>
@@ -4553,16 +4559,16 @@
       <c r="E175" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F175" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G175" s="2" t="s">
-        <v>10</v>
+      <c r="F175" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>471255</v>
+        <v>471229</v>
       </c>
       <c r="B176" t="s">
         <v>7</v>
@@ -4576,7 +4582,7 @@
       <c r="E176" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F176" s="2" t="s">
+      <c r="F176" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G176" s="2" t="s">
@@ -4585,7 +4591,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>471263</v>
+        <v>471255</v>
       </c>
       <c r="B177" t="s">
         <v>7</v>
@@ -4603,12 +4609,12 @@
         <v>9</v>
       </c>
       <c r="G177" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>471492</v>
+        <v>471263</v>
       </c>
       <c r="B178" t="s">
         <v>7</v>
@@ -4626,12 +4632,12 @@
         <v>9</v>
       </c>
       <c r="G178" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>471545</v>
+        <v>471492</v>
       </c>
       <c r="B179" t="s">
         <v>7</v>
@@ -4649,12 +4655,12 @@
         <v>9</v>
       </c>
       <c r="G179" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>471760</v>
+        <v>471545</v>
       </c>
       <c r="B180" t="s">
         <v>7</v>
@@ -4672,12 +4678,12 @@
         <v>9</v>
       </c>
       <c r="G180" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>472004</v>
+        <v>471760</v>
       </c>
       <c r="B181" t="s">
         <v>7</v>
@@ -4689,10 +4695,10 @@
         <v>7</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G181" s="2" t="s">
         <v>10</v>
@@ -4700,7 +4706,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>472145</v>
+        <v>472004</v>
       </c>
       <c r="B182" t="s">
         <v>7</v>
@@ -4715,7 +4721,7 @@
         <v>9</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G182" s="2" t="s">
         <v>10</v>
@@ -4723,7 +4729,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>472434</v>
+        <v>472145</v>
       </c>
       <c r="B183" t="s">
         <v>7</v>
@@ -4738,7 +4744,7 @@
         <v>9</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G183" s="2" t="s">
         <v>10</v>
@@ -4746,7 +4752,7 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>472501</v>
+        <v>472434</v>
       </c>
       <c r="B184" t="s">
         <v>7</v>
@@ -4761,15 +4767,15 @@
         <v>9</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>472537</v>
+        <v>472501</v>
       </c>
       <c r="B185" t="s">
         <v>7</v>
@@ -4781,18 +4787,18 @@
         <v>7</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F185" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G185" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G185" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>472782</v>
+        <v>472537</v>
       </c>
       <c r="B186" t="s">
         <v>7</v>
@@ -4807,15 +4813,15 @@
         <v>10</v>
       </c>
       <c r="F186" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G186" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G186" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>472962</v>
+        <v>472782</v>
       </c>
       <c r="B187" t="s">
         <v>7</v>
@@ -4829,16 +4835,16 @@
       <c r="E187" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F187" s="3" t="s">
+      <c r="F187" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>473195</v>
+        <v>472962</v>
       </c>
       <c r="B188" t="s">
         <v>7</v>
@@ -4850,9 +4856,9 @@
         <v>7</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F188" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F188" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G188" s="2" t="s">
@@ -4861,7 +4867,7 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>473215</v>
+        <v>473195</v>
       </c>
       <c r="B189" t="s">
         <v>7</v>
@@ -4873,18 +4879,18 @@
         <v>7</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F189" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G189" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>473482</v>
+        <v>473215</v>
       </c>
       <c r="B190" t="s">
         <v>7</v>
@@ -4902,12 +4908,12 @@
         <v>9</v>
       </c>
       <c r="G190" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>473708</v>
+        <v>473482</v>
       </c>
       <c r="B191" t="s">
         <v>7</v>
@@ -4925,12 +4931,12 @@
         <v>9</v>
       </c>
       <c r="G191" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>473899</v>
+        <v>473708</v>
       </c>
       <c r="B192" t="s">
         <v>7</v>
@@ -4948,12 +4954,12 @@
         <v>9</v>
       </c>
       <c r="G192" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>475115</v>
+        <v>473899</v>
       </c>
       <c r="B193" t="s">
         <v>7</v>
@@ -4968,15 +4974,15 @@
         <v>10</v>
       </c>
       <c r="F193" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G193" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>476008</v>
+        <v>475115</v>
       </c>
       <c r="B194" t="s">
         <v>7</v>
@@ -4991,15 +4997,15 @@
         <v>10</v>
       </c>
       <c r="F194" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>476289</v>
+        <v>476008</v>
       </c>
       <c r="B195" t="s">
         <v>7</v>
@@ -5013,7 +5019,7 @@
       <c r="E195" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F195" s="3" t="s">
+      <c r="F195" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G195" s="2" t="s">
@@ -5022,7 +5028,7 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>476531</v>
+        <v>476289</v>
       </c>
       <c r="B196" t="s">
         <v>7</v>
@@ -5034,10 +5040,10 @@
         <v>7</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F196" s="2" t="s">
-        <v>10</v>
+        <v>10</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G196" s="2" t="s">
         <v>10</v>
@@ -5045,7 +5051,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>476883</v>
+        <v>476531</v>
       </c>
       <c r="B197" t="s">
         <v>7</v>
@@ -5060,7 +5066,7 @@
         <v>9</v>
       </c>
       <c r="F197" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G197" s="2" t="s">
         <v>10</v>
@@ -5068,7 +5074,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>477153</v>
+        <v>476883</v>
       </c>
       <c r="B198" t="s">
         <v>7</v>
@@ -5080,7 +5086,7 @@
         <v>7</v>
       </c>
       <c r="E198" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F198" s="2" t="s">
         <v>9</v>
@@ -5091,7 +5097,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>477738</v>
+        <v>477153</v>
       </c>
       <c r="B199" t="s">
         <v>7</v>
@@ -5114,7 +5120,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>478406</v>
+        <v>477738</v>
       </c>
       <c r="B200" t="s">
         <v>7</v>
@@ -5126,18 +5132,18 @@
         <v>7</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F200" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>478589</v>
+        <v>478406</v>
       </c>
       <c r="B201" t="s">
         <v>7</v>
@@ -5149,10 +5155,10 @@
         <v>7</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F201" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G201" s="2" t="s">
         <v>9</v>
@@ -5160,7 +5166,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>479276</v>
+        <v>478589</v>
       </c>
       <c r="B202" t="s">
         <v>7</v>
@@ -5172,10 +5178,10 @@
         <v>7</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F202" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G202" s="2" t="s">
         <v>9</v>
@@ -5183,70 +5189,93 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
+        <v>479276</v>
+      </c>
+      <c r="B203" t="s">
+        <v>7</v>
+      </c>
+      <c r="C203" t="s">
+        <v>8</v>
+      </c>
+      <c r="D203" t="s">
+        <v>7</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F203" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
         <v>479658</v>
       </c>
-      <c r="B203" t="s">
-        <v>7</v>
-      </c>
-      <c r="C203" t="s">
-        <v>8</v>
-      </c>
-      <c r="D203" t="s">
-        <v>7</v>
-      </c>
-      <c r="E203" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F203" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G203" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A204">
-        <v>532682</v>
-      </c>
       <c r="B204" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C204" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D204" t="s">
-        <v>34</v>
-      </c>
-      <c r="E204" t="s">
-        <v>9</v>
-      </c>
-      <c r="F204" t="s">
-        <v>9</v>
-      </c>
-      <c r="G204" t="s">
+        <v>7</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F204" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G204" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205">
+        <v>532682</v>
+      </c>
+      <c r="B205" t="s">
+        <v>11</v>
+      </c>
+      <c r="C205" t="s">
+        <v>33</v>
+      </c>
+      <c r="D205" t="s">
+        <v>34</v>
+      </c>
+      <c r="E205" t="s">
+        <v>9</v>
+      </c>
+      <c r="F205" t="s">
+        <v>9</v>
+      </c>
+      <c r="G205" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206">
         <v>987654</v>
       </c>
-      <c r="B205" t="s">
-        <v>7</v>
-      </c>
-      <c r="C205" t="s">
-        <v>8</v>
-      </c>
-      <c r="D205" t="s">
+      <c r="B206" t="s">
+        <v>7</v>
+      </c>
+      <c r="C206" t="s">
+        <v>8</v>
+      </c>
+      <c r="D206" t="s">
         <v>13</v>
       </c>
-      <c r="E205" t="s">
-        <v>10</v>
-      </c>
-      <c r="F205" t="s">
-        <v>9</v>
-      </c>
-      <c r="G205" t="s">
+      <c r="E206" t="s">
+        <v>10</v>
+      </c>
+      <c r="F206" t="s">
+        <v>9</v>
+      </c>
+      <c r="G206" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited GUIs, Added Documentation
Added Descriptions to GUIs, changed Font sizes
</commit_message>
<xml_diff>
--- a/data/StudentData.xlsx
+++ b/data/StudentData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27235" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37918" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -5286,7 +5286,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H205"/>
+  <dimension ref="A1:H206"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5332,10 +5332,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2"/>
       <c r="H2"/>
@@ -5360,10 +5360,10 @@
         <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
@@ -5428,10 +5428,10 @@
         <v>31</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
@@ -5472,16 +5472,16 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
@@ -5498,10 +5498,10 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
@@ -5542,10 +5542,10 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
@@ -5564,10 +5564,10 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
@@ -5586,16 +5586,16 @@
         <v>8</v>
       </c>
       <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s">
         <v>45</v>
       </c>
-      <c r="F13" t="s">
-        <v>47</v>
-      </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14">
@@ -5634,16 +5634,16 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H15" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16">
@@ -5684,10 +5684,10 @@
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
@@ -5706,16 +5706,16 @@
         <v>8</v>
       </c>
       <c r="E18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" t="s">
         <v>45</v>
       </c>
-      <c r="F18" t="s">
-        <v>47</v>
-      </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19">
@@ -5756,10 +5756,10 @@
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
@@ -5778,10 +5778,10 @@
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
@@ -5800,10 +5800,10 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
@@ -5822,10 +5822,10 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G23"/>
       <c r="H23"/>
@@ -5844,10 +5844,10 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
@@ -5866,13 +5866,13 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F25" t="s">
         <v>48</v>
       </c>
       <c r="G25" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H25"/>
     </row>
@@ -5890,10 +5890,10 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G26"/>
       <c r="H26"/>
@@ -5912,16 +5912,16 @@
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G27" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H27" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28">
@@ -5938,10 +5938,10 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
@@ -5960,16 +5960,16 @@
         <v>8</v>
       </c>
       <c r="E29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
         <v>45</v>
       </c>
-      <c r="F29" t="s">
-        <v>47</v>
-      </c>
       <c r="G29" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H29" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30">
@@ -6034,10 +6034,10 @@
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G32"/>
       <c r="H32"/>
@@ -6080,10 +6080,10 @@
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G34"/>
       <c r="H34"/>
@@ -6102,16 +6102,16 @@
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F35" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G35" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H35" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36">
@@ -6128,10 +6128,10 @@
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F36" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G36"/>
       <c r="H36"/>
@@ -6150,16 +6150,16 @@
         <v>8</v>
       </c>
       <c r="E37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" t="s">
         <v>45</v>
       </c>
-      <c r="F37" t="s">
-        <v>47</v>
-      </c>
       <c r="G37" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H37" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38">
@@ -6176,16 +6176,16 @@
         <v>19</v>
       </c>
       <c r="E38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F38" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G38" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H38" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39">
@@ -6226,10 +6226,10 @@
         <v>8</v>
       </c>
       <c r="E40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G40"/>
       <c r="H40"/>
@@ -6248,13 +6248,13 @@
         <v>8</v>
       </c>
       <c r="E41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F41" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H41"/>
     </row>
@@ -6272,10 +6272,10 @@
         <v>8</v>
       </c>
       <c r="E42" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G42"/>
       <c r="H42"/>
@@ -6294,10 +6294,10 @@
         <v>14</v>
       </c>
       <c r="E43" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F43" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G43"/>
       <c r="H43"/>
@@ -6316,10 +6316,10 @@
         <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F44" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G44"/>
       <c r="H44"/>
@@ -6360,10 +6360,10 @@
         <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G46"/>
       <c r="H46"/>
@@ -6382,10 +6382,10 @@
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F47" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G47"/>
       <c r="H47"/>
@@ -6404,10 +6404,10 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G48"/>
       <c r="H48"/>
@@ -6426,10 +6426,10 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G49"/>
       <c r="H49"/>
@@ -6448,56 +6448,54 @@
         <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G50"/>
       <c r="H50"/>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B51" t="n">
-        <v>353515.0</v>
+        <v>351353.0</v>
       </c>
       <c r="C51" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="D51" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="E51" t="s">
         <v>45</v>
       </c>
       <c r="F51" t="s">
-        <v>47</v>
-      </c>
-      <c r="G51" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G51"/>
       <c r="H51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B52" t="n">
-        <v>353621.0</v>
+        <v>353515.0</v>
       </c>
       <c r="C52" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D52" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E52" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F52" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G52" t="s">
         <v>44</v>
@@ -6509,13 +6507,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>406490.0</v>
+        <v>353621.0</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E53" t="s">
         <v>48</v>
@@ -6530,10 +6528,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>409089.0</v>
+        <v>406490.0</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
@@ -6545,63 +6543,63 @@
         <v>48</v>
       </c>
       <c r="F54" t="s">
-        <v>44</v>
-      </c>
-      <c r="G54"/>
+        <v>45</v>
+      </c>
+      <c r="G54" t="s">
+        <v>44</v>
+      </c>
       <c r="H54"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B55" t="n">
-        <v>411168.0</v>
+        <v>409089.0</v>
       </c>
       <c r="C55" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E55" t="s">
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G55"/>
       <c r="H55"/>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B56" t="n">
-        <v>417688.0</v>
+        <v>411168.0</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E56" t="s">
         <v>45</v>
       </c>
       <c r="F56" t="s">
-        <v>48</v>
-      </c>
-      <c r="G56" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G56"/>
       <c r="H56"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B57" t="n">
-        <v>419371.0</v>
+        <v>417688.0</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
@@ -6610,13 +6608,13 @@
         <v>8</v>
       </c>
       <c r="E57" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G57" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H57"/>
     </row>
@@ -6625,7 +6623,7 @@
         <v>49</v>
       </c>
       <c r="B58" t="n">
-        <v>419659.0</v>
+        <v>419371.0</v>
       </c>
       <c r="C58" t="s">
         <v>7</v>
@@ -6646,10 +6644,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B59" t="n">
-        <v>420119.0</v>
+        <v>419659.0</v>
       </c>
       <c r="C59" t="s">
         <v>7</v>
@@ -6658,24 +6656,22 @@
         <v>8</v>
       </c>
       <c r="E59" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F59" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G59" t="s">
-        <v>44</v>
-      </c>
-      <c r="H59" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H59"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B60" t="n">
-        <v>436542.0</v>
+        <v>420119.0</v>
       </c>
       <c r="C60" t="s">
         <v>7</v>
@@ -6684,20 +6680,24 @@
         <v>8</v>
       </c>
       <c r="E60" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F60" t="s">
-        <v>48</v>
-      </c>
-      <c r="G60"/>
-      <c r="H60"/>
+        <v>45</v>
+      </c>
+      <c r="G60" t="s">
+        <v>48</v>
+      </c>
+      <c r="H60" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
         <v>50</v>
       </c>
       <c r="B61" t="n">
-        <v>439155.0</v>
+        <v>436542.0</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
@@ -6719,7 +6719,7 @@
         <v>50</v>
       </c>
       <c r="B62" t="n">
-        <v>441021.0</v>
+        <v>439155.0</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
@@ -6738,10 +6738,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B63" t="n">
-        <v>442262.0</v>
+        <v>441021.0</v>
       </c>
       <c r="C63" t="s">
         <v>7</v>
@@ -6750,20 +6750,20 @@
         <v>8</v>
       </c>
       <c r="E63" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F63" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G63"/>
       <c r="H63"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B64" t="n">
-        <v>442931.0</v>
+        <v>442262.0</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
@@ -6775,21 +6775,17 @@
         <v>47</v>
       </c>
       <c r="F64" t="s">
-        <v>45</v>
-      </c>
-      <c r="G64" t="s">
-        <v>48</v>
-      </c>
-      <c r="H64" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G64"/>
+      <c r="H64"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B65" t="n">
-        <v>443257.0</v>
+        <v>442931.0</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
@@ -6801,19 +6797,21 @@
         <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G65" t="s">
-        <v>48</v>
-      </c>
-      <c r="H65"/>
+        <v>44</v>
+      </c>
+      <c r="H65" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
         <v>52</v>
       </c>
       <c r="B66" t="n">
-        <v>446253.0</v>
+        <v>443257.0</v>
       </c>
       <c r="C66" t="s">
         <v>7</v>
@@ -6834,10 +6832,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B67" t="n">
-        <v>448013.0</v>
+        <v>446253.0</v>
       </c>
       <c r="C67" t="s">
         <v>7</v>
@@ -6849,19 +6847,19 @@
         <v>48</v>
       </c>
       <c r="F67" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G67" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H67"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B68" t="n">
-        <v>452390.0</v>
+        <v>448013.0</v>
       </c>
       <c r="C68" t="s">
         <v>7</v>
@@ -6870,24 +6868,22 @@
         <v>8</v>
       </c>
       <c r="E68" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F68" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G68" t="s">
-        <v>44</v>
-      </c>
-      <c r="H68" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H68"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B69" t="n">
-        <v>452992.0</v>
+        <v>452390.0</v>
       </c>
       <c r="C69" t="s">
         <v>7</v>
@@ -6899,19 +6895,21 @@
         <v>47</v>
       </c>
       <c r="F69" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G69" t="s">
-        <v>44</v>
-      </c>
-      <c r="H69"/>
+        <v>48</v>
+      </c>
+      <c r="H69" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
         <v>49</v>
       </c>
       <c r="B70" t="n">
-        <v>454280.0</v>
+        <v>452992.0</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
@@ -6920,22 +6918,22 @@
         <v>8</v>
       </c>
       <c r="E70" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F70" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G70" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H70"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B71" t="n">
-        <v>454287.0</v>
+        <v>454280.0</v>
       </c>
       <c r="C71" t="s">
         <v>7</v>
@@ -6949,15 +6947,17 @@
       <c r="F71" t="s">
         <v>44</v>
       </c>
-      <c r="G71"/>
+      <c r="G71" t="s">
+        <v>47</v>
+      </c>
       <c r="H71"/>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B72" t="n">
-        <v>454745.0</v>
+        <v>454287.0</v>
       </c>
       <c r="C72" t="s">
         <v>7</v>
@@ -6969,19 +6969,17 @@
         <v>44</v>
       </c>
       <c r="F72" t="s">
-        <v>45</v>
-      </c>
-      <c r="G72" t="s">
-        <v>47</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G72"/>
       <c r="H72"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B73" t="n">
-        <v>454770.0</v>
+        <v>454745.0</v>
       </c>
       <c r="C73" t="s">
         <v>7</v>
@@ -6990,20 +6988,22 @@
         <v>8</v>
       </c>
       <c r="E73" t="s">
+        <v>44</v>
+      </c>
+      <c r="F73" t="s">
         <v>45</v>
       </c>
-      <c r="F73" t="s">
-        <v>44</v>
-      </c>
-      <c r="G73"/>
+      <c r="G73" t="s">
+        <v>47</v>
+      </c>
       <c r="H73"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B74" t="n">
-        <v>455839.0</v>
+        <v>454770.0</v>
       </c>
       <c r="C74" t="s">
         <v>7</v>
@@ -7012,14 +7012,12 @@
         <v>8</v>
       </c>
       <c r="E74" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F74" t="s">
         <v>44</v>
       </c>
-      <c r="G74" t="s">
-        <v>47</v>
-      </c>
+      <c r="G74"/>
       <c r="H74"/>
     </row>
     <row r="75">
@@ -7027,7 +7025,7 @@
         <v>49</v>
       </c>
       <c r="B75" t="n">
-        <v>461540.0</v>
+        <v>455839.0</v>
       </c>
       <c r="C75" t="s">
         <v>7</v>
@@ -7036,13 +7034,13 @@
         <v>8</v>
       </c>
       <c r="E75" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F75" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G75" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H75"/>
     </row>
@@ -7051,7 +7049,7 @@
         <v>49</v>
       </c>
       <c r="B76" t="n">
-        <v>462838.0</v>
+        <v>461540.0</v>
       </c>
       <c r="C76" t="s">
         <v>7</v>
@@ -7060,10 +7058,10 @@
         <v>8</v>
       </c>
       <c r="E76" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F76" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G76" t="s">
         <v>44</v>
@@ -7075,19 +7073,19 @@
         <v>49</v>
       </c>
       <c r="B77" t="n">
-        <v>463462.0</v>
+        <v>462838.0</v>
       </c>
       <c r="C77" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E77" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F77" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G77" t="s">
         <v>44</v>
@@ -7096,36 +7094,34 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B78" t="n">
-        <v>463934.0</v>
+        <v>463462.0</v>
       </c>
       <c r="C78" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D78" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E78" t="s">
         <v>47</v>
       </c>
       <c r="F78" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G78" t="s">
-        <v>48</v>
-      </c>
-      <c r="H78" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H78"/>
     </row>
     <row r="79">
       <c r="A79" t="s">
         <v>46</v>
       </c>
       <c r="B79" t="n">
-        <v>464863.0</v>
+        <v>463934.0</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
@@ -7148,10 +7144,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B80" t="n">
-        <v>465018.0</v>
+        <v>464863.0</v>
       </c>
       <c r="C80" t="s">
         <v>7</v>
@@ -7160,22 +7156,24 @@
         <v>8</v>
       </c>
       <c r="E80" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F80" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G80" t="s">
-        <v>44</v>
-      </c>
-      <c r="H80"/>
+        <v>48</v>
+      </c>
+      <c r="H80" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B81" t="n">
-        <v>465085.0</v>
+        <v>465018.0</v>
       </c>
       <c r="C81" t="s">
         <v>7</v>
@@ -7184,20 +7182,22 @@
         <v>8</v>
       </c>
       <c r="E81" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F81" t="s">
-        <v>44</v>
-      </c>
-      <c r="G81"/>
+        <v>47</v>
+      </c>
+      <c r="G81" t="s">
+        <v>44</v>
+      </c>
       <c r="H81"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B82" t="n">
-        <v>465090.0</v>
+        <v>465085.0</v>
       </c>
       <c r="C82" t="s">
         <v>7</v>
@@ -7206,14 +7206,12 @@
         <v>8</v>
       </c>
       <c r="E82" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F82" t="s">
-        <v>48</v>
-      </c>
-      <c r="G82" t="s">
-        <v>44</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G82"/>
       <c r="H82"/>
     </row>
     <row r="83">
@@ -7221,7 +7219,7 @@
         <v>49</v>
       </c>
       <c r="B83" t="n">
-        <v>465141.0</v>
+        <v>465090.0</v>
       </c>
       <c r="C83" t="s">
         <v>7</v>
@@ -7230,22 +7228,22 @@
         <v>8</v>
       </c>
       <c r="E83" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F83" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G83" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H83"/>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B84" t="n">
-        <v>465275.0</v>
+        <v>465141.0</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -7254,24 +7252,22 @@
         <v>8</v>
       </c>
       <c r="E84" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F84" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G84" t="s">
-        <v>48</v>
-      </c>
-      <c r="H84" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H84"/>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B85" t="n">
-        <v>465391.0</v>
+        <v>465275.0</v>
       </c>
       <c r="C85" t="s">
         <v>7</v>
@@ -7280,22 +7276,24 @@
         <v>8</v>
       </c>
       <c r="E85" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F85" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G85" t="s">
         <v>44</v>
       </c>
-      <c r="H85"/>
+      <c r="H85" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B86" t="n">
-        <v>465431.0</v>
+        <v>465391.0</v>
       </c>
       <c r="C86" t="s">
         <v>7</v>
@@ -7304,24 +7302,22 @@
         <v>8</v>
       </c>
       <c r="E86" t="s">
+        <v>48</v>
+      </c>
+      <c r="F86" t="s">
         <v>45</v>
       </c>
-      <c r="F86" t="s">
-        <v>47</v>
-      </c>
       <c r="G86" t="s">
         <v>44</v>
       </c>
-      <c r="H86" t="s">
-        <v>48</v>
-      </c>
+      <c r="H86"/>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B87" t="n">
-        <v>465484.0</v>
+        <v>465431.0</v>
       </c>
       <c r="C87" t="s">
         <v>7</v>
@@ -7330,20 +7326,24 @@
         <v>8</v>
       </c>
       <c r="E87" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F87" t="s">
-        <v>48</v>
-      </c>
-      <c r="G87"/>
-      <c r="H87"/>
+        <v>45</v>
+      </c>
+      <c r="G87" t="s">
+        <v>48</v>
+      </c>
+      <c r="H87" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B88" t="n">
-        <v>465644.0</v>
+        <v>465484.0</v>
       </c>
       <c r="C88" t="s">
         <v>7</v>
@@ -7355,19 +7355,17 @@
         <v>48</v>
       </c>
       <c r="F88" t="s">
-        <v>47</v>
-      </c>
-      <c r="G88" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G88"/>
       <c r="H88"/>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B89" t="n">
-        <v>465653.0</v>
+        <v>465644.0</v>
       </c>
       <c r="C89" t="s">
         <v>7</v>
@@ -7376,20 +7374,22 @@
         <v>8</v>
       </c>
       <c r="E89" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F89" t="s">
-        <v>44</v>
-      </c>
-      <c r="G89"/>
+        <v>48</v>
+      </c>
+      <c r="G89" t="s">
+        <v>44</v>
+      </c>
       <c r="H89"/>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B90" t="n">
-        <v>465814.0</v>
+        <v>465653.0</v>
       </c>
       <c r="C90" t="s">
         <v>7</v>
@@ -7398,24 +7398,20 @@
         <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F90" t="s">
-        <v>45</v>
-      </c>
-      <c r="G90" t="s">
-        <v>48</v>
-      </c>
-      <c r="H90" t="s">
-        <v>44</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G90"/>
+      <c r="H90"/>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B91" t="n">
-        <v>465850.0</v>
+        <v>465814.0</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
@@ -7424,20 +7420,24 @@
         <v>8</v>
       </c>
       <c r="E91" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F91" t="s">
-        <v>48</v>
-      </c>
-      <c r="G91"/>
-      <c r="H91"/>
+        <v>47</v>
+      </c>
+      <c r="G91" t="s">
+        <v>44</v>
+      </c>
+      <c r="H91" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B92" t="n">
-        <v>466433.0</v>
+        <v>465850.0</v>
       </c>
       <c r="C92" t="s">
         <v>7</v>
@@ -7449,19 +7449,17 @@
         <v>48</v>
       </c>
       <c r="F92" t="s">
-        <v>45</v>
-      </c>
-      <c r="G92" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G92"/>
       <c r="H92"/>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B93" t="n">
-        <v>466579.0</v>
+        <v>466433.0</v>
       </c>
       <c r="C93" t="s">
         <v>7</v>
@@ -7470,24 +7468,22 @@
         <v>8</v>
       </c>
       <c r="E93" t="s">
+        <v>48</v>
+      </c>
+      <c r="F93" t="s">
         <v>45</v>
       </c>
-      <c r="F93" t="s">
-        <v>47</v>
-      </c>
       <c r="G93" t="s">
         <v>44</v>
       </c>
-      <c r="H93" t="s">
-        <v>48</v>
-      </c>
+      <c r="H93"/>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B94" t="n">
-        <v>466801.0</v>
+        <v>466579.0</v>
       </c>
       <c r="C94" t="s">
         <v>7</v>
@@ -7499,67 +7495,67 @@
         <v>47</v>
       </c>
       <c r="F94" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G94" t="s">
-        <v>44</v>
-      </c>
-      <c r="H94"/>
+        <v>48</v>
+      </c>
+      <c r="H94" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B95" t="n">
-        <v>466803.0</v>
+        <v>466801.0</v>
       </c>
       <c r="C95" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D95" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E95" t="s">
         <v>44</v>
       </c>
       <c r="F95" t="s">
-        <v>45</v>
-      </c>
-      <c r="G95"/>
+        <v>47</v>
+      </c>
+      <c r="G95" t="s">
+        <v>48</v>
+      </c>
       <c r="H95"/>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B96" t="n">
-        <v>466831.0</v>
+        <v>466803.0</v>
       </c>
       <c r="C96" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D96" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E96" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F96" t="s">
-        <v>45</v>
-      </c>
-      <c r="G96" t="s">
-        <v>48</v>
-      </c>
-      <c r="H96" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G96"/>
+      <c r="H96"/>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B97" t="n">
-        <v>466968.0</v>
+        <v>466831.0</v>
       </c>
       <c r="C97" t="s">
         <v>7</v>
@@ -7568,20 +7564,24 @@
         <v>8</v>
       </c>
       <c r="E97" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F97" t="s">
-        <v>44</v>
-      </c>
-      <c r="G97"/>
-      <c r="H97"/>
+        <v>47</v>
+      </c>
+      <c r="G97" t="s">
+        <v>44</v>
+      </c>
+      <c r="H97" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B98" t="n">
-        <v>467069.0</v>
+        <v>466968.0</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
@@ -7590,22 +7590,20 @@
         <v>8</v>
       </c>
       <c r="E98" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F98" t="s">
-        <v>47</v>
-      </c>
-      <c r="G98" t="s">
-        <v>44</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G98"/>
       <c r="H98"/>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B99" t="n">
-        <v>467189.0</v>
+        <v>467069.0</v>
       </c>
       <c r="C99" t="s">
         <v>7</v>
@@ -7622,16 +7620,14 @@
       <c r="G99" t="s">
         <v>44</v>
       </c>
-      <c r="H99" t="s">
-        <v>48</v>
-      </c>
+      <c r="H99"/>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B100" t="n">
-        <v>467214.0</v>
+        <v>467189.0</v>
       </c>
       <c r="C100" t="s">
         <v>7</v>
@@ -7640,20 +7636,24 @@
         <v>8</v>
       </c>
       <c r="E100" t="s">
+        <v>47</v>
+      </c>
+      <c r="F100" t="s">
         <v>45</v>
       </c>
-      <c r="F100" t="s">
-        <v>44</v>
-      </c>
-      <c r="G100"/>
-      <c r="H100"/>
+      <c r="G100" t="s">
+        <v>48</v>
+      </c>
+      <c r="H100" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B101" t="n">
-        <v>467243.0</v>
+        <v>467214.0</v>
       </c>
       <c r="C101" t="s">
         <v>7</v>
@@ -7662,20 +7662,20 @@
         <v>8</v>
       </c>
       <c r="E101" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F101" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G101"/>
       <c r="H101"/>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B102" t="n">
-        <v>467436.0</v>
+        <v>467243.0</v>
       </c>
       <c r="C102" t="s">
         <v>7</v>
@@ -7684,22 +7684,20 @@
         <v>8</v>
       </c>
       <c r="E102" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F102" t="s">
-        <v>47</v>
-      </c>
-      <c r="G102" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G102"/>
       <c r="H102"/>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B103" t="n">
-        <v>467451.0</v>
+        <v>467436.0</v>
       </c>
       <c r="C103" t="s">
         <v>7</v>
@@ -7708,20 +7706,22 @@
         <v>8</v>
       </c>
       <c r="E103" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F103" t="s">
-        <v>45</v>
-      </c>
-      <c r="G103"/>
+        <v>47</v>
+      </c>
+      <c r="G103" t="s">
+        <v>44</v>
+      </c>
       <c r="H103"/>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B104" t="n">
-        <v>467455.0</v>
+        <v>467451.0</v>
       </c>
       <c r="C104" t="s">
         <v>7</v>
@@ -7730,22 +7730,20 @@
         <v>8</v>
       </c>
       <c r="E104" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F104" t="s">
-        <v>48</v>
-      </c>
-      <c r="G104" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G104"/>
       <c r="H104"/>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B105" t="n">
-        <v>467461.0</v>
+        <v>467455.0</v>
       </c>
       <c r="C105" t="s">
         <v>7</v>
@@ -7757,21 +7755,19 @@
         <v>47</v>
       </c>
       <c r="F105" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G105" t="s">
-        <v>48</v>
-      </c>
-      <c r="H105" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H105"/>
     </row>
     <row r="106">
       <c r="A106" t="s">
         <v>46</v>
       </c>
       <c r="B106" t="n">
-        <v>467493.0</v>
+        <v>467461.0</v>
       </c>
       <c r="C106" t="s">
         <v>7</v>
@@ -7794,10 +7790,10 @@
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B107" t="n">
-        <v>467497.0</v>
+        <v>467493.0</v>
       </c>
       <c r="C107" t="s">
         <v>7</v>
@@ -7806,20 +7802,24 @@
         <v>8</v>
       </c>
       <c r="E107" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F107" t="s">
-        <v>47</v>
-      </c>
-      <c r="G107"/>
-      <c r="H107"/>
+        <v>45</v>
+      </c>
+      <c r="G107" t="s">
+        <v>48</v>
+      </c>
+      <c r="H107" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B108" t="n">
-        <v>467501.0</v>
+        <v>467497.0</v>
       </c>
       <c r="C108" t="s">
         <v>7</v>
@@ -7828,7 +7828,7 @@
         <v>8</v>
       </c>
       <c r="E108" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F108" t="s">
         <v>44</v>
@@ -7838,10 +7838,10 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B109" t="n">
-        <v>467636.0</v>
+        <v>467501.0</v>
       </c>
       <c r="C109" t="s">
         <v>7</v>
@@ -7850,24 +7850,20 @@
         <v>8</v>
       </c>
       <c r="E109" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F109" t="s">
         <v>45</v>
       </c>
-      <c r="G109" t="s">
-        <v>48</v>
-      </c>
-      <c r="H109" t="s">
-        <v>44</v>
-      </c>
+      <c r="G109"/>
+      <c r="H109"/>
     </row>
     <row r="110">
       <c r="A110" t="s">
         <v>46</v>
       </c>
       <c r="B110" t="n">
-        <v>467744.0</v>
+        <v>467636.0</v>
       </c>
       <c r="C110" t="s">
         <v>7</v>
@@ -7890,10 +7886,10 @@
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B111" t="n">
-        <v>467750.0</v>
+        <v>467744.0</v>
       </c>
       <c r="C111" t="s">
         <v>7</v>
@@ -7902,22 +7898,24 @@
         <v>8</v>
       </c>
       <c r="E111" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F111" t="s">
         <v>45</v>
       </c>
       <c r="G111" t="s">
-        <v>44</v>
-      </c>
-      <c r="H111"/>
+        <v>48</v>
+      </c>
+      <c r="H111" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B112" t="n">
-        <v>467765.0</v>
+        <v>467750.0</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
@@ -7929,9 +7927,11 @@
         <v>48</v>
       </c>
       <c r="F112" t="s">
-        <v>44</v>
-      </c>
-      <c r="G112"/>
+        <v>45</v>
+      </c>
+      <c r="G112" t="s">
+        <v>44</v>
+      </c>
       <c r="H112"/>
     </row>
     <row r="113">
@@ -7939,7 +7939,7 @@
         <v>50</v>
       </c>
       <c r="B113" t="n">
-        <v>467775.0</v>
+        <v>467765.0</v>
       </c>
       <c r="C113" t="s">
         <v>7</v>
@@ -7961,7 +7961,7 @@
         <v>50</v>
       </c>
       <c r="B114" t="n">
-        <v>467836.0</v>
+        <v>467775.0</v>
       </c>
       <c r="C114" t="s">
         <v>7</v>
@@ -7980,10 +7980,10 @@
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B115" t="n">
-        <v>467870.0</v>
+        <v>467836.0</v>
       </c>
       <c r="C115" t="s">
         <v>7</v>
@@ -7992,22 +7992,20 @@
         <v>8</v>
       </c>
       <c r="E115" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F115" t="s">
-        <v>47</v>
-      </c>
-      <c r="G115" t="s">
-        <v>44</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G115"/>
       <c r="H115"/>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B116" t="n">
-        <v>467873.0</v>
+        <v>467870.0</v>
       </c>
       <c r="C116" t="s">
         <v>7</v>
@@ -8016,13 +8014,13 @@
         <v>8</v>
       </c>
       <c r="E116" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F116" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G116" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="H116"/>
     </row>
@@ -8031,7 +8029,7 @@
         <v>52</v>
       </c>
       <c r="B117" t="n">
-        <v>467940.0</v>
+        <v>467873.0</v>
       </c>
       <c r="C117" t="s">
         <v>7</v>
@@ -8040,10 +8038,10 @@
         <v>8</v>
       </c>
       <c r="E117" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F117" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G117" t="s">
         <v>44</v>
@@ -8052,10 +8050,10 @@
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B118" t="n">
-        <v>467947.0</v>
+        <v>467940.0</v>
       </c>
       <c r="C118" t="s">
         <v>7</v>
@@ -8064,22 +8062,22 @@
         <v>8</v>
       </c>
       <c r="E118" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F118" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G118" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H118"/>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B119" t="n">
-        <v>467963.0</v>
+        <v>467947.0</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -8091,21 +8089,19 @@
         <v>47</v>
       </c>
       <c r="F119" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G119" t="s">
-        <v>48</v>
-      </c>
-      <c r="H119" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="H119"/>
     </row>
     <row r="120">
       <c r="A120" t="s">
         <v>46</v>
       </c>
       <c r="B120" t="n">
-        <v>467975.0</v>
+        <v>467963.0</v>
       </c>
       <c r="C120" t="s">
         <v>7</v>
@@ -8131,13 +8127,13 @@
         <v>46</v>
       </c>
       <c r="B121" t="n">
-        <v>467986.0</v>
+        <v>467975.0</v>
       </c>
       <c r="C121" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D121" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E121" t="s">
         <v>47</v>
@@ -8154,32 +8150,36 @@
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B122" t="n">
-        <v>468167.0</v>
+        <v>467986.0</v>
       </c>
       <c r="C122" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D122" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E122" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F122" t="s">
-        <v>45</v>
-      </c>
-      <c r="G122"/>
-      <c r="H122"/>
+        <v>47</v>
+      </c>
+      <c r="G122" t="s">
+        <v>44</v>
+      </c>
+      <c r="H122" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B123" t="n">
-        <v>468178.0</v>
+        <v>468167.0</v>
       </c>
       <c r="C123" t="s">
         <v>7</v>
@@ -8188,7 +8188,7 @@
         <v>8</v>
       </c>
       <c r="E123" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F123" t="s">
         <v>44</v>
@@ -8198,10 +8198,10 @@
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B124" t="n">
-        <v>468255.0</v>
+        <v>468178.0</v>
       </c>
       <c r="C124" t="s">
         <v>7</v>
@@ -8210,24 +8210,20 @@
         <v>8</v>
       </c>
       <c r="E124" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F124" t="s">
         <v>47</v>
       </c>
-      <c r="G124" t="s">
-        <v>44</v>
-      </c>
-      <c r="H124" t="s">
-        <v>48</v>
-      </c>
+      <c r="G124"/>
+      <c r="H124"/>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B125" t="n">
-        <v>468284.0</v>
+        <v>468255.0</v>
       </c>
       <c r="C125" t="s">
         <v>7</v>
@@ -8236,20 +8232,24 @@
         <v>8</v>
       </c>
       <c r="E125" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F125" t="s">
-        <v>47</v>
-      </c>
-      <c r="G125"/>
-      <c r="H125"/>
+        <v>45</v>
+      </c>
+      <c r="G125" t="s">
+        <v>48</v>
+      </c>
+      <c r="H125" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B126" t="n">
-        <v>468311.0</v>
+        <v>468284.0</v>
       </c>
       <c r="C126" t="s">
         <v>7</v>
@@ -8261,21 +8261,17 @@
         <v>47</v>
       </c>
       <c r="F126" t="s">
-        <v>45</v>
-      </c>
-      <c r="G126" t="s">
-        <v>48</v>
-      </c>
-      <c r="H126" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G126"/>
+      <c r="H126"/>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B127" t="n">
-        <v>468546.0</v>
+        <v>468311.0</v>
       </c>
       <c r="C127" t="s">
         <v>7</v>
@@ -8284,20 +8280,24 @@
         <v>8</v>
       </c>
       <c r="E127" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F127" t="s">
-        <v>48</v>
-      </c>
-      <c r="G127"/>
-      <c r="H127"/>
+        <v>47</v>
+      </c>
+      <c r="G127" t="s">
+        <v>44</v>
+      </c>
+      <c r="H127" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B128" t="n">
-        <v>468554.0</v>
+        <v>468546.0</v>
       </c>
       <c r="C128" t="s">
         <v>7</v>
@@ -8306,7 +8306,7 @@
         <v>8</v>
       </c>
       <c r="E128" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F128" t="s">
         <v>44</v>
@@ -8316,10 +8316,10 @@
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B129" t="n">
-        <v>468607.0</v>
+        <v>468554.0</v>
       </c>
       <c r="C129" t="s">
         <v>7</v>
@@ -8328,10 +8328,10 @@
         <v>8</v>
       </c>
       <c r="E129" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F129" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G129"/>
       <c r="H129"/>
@@ -8341,7 +8341,7 @@
         <v>50</v>
       </c>
       <c r="B130" t="n">
-        <v>468643.0</v>
+        <v>468607.0</v>
       </c>
       <c r="C130" t="s">
         <v>7</v>
@@ -8360,10 +8360,10 @@
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B131" t="n">
-        <v>468736.0</v>
+        <v>468643.0</v>
       </c>
       <c r="C131" t="s">
         <v>7</v>
@@ -8372,22 +8372,20 @@
         <v>8</v>
       </c>
       <c r="E131" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F131" t="s">
-        <v>48</v>
-      </c>
-      <c r="G131" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G131"/>
       <c r="H131"/>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B132" t="n">
-        <v>468763.0</v>
+        <v>468736.0</v>
       </c>
       <c r="C132" t="s">
         <v>7</v>
@@ -8396,20 +8394,22 @@
         <v>8</v>
       </c>
       <c r="E132" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F132" t="s">
-        <v>45</v>
-      </c>
-      <c r="G132"/>
+        <v>47</v>
+      </c>
+      <c r="G132" t="s">
+        <v>44</v>
+      </c>
       <c r="H132"/>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B133" t="n">
-        <v>468859.0</v>
+        <v>468763.0</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
@@ -8418,7 +8418,7 @@
         <v>8</v>
       </c>
       <c r="E133" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F133" t="s">
         <v>44</v>
@@ -8428,10 +8428,10 @@
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B134" t="n">
-        <v>468876.0</v>
+        <v>468859.0</v>
       </c>
       <c r="C134" t="s">
         <v>7</v>
@@ -8440,24 +8440,20 @@
         <v>8</v>
       </c>
       <c r="E134" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F134" t="s">
         <v>47</v>
       </c>
-      <c r="G134" t="s">
-        <v>44</v>
-      </c>
-      <c r="H134" t="s">
-        <v>48</v>
-      </c>
+      <c r="G134"/>
+      <c r="H134"/>
     </row>
     <row r="135">
       <c r="A135" t="s">
         <v>46</v>
       </c>
       <c r="B135" t="n">
-        <v>468882.0</v>
+        <v>468876.0</v>
       </c>
       <c r="C135" t="s">
         <v>7</v>
@@ -8480,10 +8476,10 @@
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B136" t="n">
-        <v>468898.0</v>
+        <v>468882.0</v>
       </c>
       <c r="C136" t="s">
         <v>7</v>
@@ -8495,17 +8491,21 @@
         <v>45</v>
       </c>
       <c r="F136" t="s">
-        <v>44</v>
-      </c>
-      <c r="G136"/>
-      <c r="H136"/>
+        <v>47</v>
+      </c>
+      <c r="G136" t="s">
+        <v>44</v>
+      </c>
+      <c r="H136" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
         <v>43</v>
       </c>
       <c r="B137" t="n">
-        <v>468903.0</v>
+        <v>468898.0</v>
       </c>
       <c r="C137" t="s">
         <v>7</v>
@@ -8524,10 +8524,10 @@
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B138" t="n">
-        <v>468961.0</v>
+        <v>468903.0</v>
       </c>
       <c r="C138" t="s">
         <v>7</v>
@@ -8536,22 +8536,20 @@
         <v>8</v>
       </c>
       <c r="E138" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F138" t="s">
-        <v>47</v>
-      </c>
-      <c r="G138" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G138"/>
       <c r="H138"/>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B139" t="n">
-        <v>469129.0</v>
+        <v>468961.0</v>
       </c>
       <c r="C139" t="s">
         <v>7</v>
@@ -8565,7 +8563,9 @@
       <c r="F139" t="s">
         <v>47</v>
       </c>
-      <c r="G139"/>
+      <c r="G139" t="s">
+        <v>48</v>
+      </c>
       <c r="H139"/>
     </row>
     <row r="140">
@@ -8573,7 +8573,7 @@
         <v>51</v>
       </c>
       <c r="B140" t="n">
-        <v>469142.0</v>
+        <v>469129.0</v>
       </c>
       <c r="C140" t="s">
         <v>7</v>
@@ -8592,10 +8592,10 @@
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B141" t="n">
-        <v>469186.0</v>
+        <v>469142.0</v>
       </c>
       <c r="C141" t="s">
         <v>7</v>
@@ -8604,24 +8604,20 @@
         <v>8</v>
       </c>
       <c r="E141" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F141" t="s">
         <v>47</v>
       </c>
-      <c r="G141" t="s">
-        <v>44</v>
-      </c>
-      <c r="H141" t="s">
-        <v>48</v>
-      </c>
+      <c r="G141"/>
+      <c r="H141"/>
     </row>
     <row r="142">
       <c r="A142" t="s">
         <v>46</v>
       </c>
       <c r="B142" t="n">
-        <v>469193.0</v>
+        <v>469186.0</v>
       </c>
       <c r="C142" t="s">
         <v>7</v>
@@ -8644,10 +8640,10 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B143" t="n">
-        <v>469213.0</v>
+        <v>469193.0</v>
       </c>
       <c r="C143" t="s">
         <v>7</v>
@@ -8656,20 +8652,24 @@
         <v>8</v>
       </c>
       <c r="E143" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F143" t="s">
-        <v>44</v>
-      </c>
-      <c r="G143"/>
-      <c r="H143"/>
+        <v>47</v>
+      </c>
+      <c r="G143" t="s">
+        <v>44</v>
+      </c>
+      <c r="H143" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B144" t="n">
-        <v>469288.0</v>
+        <v>469213.0</v>
       </c>
       <c r="C144" t="s">
         <v>7</v>
@@ -8678,24 +8678,20 @@
         <v>8</v>
       </c>
       <c r="E144" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F144" t="s">
-        <v>47</v>
-      </c>
-      <c r="G144" t="s">
-        <v>44</v>
-      </c>
-      <c r="H144" t="s">
-        <v>48</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G144"/>
+      <c r="H144"/>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B145" t="n">
-        <v>469327.0</v>
+        <v>469288.0</v>
       </c>
       <c r="C145" t="s">
         <v>7</v>
@@ -8704,22 +8700,24 @@
         <v>8</v>
       </c>
       <c r="E145" t="s">
+        <v>47</v>
+      </c>
+      <c r="F145" t="s">
         <v>45</v>
       </c>
-      <c r="F145" t="s">
-        <v>48</v>
-      </c>
       <c r="G145" t="s">
-        <v>44</v>
-      </c>
-      <c r="H145"/>
+        <v>48</v>
+      </c>
+      <c r="H145" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B146" t="n">
-        <v>469351.0</v>
+        <v>469327.0</v>
       </c>
       <c r="C146" t="s">
         <v>7</v>
@@ -8731,17 +8729,19 @@
         <v>45</v>
       </c>
       <c r="F146" t="s">
-        <v>44</v>
-      </c>
-      <c r="G146"/>
+        <v>48</v>
+      </c>
+      <c r="G146" t="s">
+        <v>44</v>
+      </c>
       <c r="H146"/>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B147" t="n">
-        <v>469358.0</v>
+        <v>469351.0</v>
       </c>
       <c r="C147" t="s">
         <v>7</v>
@@ -8755,17 +8755,15 @@
       <c r="F147" t="s">
         <v>45</v>
       </c>
-      <c r="G147" t="s">
-        <v>47</v>
-      </c>
+      <c r="G147"/>
       <c r="H147"/>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B148" t="n">
-        <v>469474.0</v>
+        <v>469358.0</v>
       </c>
       <c r="C148" t="s">
         <v>7</v>
@@ -8774,24 +8772,22 @@
         <v>8</v>
       </c>
       <c r="E148" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F148" t="s">
         <v>45</v>
       </c>
       <c r="G148" t="s">
-        <v>48</v>
-      </c>
-      <c r="H148" t="s">
-        <v>44</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="H148"/>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B149" t="n">
-        <v>469486.0</v>
+        <v>469474.0</v>
       </c>
       <c r="C149" t="s">
         <v>7</v>
@@ -8800,20 +8796,24 @@
         <v>8</v>
       </c>
       <c r="E149" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F149" t="s">
-        <v>48</v>
-      </c>
-      <c r="G149"/>
-      <c r="H149"/>
+        <v>47</v>
+      </c>
+      <c r="G149" t="s">
+        <v>44</v>
+      </c>
+      <c r="H149" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B150" t="n">
-        <v>469625.0</v>
+        <v>469486.0</v>
       </c>
       <c r="C150" t="s">
         <v>7</v>
@@ -8822,24 +8822,20 @@
         <v>8</v>
       </c>
       <c r="E150" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F150" t="s">
-        <v>47</v>
-      </c>
-      <c r="G150" t="s">
-        <v>44</v>
-      </c>
-      <c r="H150" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G150"/>
+      <c r="H150"/>
     </row>
     <row r="151">
       <c r="A151" t="s">
         <v>46</v>
       </c>
       <c r="B151" t="n">
-        <v>469740.0</v>
+        <v>469625.0</v>
       </c>
       <c r="C151" t="s">
         <v>7</v>
@@ -8862,10 +8858,10 @@
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B152" t="n">
-        <v>469823.0</v>
+        <v>469740.0</v>
       </c>
       <c r="C152" t="s">
         <v>7</v>
@@ -8874,20 +8870,24 @@
         <v>8</v>
       </c>
       <c r="E152" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F152" t="s">
-        <v>45</v>
-      </c>
-      <c r="G152"/>
-      <c r="H152"/>
+        <v>47</v>
+      </c>
+      <c r="G152" t="s">
+        <v>44</v>
+      </c>
+      <c r="H152" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B153" t="n">
-        <v>469857.0</v>
+        <v>469823.0</v>
       </c>
       <c r="C153" t="s">
         <v>7</v>
@@ -8896,22 +8896,20 @@
         <v>8</v>
       </c>
       <c r="E153" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F153" t="s">
-        <v>48</v>
-      </c>
-      <c r="G153" t="s">
-        <v>47</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G153"/>
       <c r="H153"/>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B154" t="n">
-        <v>469975.0</v>
+        <v>469857.0</v>
       </c>
       <c r="C154" t="s">
         <v>7</v>
@@ -8920,24 +8918,22 @@
         <v>8</v>
       </c>
       <c r="E154" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F154" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G154" t="s">
         <v>44</v>
       </c>
-      <c r="H154" t="s">
-        <v>48</v>
-      </c>
+      <c r="H154"/>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B155" t="n">
-        <v>470129.0</v>
+        <v>469975.0</v>
       </c>
       <c r="C155" t="s">
         <v>7</v>
@@ -8946,20 +8942,24 @@
         <v>8</v>
       </c>
       <c r="E155" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F155" t="s">
-        <v>44</v>
-      </c>
-      <c r="G155"/>
-      <c r="H155"/>
+        <v>45</v>
+      </c>
+      <c r="G155" t="s">
+        <v>48</v>
+      </c>
+      <c r="H155" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B156" t="n">
-        <v>470144.0</v>
+        <v>470129.0</v>
       </c>
       <c r="C156" t="s">
         <v>7</v>
@@ -8971,17 +8971,17 @@
         <v>44</v>
       </c>
       <c r="F156" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G156"/>
       <c r="H156"/>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B157" t="n">
-        <v>470282.0</v>
+        <v>470144.0</v>
       </c>
       <c r="C157" t="s">
         <v>7</v>
@@ -8993,21 +8993,17 @@
         <v>47</v>
       </c>
       <c r="F157" t="s">
-        <v>45</v>
-      </c>
-      <c r="G157" t="s">
-        <v>48</v>
-      </c>
-      <c r="H157" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G157"/>
+      <c r="H157"/>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B158" t="n">
-        <v>470290.0</v>
+        <v>470282.0</v>
       </c>
       <c r="C158" t="s">
         <v>7</v>
@@ -9016,20 +9012,24 @@
         <v>8</v>
       </c>
       <c r="E158" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F158" t="s">
-        <v>44</v>
-      </c>
-      <c r="G158"/>
-      <c r="H158"/>
+        <v>47</v>
+      </c>
+      <c r="G158" t="s">
+        <v>44</v>
+      </c>
+      <c r="H158" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B159" t="n">
-        <v>470309.0</v>
+        <v>470290.0</v>
       </c>
       <c r="C159" t="s">
         <v>7</v>
@@ -9038,20 +9038,20 @@
         <v>8</v>
       </c>
       <c r="E159" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F159" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="G159"/>
       <c r="H159"/>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B160" t="n">
-        <v>470373.0</v>
+        <v>470309.0</v>
       </c>
       <c r="C160" t="s">
         <v>7</v>
@@ -9060,22 +9060,20 @@
         <v>8</v>
       </c>
       <c r="E160" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F160" t="s">
-        <v>47</v>
-      </c>
-      <c r="G160" t="s">
-        <v>44</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G160"/>
       <c r="H160"/>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B161" t="n">
-        <v>470405.0</v>
+        <v>470373.0</v>
       </c>
       <c r="C161" t="s">
         <v>7</v>
@@ -9084,20 +9082,22 @@
         <v>8</v>
       </c>
       <c r="E161" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F161" t="s">
         <v>47</v>
       </c>
-      <c r="G161"/>
+      <c r="G161" t="s">
+        <v>44</v>
+      </c>
       <c r="H161"/>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B162" t="n">
-        <v>470467.0</v>
+        <v>470405.0</v>
       </c>
       <c r="C162" t="s">
         <v>7</v>
@@ -9109,11 +9109,9 @@
         <v>47</v>
       </c>
       <c r="F162" t="s">
-        <v>48</v>
-      </c>
-      <c r="G162" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G162"/>
       <c r="H162"/>
     </row>
     <row r="163">
@@ -9121,7 +9119,7 @@
         <v>49</v>
       </c>
       <c r="B163" t="n">
-        <v>470488.0</v>
+        <v>470467.0</v>
       </c>
       <c r="C163" t="s">
         <v>7</v>
@@ -9133,19 +9131,19 @@
         <v>44</v>
       </c>
       <c r="F163" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G163" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H163"/>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B164" t="n">
-        <v>470638.0</v>
+        <v>470488.0</v>
       </c>
       <c r="C164" t="s">
         <v>7</v>
@@ -9154,20 +9152,22 @@
         <v>8</v>
       </c>
       <c r="E164" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F164" t="s">
-        <v>48</v>
-      </c>
-      <c r="G164"/>
+        <v>47</v>
+      </c>
+      <c r="G164" t="s">
+        <v>44</v>
+      </c>
       <c r="H164"/>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B165" t="n">
-        <v>470668.0</v>
+        <v>470638.0</v>
       </c>
       <c r="C165" t="s">
         <v>7</v>
@@ -9176,20 +9176,20 @@
         <v>8</v>
       </c>
       <c r="E165" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F165" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G165"/>
       <c r="H165"/>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B166" t="n">
-        <v>470754.0</v>
+        <v>470668.0</v>
       </c>
       <c r="C166" t="s">
         <v>7</v>
@@ -9198,22 +9198,20 @@
         <v>8</v>
       </c>
       <c r="E166" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F166" t="s">
         <v>44</v>
       </c>
-      <c r="G166" t="s">
-        <v>47</v>
-      </c>
+      <c r="G166"/>
       <c r="H166"/>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B167" t="n">
-        <v>470773.0</v>
+        <v>470754.0</v>
       </c>
       <c r="C167" t="s">
         <v>7</v>
@@ -9222,24 +9220,22 @@
         <v>8</v>
       </c>
       <c r="E167" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F167" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G167" t="s">
         <v>44</v>
       </c>
-      <c r="H167" t="s">
-        <v>48</v>
-      </c>
+      <c r="H167"/>
     </row>
     <row r="168">
       <c r="A168" t="s">
         <v>46</v>
       </c>
       <c r="B168" t="n">
-        <v>470782.0</v>
+        <v>470773.0</v>
       </c>
       <c r="C168" t="s">
         <v>7</v>
@@ -9262,10 +9258,10 @@
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B169" t="n">
-        <v>470830.0</v>
+        <v>470782.0</v>
       </c>
       <c r="C169" t="s">
         <v>7</v>
@@ -9274,20 +9270,24 @@
         <v>8</v>
       </c>
       <c r="E169" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F169" t="s">
-        <v>44</v>
-      </c>
-      <c r="G169"/>
-      <c r="H169"/>
+        <v>47</v>
+      </c>
+      <c r="G169" t="s">
+        <v>44</v>
+      </c>
+      <c r="H169" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B170" t="n">
-        <v>470859.0</v>
+        <v>470830.0</v>
       </c>
       <c r="C170" t="s">
         <v>7</v>
@@ -9296,22 +9296,20 @@
         <v>8</v>
       </c>
       <c r="E170" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F170" t="s">
-        <v>48</v>
-      </c>
-      <c r="G170" t="s">
-        <v>44</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G170"/>
       <c r="H170"/>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B171" t="n">
-        <v>470921.0</v>
+        <v>470859.0</v>
       </c>
       <c r="C171" t="s">
         <v>7</v>
@@ -9320,12 +9318,14 @@
         <v>8</v>
       </c>
       <c r="E171" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F171" t="s">
-        <v>44</v>
-      </c>
-      <c r="G171"/>
+        <v>47</v>
+      </c>
+      <c r="G171" t="s">
+        <v>48</v>
+      </c>
       <c r="H171"/>
     </row>
     <row r="172">
@@ -9333,7 +9333,7 @@
         <v>50</v>
       </c>
       <c r="B172" t="n">
-        <v>471016.0</v>
+        <v>470921.0</v>
       </c>
       <c r="C172" t="s">
         <v>7</v>
@@ -9352,10 +9352,10 @@
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B173" t="n">
-        <v>471028.0</v>
+        <v>471016.0</v>
       </c>
       <c r="C173" t="s">
         <v>7</v>
@@ -9364,24 +9364,20 @@
         <v>8</v>
       </c>
       <c r="E173" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F173" t="s">
-        <v>47</v>
-      </c>
-      <c r="G173" t="s">
-        <v>44</v>
-      </c>
-      <c r="H173" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G173"/>
+      <c r="H173"/>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B174" t="n">
-        <v>471129.0</v>
+        <v>471028.0</v>
       </c>
       <c r="C174" t="s">
         <v>7</v>
@@ -9390,20 +9386,24 @@
         <v>8</v>
       </c>
       <c r="E174" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F174" t="s">
-        <v>47</v>
-      </c>
-      <c r="G174"/>
-      <c r="H174"/>
+        <v>45</v>
+      </c>
+      <c r="G174" t="s">
+        <v>48</v>
+      </c>
+      <c r="H174" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B175" t="n">
-        <v>471229.0</v>
+        <v>471129.0</v>
       </c>
       <c r="C175" t="s">
         <v>7</v>
@@ -9412,7 +9412,7 @@
         <v>8</v>
       </c>
       <c r="E175" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F175" t="s">
         <v>44</v>
@@ -9425,7 +9425,7 @@
         <v>50</v>
       </c>
       <c r="B176" t="n">
-        <v>471255.0</v>
+        <v>471229.0</v>
       </c>
       <c r="C176" t="s">
         <v>7</v>
@@ -9444,10 +9444,10 @@
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B177" t="n">
-        <v>471263.0</v>
+        <v>471255.0</v>
       </c>
       <c r="C177" t="s">
         <v>7</v>
@@ -9456,22 +9456,20 @@
         <v>8</v>
       </c>
       <c r="E177" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F177" t="s">
-        <v>47</v>
-      </c>
-      <c r="G177" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G177"/>
       <c r="H177"/>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B178" t="n">
-        <v>471492.0</v>
+        <v>471263.0</v>
       </c>
       <c r="C178" t="s">
         <v>7</v>
@@ -9485,15 +9483,17 @@
       <c r="F178" t="s">
         <v>44</v>
       </c>
-      <c r="G178"/>
+      <c r="G178" t="s">
+        <v>47</v>
+      </c>
       <c r="H178"/>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B179" t="n">
-        <v>471545.0</v>
+        <v>471492.0</v>
       </c>
       <c r="C179" t="s">
         <v>7</v>
@@ -9502,22 +9502,20 @@
         <v>8</v>
       </c>
       <c r="E179" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F179" t="s">
-        <v>44</v>
-      </c>
-      <c r="G179" t="s">
-        <v>47</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G179"/>
       <c r="H179"/>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B180" t="n">
-        <v>471760.0</v>
+        <v>471545.0</v>
       </c>
       <c r="C180" t="s">
         <v>7</v>
@@ -9526,20 +9524,22 @@
         <v>8</v>
       </c>
       <c r="E180" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F180" t="s">
         <v>48</v>
       </c>
-      <c r="G180"/>
+      <c r="G180" t="s">
+        <v>44</v>
+      </c>
       <c r="H180"/>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B181" t="n">
-        <v>472004.0</v>
+        <v>471760.0</v>
       </c>
       <c r="C181" t="s">
         <v>7</v>
@@ -9548,7 +9548,7 @@
         <v>8</v>
       </c>
       <c r="E181" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F181" t="s">
         <v>44</v>
@@ -9558,10 +9558,10 @@
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B182" t="n">
-        <v>472145.0</v>
+        <v>472004.0</v>
       </c>
       <c r="C182" t="s">
         <v>7</v>
@@ -9570,22 +9570,20 @@
         <v>8</v>
       </c>
       <c r="E182" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F182" t="s">
         <v>45</v>
       </c>
-      <c r="G182" t="s">
-        <v>44</v>
-      </c>
+      <c r="G182"/>
       <c r="H182"/>
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B183" t="n">
-        <v>472434.0</v>
+        <v>472145.0</v>
       </c>
       <c r="C183" t="s">
         <v>7</v>
@@ -9594,20 +9592,22 @@
         <v>8</v>
       </c>
       <c r="E183" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F183" t="s">
         <v>45</v>
       </c>
-      <c r="G183"/>
+      <c r="G183" t="s">
+        <v>44</v>
+      </c>
       <c r="H183"/>
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B184" t="n">
-        <v>472501.0</v>
+        <v>472434.0</v>
       </c>
       <c r="C184" t="s">
         <v>7</v>
@@ -9616,24 +9616,20 @@
         <v>8</v>
       </c>
       <c r="E184" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F184" t="s">
-        <v>45</v>
-      </c>
-      <c r="G184" t="s">
-        <v>48</v>
-      </c>
-      <c r="H184" t="s">
-        <v>44</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G184"/>
+      <c r="H184"/>
     </row>
     <row r="185">
       <c r="A185" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B185" t="n">
-        <v>472537.0</v>
+        <v>472501.0</v>
       </c>
       <c r="C185" t="s">
         <v>7</v>
@@ -9642,20 +9638,24 @@
         <v>8</v>
       </c>
       <c r="E185" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F185" t="s">
-        <v>44</v>
-      </c>
-      <c r="G185"/>
-      <c r="H185"/>
+        <v>47</v>
+      </c>
+      <c r="G185" t="s">
+        <v>44</v>
+      </c>
+      <c r="H185" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B186" t="n">
-        <v>472782.0</v>
+        <v>472537.0</v>
       </c>
       <c r="C186" t="s">
         <v>7</v>
@@ -9664,22 +9664,20 @@
         <v>8</v>
       </c>
       <c r="E186" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F186" t="s">
-        <v>48</v>
-      </c>
-      <c r="G186" t="s">
-        <v>44</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G186"/>
       <c r="H186"/>
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B187" t="n">
-        <v>472962.0</v>
+        <v>472782.0</v>
       </c>
       <c r="C187" t="s">
         <v>7</v>
@@ -9688,20 +9686,22 @@
         <v>8</v>
       </c>
       <c r="E187" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F187" t="s">
-        <v>44</v>
-      </c>
-      <c r="G187"/>
+        <v>47</v>
+      </c>
+      <c r="G187" t="s">
+        <v>48</v>
+      </c>
       <c r="H187"/>
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B188" t="n">
-        <v>473195.0</v>
+        <v>472962.0</v>
       </c>
       <c r="C188" t="s">
         <v>7</v>
@@ -9710,22 +9710,20 @@
         <v>8</v>
       </c>
       <c r="E188" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F188" t="s">
         <v>48</v>
       </c>
-      <c r="G188" t="s">
-        <v>44</v>
-      </c>
+      <c r="G188"/>
       <c r="H188"/>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B189" t="n">
-        <v>473215.0</v>
+        <v>473195.0</v>
       </c>
       <c r="C189" t="s">
         <v>7</v>
@@ -9734,22 +9732,22 @@
         <v>8</v>
       </c>
       <c r="E189" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F189" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G189" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H189"/>
     </row>
     <row r="190">
       <c r="A190" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B190" t="n">
-        <v>473482.0</v>
+        <v>473215.0</v>
       </c>
       <c r="C190" t="s">
         <v>7</v>
@@ -9758,20 +9756,22 @@
         <v>8</v>
       </c>
       <c r="E190" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F190" t="s">
-        <v>48</v>
-      </c>
-      <c r="G190"/>
+        <v>44</v>
+      </c>
+      <c r="G190" t="s">
+        <v>47</v>
+      </c>
       <c r="H190"/>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B191" t="n">
-        <v>473708.0</v>
+        <v>473482.0</v>
       </c>
       <c r="C191" t="s">
         <v>7</v>
@@ -9785,17 +9785,15 @@
       <c r="F191" t="s">
         <v>44</v>
       </c>
-      <c r="G191" t="s">
-        <v>47</v>
-      </c>
+      <c r="G191"/>
       <c r="H191"/>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B192" t="n">
-        <v>473899.0</v>
+        <v>473708.0</v>
       </c>
       <c r="C192" t="s">
         <v>7</v>
@@ -9804,20 +9802,22 @@
         <v>8</v>
       </c>
       <c r="E192" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F192" t="s">
-        <v>44</v>
-      </c>
-      <c r="G192"/>
+        <v>48</v>
+      </c>
+      <c r="G192" t="s">
+        <v>44</v>
+      </c>
       <c r="H192"/>
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B193" t="n">
-        <v>475115.0</v>
+        <v>473899.0</v>
       </c>
       <c r="C193" t="s">
         <v>7</v>
@@ -9829,17 +9829,17 @@
         <v>44</v>
       </c>
       <c r="F193" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G193"/>
       <c r="H193"/>
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B194" t="n">
-        <v>476008.0</v>
+        <v>475115.0</v>
       </c>
       <c r="C194" t="s">
         <v>7</v>
@@ -9848,10 +9848,10 @@
         <v>8</v>
       </c>
       <c r="E194" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F194" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G194"/>
       <c r="H194"/>
@@ -9861,7 +9861,7 @@
         <v>50</v>
       </c>
       <c r="B195" t="n">
-        <v>476289.0</v>
+        <v>476008.0</v>
       </c>
       <c r="C195" t="s">
         <v>7</v>
@@ -9880,10 +9880,10 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B196" t="n">
-        <v>476531.0</v>
+        <v>476289.0</v>
       </c>
       <c r="C196" t="s">
         <v>7</v>
@@ -9892,20 +9892,20 @@
         <v>8</v>
       </c>
       <c r="E196" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F196" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G196"/>
       <c r="H196"/>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B197" t="n">
-        <v>476883.0</v>
+        <v>476531.0</v>
       </c>
       <c r="C197" t="s">
         <v>7</v>
@@ -9914,22 +9914,20 @@
         <v>8</v>
       </c>
       <c r="E197" t="s">
+        <v>44</v>
+      </c>
+      <c r="F197" t="s">
         <v>45</v>
       </c>
-      <c r="F197" t="s">
-        <v>48</v>
-      </c>
-      <c r="G197" t="s">
-        <v>44</v>
-      </c>
+      <c r="G197"/>
       <c r="H197"/>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B198" t="n">
-        <v>477153.0</v>
+        <v>476883.0</v>
       </c>
       <c r="C198" t="s">
         <v>7</v>
@@ -9938,12 +9936,14 @@
         <v>8</v>
       </c>
       <c r="E198" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F198" t="s">
         <v>48</v>
       </c>
-      <c r="G198"/>
+      <c r="G198" t="s">
+        <v>44</v>
+      </c>
       <c r="H198"/>
     </row>
     <row r="199">
@@ -9951,7 +9951,7 @@
         <v>50</v>
       </c>
       <c r="B199" t="n">
-        <v>477738.0</v>
+        <v>477153.0</v>
       </c>
       <c r="C199" t="s">
         <v>7</v>
@@ -9970,10 +9970,10 @@
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B200" t="n">
-        <v>478406.0</v>
+        <v>477738.0</v>
       </c>
       <c r="C200" t="s">
         <v>7</v>
@@ -9982,24 +9982,20 @@
         <v>8</v>
       </c>
       <c r="E200" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F200" t="s">
-        <v>47</v>
-      </c>
-      <c r="G200" t="s">
-        <v>44</v>
-      </c>
-      <c r="H200" t="s">
-        <v>48</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G200"/>
+      <c r="H200"/>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B201" t="n">
-        <v>478589.0</v>
+        <v>478406.0</v>
       </c>
       <c r="C201" t="s">
         <v>7</v>
@@ -10011,17 +10007,21 @@
         <v>47</v>
       </c>
       <c r="F201" t="s">
-        <v>44</v>
-      </c>
-      <c r="G201"/>
-      <c r="H201"/>
+        <v>45</v>
+      </c>
+      <c r="G201" t="s">
+        <v>48</v>
+      </c>
+      <c r="H201" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B202" t="n">
-        <v>479276.0</v>
+        <v>478589.0</v>
       </c>
       <c r="C202" t="s">
         <v>7</v>
@@ -10030,24 +10030,20 @@
         <v>8</v>
       </c>
       <c r="E202" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F202" t="s">
-        <v>45</v>
-      </c>
-      <c r="G202" t="s">
-        <v>48</v>
-      </c>
-      <c r="H202" t="s">
-        <v>44</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G202"/>
+      <c r="H202"/>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B203" t="n">
-        <v>479658.0</v>
+        <v>479276.0</v>
       </c>
       <c r="C203" t="s">
         <v>7</v>
@@ -10056,63 +10052,89 @@
         <v>8</v>
       </c>
       <c r="E203" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F203" t="s">
         <v>47</v>
       </c>
-      <c r="G203"/>
-      <c r="H203"/>
+      <c r="G203" t="s">
+        <v>44</v>
+      </c>
+      <c r="H203" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B204" t="n">
-        <v>532682.0</v>
+        <v>479658.0</v>
       </c>
       <c r="C204" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D204" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="E204" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F204" t="s">
-        <v>47</v>
-      </c>
-      <c r="G204" t="s">
-        <v>44</v>
-      </c>
-      <c r="H204" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G204"/>
+      <c r="H204"/>
     </row>
     <row r="205">
       <c r="A205" t="s">
+        <v>46</v>
+      </c>
+      <c r="B205" t="n">
+        <v>532682.0</v>
+      </c>
+      <c r="C205" t="s">
+        <v>11</v>
+      </c>
+      <c r="D205" t="s">
+        <v>33</v>
+      </c>
+      <c r="E205" t="s">
+        <v>47</v>
+      </c>
+      <c r="F205" t="s">
+        <v>45</v>
+      </c>
+      <c r="G205" t="s">
+        <v>48</v>
+      </c>
+      <c r="H205" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
         <v>49</v>
       </c>
-      <c r="B205" t="n">
+      <c r="B206" t="n">
         <v>987654.0</v>
       </c>
-      <c r="C205" t="s">
-        <v>7</v>
-      </c>
-      <c r="D205" t="s">
-        <v>8</v>
-      </c>
-      <c r="E205" t="s">
-        <v>47</v>
-      </c>
-      <c r="F205" t="s">
-        <v>48</v>
-      </c>
-      <c r="G205" t="s">
-        <v>44</v>
-      </c>
-      <c r="H205"/>
+      <c r="C206" t="s">
+        <v>7</v>
+      </c>
+      <c r="D206" t="s">
+        <v>8</v>
+      </c>
+      <c r="E206" t="s">
+        <v>44</v>
+      </c>
+      <c r="F206" t="s">
+        <v>47</v>
+      </c>
+      <c r="G206" t="s">
+        <v>48</v>
+      </c>
+      <c r="H206"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>